<commit_message>
solve task 75. Sort Colors
</commit_message>
<xml_diff>
--- a/DSA studing (in acc. with Claude plan)/DSA_Leetcode_plan from Claude.xlsx
+++ b/DSA studing (in acc. with Claude plan)/DSA_Leetcode_plan from Claude.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Programming\Python\Leetcode\Leetcode practise\DSA studing (in acc. with Claude plan)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A912A9C8-C97F-44C1-AB5E-0BC094953A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA09BCF-D7F6-4874-B357-D9130193B24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1268,20 +1268,32 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1297,18 +1309,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1599,8 +1599,8 @@
   <dimension ref="A1:L126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B2"/>
+      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1616,31 +1616,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="16" t="s">
+      <c r="B1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="23" t="s">
         <v>316</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="23" t="s">
         <v>317</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="23" t="s">
         <v>318</v>
       </c>
       <c r="J1" s="9" t="s">
@@ -1654,36 +1654,36 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
       <c r="J2" s="10">
         <f>COUNTIF(G3:G126,"решена")/124</f>
-        <v>0.42741935483870969</v>
+        <v>0.43548387096774194</v>
       </c>
       <c r="K2" s="11">
         <f>SUM(H3:H126)/(COUNTIF(G3:G126,"решена") + COUNTIF(G3:G126,"не решена"))</f>
-        <v>2.2545454545454544</v>
+        <v>2.25</v>
       </c>
       <c r="L2" s="10">
         <f>SUM(I3:I126)/SUM(H3:H126)</f>
-        <v>0.72580645161290325</v>
+        <v>0.73015873015873012</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="18">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -1709,9 +1709,9 @@
       <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="28"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="6" t="s">
         <v>11</v>
       </c>
@@ -1732,9 +1732,9 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="28">
+      <c r="A5" s="16"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="18">
         <v>2</v>
       </c>
       <c r="D5" s="6" t="s">
@@ -1757,9 +1757,9 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="29"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="18"/>
       <c r="D6" s="6" t="s">
         <v>15</v>
       </c>
@@ -1780,13 +1780,13 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="20" t="s">
         <v>324</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="18">
         <v>3</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -1809,9 +1809,9 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="29"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="28"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="18"/>
       <c r="D8" s="6" t="s">
         <v>20</v>
       </c>
@@ -1832,9 +1832,9 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="29"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28">
+      <c r="A9" s="16"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="18">
         <v>4</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -1857,9 +1857,9 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="29"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="28"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="6" t="s">
         <v>24</v>
       </c>
@@ -1880,13 +1880,13 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="18">
         <v>5</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -1909,9 +1909,9 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="29"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="18"/>
       <c r="D12" s="6" t="s">
         <v>29</v>
       </c>
@@ -1932,9 +1932,9 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="29"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28">
+      <c r="A13" s="16"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="18">
         <v>6</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -1957,9 +1957,9 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="28"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="6" t="s">
         <v>33</v>
       </c>
@@ -1980,13 +1980,13 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="C15" s="28">
+      <c r="C15" s="18">
         <v>7</v>
       </c>
       <c r="D15" s="6" t="s">
@@ -2009,9 +2009,9 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="18"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="28"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="6" t="s">
         <v>38</v>
       </c>
@@ -2032,9 +2032,9 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="28">
+      <c r="A17" s="17"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="18">
         <v>8</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -2057,9 +2057,9 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="28"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="18"/>
       <c r="D18" s="6" t="s">
         <v>42</v>
       </c>
@@ -2080,13 +2080,13 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="C19" s="28">
+      <c r="C19" s="18">
         <v>9</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -2109,9 +2109,9 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="28"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="18"/>
       <c r="D20" s="6" t="s">
         <v>47</v>
       </c>
@@ -2132,9 +2132,9 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="18"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="20">
+      <c r="A21" s="17"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="19">
         <v>10</v>
       </c>
       <c r="D21" s="6" t="s">
@@ -2157,9 +2157,9 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="20"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="19"/>
       <c r="D22" s="13" t="s">
         <v>51</v>
       </c>
@@ -2180,13 +2180,13 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="C23" s="28">
+      <c r="C23" s="18">
         <v>11</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -2209,9 +2209,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="18"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="28"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="18"/>
       <c r="D24" s="6" t="s">
         <v>56</v>
       </c>
@@ -2232,9 +2232,9 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="28">
+      <c r="A25" s="17"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="18">
         <v>12</v>
       </c>
       <c r="D25" s="6" t="s">
@@ -2257,9 +2257,9 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="18"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="28"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="18"/>
       <c r="D26" s="6" t="s">
         <v>60</v>
       </c>
@@ -2280,13 +2280,13 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="C27" s="28">
+      <c r="C27" s="18">
         <v>13</v>
       </c>
       <c r="D27" s="6" t="s">
@@ -2309,9 +2309,9 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="29"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="28"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="18"/>
       <c r="D28" s="6" t="s">
         <v>65</v>
       </c>
@@ -2332,9 +2332,9 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="29"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="28">
+      <c r="A29" s="16"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="18">
         <v>14</v>
       </c>
       <c r="D29" s="6" t="s">
@@ -2357,9 +2357,9 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="29"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="28"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="18"/>
       <c r="D30" s="6" t="s">
         <v>69</v>
       </c>
@@ -2380,13 +2380,13 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="27" t="s">
+      <c r="B31" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="C31" s="28">
+      <c r="C31" s="18">
         <v>15</v>
       </c>
       <c r="D31" s="6" t="s">
@@ -2409,9 +2409,9 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="29"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="28"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="18"/>
       <c r="D32" s="6" t="s">
         <v>74</v>
       </c>
@@ -2432,9 +2432,9 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="29"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="28">
+      <c r="A33" s="16"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="18">
         <v>16</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -2457,9 +2457,9 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="29"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="28"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="18"/>
       <c r="D34" s="6" t="s">
         <v>78</v>
       </c>
@@ -2480,13 +2480,13 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="C35" s="28">
+      <c r="C35" s="18">
         <v>17</v>
       </c>
       <c r="D35" s="6" t="s">
@@ -2509,9 +2509,9 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="29"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="28"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="18"/>
       <c r="D36" s="6" t="s">
         <v>83</v>
       </c>
@@ -2532,13 +2532,13 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="B37" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="C37" s="28">
+      <c r="C37" s="18">
         <v>18</v>
       </c>
       <c r="D37" s="6" t="s">
@@ -2561,9 +2561,9 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="29"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="28"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="18"/>
       <c r="D38" s="6" t="s">
         <v>88</v>
       </c>
@@ -2584,9 +2584,9 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="29"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="28">
+      <c r="A39" s="16"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="18">
         <v>19</v>
       </c>
       <c r="D39" s="6" t="s">
@@ -2609,9 +2609,9 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="29"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="28"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="18"/>
       <c r="D40" s="6" t="s">
         <v>92</v>
       </c>
@@ -2632,13 +2632,13 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="29" t="s">
+      <c r="A41" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B41" s="27" t="s">
+      <c r="B41" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="C41" s="28">
+      <c r="C41" s="18">
         <v>20</v>
       </c>
       <c r="D41" s="6" t="s">
@@ -2661,9 +2661,9 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="29"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="28"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="18"/>
       <c r="D42" s="6" t="s">
         <v>97</v>
       </c>
@@ -2684,9 +2684,9 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="29"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="28">
+      <c r="A43" s="16"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="18">
         <v>21</v>
       </c>
       <c r="D43" s="6" t="s">
@@ -2709,9 +2709,9 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="29"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="28"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="18"/>
       <c r="D44" s="6" t="s">
         <v>101</v>
       </c>
@@ -2732,13 +2732,13 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="29" t="s">
+      <c r="A45" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="B45" s="27" t="s">
+      <c r="B45" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="C45" s="28">
+      <c r="C45" s="18">
         <v>22</v>
       </c>
       <c r="D45" s="6" t="s">
@@ -2761,9 +2761,9 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="29"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="28"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="18"/>
       <c r="D46" s="6" t="s">
         <v>106</v>
       </c>
@@ -2784,13 +2784,13 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="29" t="s">
+      <c r="A47" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B47" s="27" t="s">
+      <c r="B47" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="C47" s="28">
+      <c r="C47" s="18">
         <v>23</v>
       </c>
       <c r="D47" s="6" t="s">
@@ -2813,9 +2813,9 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="29"/>
-      <c r="B48" s="27"/>
-      <c r="C48" s="28"/>
+      <c r="A48" s="16"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="18"/>
       <c r="D48" s="6" t="s">
         <v>111</v>
       </c>
@@ -2836,9 +2836,9 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="29"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="28">
+      <c r="A49" s="16"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="18">
         <v>24</v>
       </c>
       <c r="D49" s="6" t="s">
@@ -2861,9 +2861,9 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="29"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="28"/>
+      <c r="A50" s="16"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="18"/>
       <c r="D50" s="6" t="s">
         <v>115</v>
       </c>
@@ -2884,13 +2884,13 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="29" t="s">
+      <c r="A51" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B51" s="27" t="s">
+      <c r="B51" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="C51" s="28">
+      <c r="C51" s="18">
         <v>25</v>
       </c>
       <c r="D51" s="6" t="s">
@@ -2913,9 +2913,9 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="29"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="28"/>
+      <c r="A52" s="16"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="18"/>
       <c r="D52" s="6" t="s">
         <v>120</v>
       </c>
@@ -2936,13 +2936,13 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="18" t="s">
+      <c r="A53" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B53" s="26" t="s">
+      <c r="B53" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="C53" s="28">
+      <c r="C53" s="18">
         <v>26</v>
       </c>
       <c r="D53" s="6" t="s">
@@ -2965,9 +2965,9 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="18"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="28"/>
+      <c r="A54" s="16"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="18"/>
       <c r="D54" s="6" t="s">
         <v>125</v>
       </c>
@@ -2988,9 +2988,9 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="18"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="20">
+      <c r="A55" s="16"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="19">
         <v>27</v>
       </c>
       <c r="D55" s="6" t="s">
@@ -3013,9 +3013,9 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="18"/>
-      <c r="B56" s="26"/>
-      <c r="C56" s="20"/>
+      <c r="A56" s="16"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="19"/>
       <c r="D56" s="13" t="s">
         <v>129</v>
       </c>
@@ -3036,13 +3036,13 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="18" t="s">
+      <c r="A57" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="B57" s="26" t="s">
+      <c r="B57" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="C57" s="20">
+      <c r="C57" s="18">
         <v>28</v>
       </c>
       <c r="D57" s="6" t="s">
@@ -3065,28 +3065,32 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="18"/>
-      <c r="B58" s="26"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="1" t="s">
+      <c r="A58" s="17"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F58" s="1" t="s">
+      <c r="E58" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F58" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="G58" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
+      <c r="G58" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="H58" s="5">
+        <v>2</v>
+      </c>
+      <c r="I58" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="18"/>
-      <c r="B59" s="26"/>
-      <c r="C59" s="20">
+      <c r="A59" s="17"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="19">
         <v>29</v>
       </c>
       <c r="D59" s="1" t="s">
@@ -3105,9 +3109,9 @@
       <c r="I59" s="4"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="18"/>
-      <c r="B60" s="26"/>
-      <c r="C60" s="20"/>
+      <c r="A60" s="17"/>
+      <c r="B60" s="21"/>
+      <c r="C60" s="19"/>
       <c r="D60" s="1" t="s">
         <v>138</v>
       </c>
@@ -3124,13 +3128,13 @@
       <c r="I60" s="4"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="18" t="s">
+      <c r="A61" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="B61" s="26" t="s">
+      <c r="B61" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="C61" s="20">
+      <c r="C61" s="19">
         <v>30</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -3149,9 +3153,9 @@
       <c r="I61" s="4"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="18"/>
-      <c r="B62" s="26"/>
-      <c r="C62" s="20"/>
+      <c r="A62" s="17"/>
+      <c r="B62" s="21"/>
+      <c r="C62" s="19"/>
       <c r="D62" s="1" t="s">
         <v>143</v>
       </c>
@@ -3168,9 +3172,9 @@
       <c r="I62" s="4"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="18"/>
-      <c r="B63" s="26"/>
-      <c r="C63" s="20">
+      <c r="A63" s="17"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="19">
         <v>31</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -3189,9 +3193,9 @@
       <c r="I63" s="4"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="18"/>
-      <c r="B64" s="26"/>
-      <c r="C64" s="20"/>
+      <c r="A64" s="17"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="19"/>
       <c r="D64" s="1" t="s">
         <v>147</v>
       </c>
@@ -3208,13 +3212,13 @@
       <c r="I64" s="4"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="18" t="s">
+      <c r="A65" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="B65" s="26" t="s">
+      <c r="B65" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="C65" s="20">
+      <c r="C65" s="19">
         <v>32</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -3233,9 +3237,9 @@
       <c r="I65" s="4"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="18"/>
-      <c r="B66" s="26"/>
-      <c r="C66" s="20"/>
+      <c r="A66" s="17"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="19"/>
       <c r="D66" s="1" t="s">
         <v>152</v>
       </c>
@@ -3252,9 +3256,9 @@
       <c r="I66" s="4"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="18"/>
-      <c r="B67" s="26"/>
-      <c r="C67" s="20">
+      <c r="A67" s="17"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="19">
         <v>33</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -3273,9 +3277,9 @@
       <c r="I67" s="4"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="18"/>
-      <c r="B68" s="26"/>
-      <c r="C68" s="20"/>
+      <c r="A68" s="17"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="19"/>
       <c r="D68" s="1" t="s">
         <v>156</v>
       </c>
@@ -3292,13 +3296,13 @@
       <c r="I68" s="4"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="18" t="s">
+      <c r="A69" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="B69" s="26" t="s">
+      <c r="B69" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="C69" s="20">
+      <c r="C69" s="19">
         <v>34</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -3317,9 +3321,9 @@
       <c r="I69" s="4"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="18"/>
-      <c r="B70" s="26"/>
-      <c r="C70" s="20"/>
+      <c r="A70" s="17"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="19"/>
       <c r="D70" s="1" t="s">
         <v>161</v>
       </c>
@@ -3336,13 +3340,13 @@
       <c r="I70" s="4"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="18" t="s">
+      <c r="A71" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="B71" s="26" t="s">
+      <c r="B71" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="C71" s="20">
+      <c r="C71" s="19">
         <v>35</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -3361,9 +3365,9 @@
       <c r="I71" s="4"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="18"/>
-      <c r="B72" s="26"/>
-      <c r="C72" s="20"/>
+      <c r="A72" s="17"/>
+      <c r="B72" s="21"/>
+      <c r="C72" s="19"/>
       <c r="D72" s="1" t="s">
         <v>166</v>
       </c>
@@ -3380,9 +3384,9 @@
       <c r="I72" s="4"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="18"/>
-      <c r="B73" s="26"/>
-      <c r="C73" s="20">
+      <c r="A73" s="17"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="19">
         <v>36</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -3401,9 +3405,9 @@
       <c r="I73" s="4"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="18"/>
-      <c r="B74" s="26"/>
-      <c r="C74" s="20"/>
+      <c r="A74" s="17"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="19"/>
       <c r="D74" s="1" t="s">
         <v>170</v>
       </c>
@@ -3420,13 +3424,13 @@
       <c r="I74" s="4"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="18" t="s">
+      <c r="A75" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="B75" s="26" t="s">
+      <c r="B75" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="C75" s="20">
+      <c r="C75" s="19">
         <v>37</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -3445,9 +3449,9 @@
       <c r="I75" s="4"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="18"/>
-      <c r="B76" s="26"/>
-      <c r="C76" s="20"/>
+      <c r="A76" s="17"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="19"/>
       <c r="D76" s="1" t="s">
         <v>175</v>
       </c>
@@ -3464,9 +3468,9 @@
       <c r="I76" s="4"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="18"/>
-      <c r="B77" s="26"/>
-      <c r="C77" s="20">
+      <c r="A77" s="17"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="19">
         <v>38</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -3485,9 +3489,9 @@
       <c r="I77" s="4"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="18"/>
-      <c r="B78" s="26"/>
-      <c r="C78" s="20"/>
+      <c r="A78" s="17"/>
+      <c r="B78" s="21"/>
+      <c r="C78" s="19"/>
       <c r="D78" s="1" t="s">
         <v>179</v>
       </c>
@@ -3504,13 +3508,13 @@
       <c r="I78" s="4"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="18" t="s">
+      <c r="A79" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="B79" s="26" t="s">
+      <c r="B79" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="C79" s="20">
+      <c r="C79" s="19">
         <v>39</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -3529,9 +3533,9 @@
       <c r="I79" s="4"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="18"/>
-      <c r="B80" s="26"/>
-      <c r="C80" s="20"/>
+      <c r="A80" s="17"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="19"/>
       <c r="D80" s="1" t="s">
         <v>184</v>
       </c>
@@ -3548,13 +3552,13 @@
       <c r="I80" s="4"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="18" t="s">
+      <c r="A81" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="B81" s="26" t="s">
+      <c r="B81" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="C81" s="20">
+      <c r="C81" s="19">
         <v>40</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -3573,9 +3577,9 @@
       <c r="I81" s="4"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="18"/>
-      <c r="B82" s="26"/>
-      <c r="C82" s="20"/>
+      <c r="A82" s="17"/>
+      <c r="B82" s="21"/>
+      <c r="C82" s="19"/>
       <c r="D82" s="1" t="s">
         <v>189</v>
       </c>
@@ -3592,13 +3596,13 @@
       <c r="I82" s="4"/>
     </row>
     <row r="83" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="18" t="s">
+      <c r="A83" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="B83" s="23" t="s">
+      <c r="B83" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="C83" s="20">
+      <c r="C83" s="19">
         <v>41</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -3617,9 +3621,9 @@
       <c r="I83" s="4"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="18"/>
-      <c r="B84" s="24"/>
-      <c r="C84" s="20"/>
+      <c r="A84" s="17"/>
+      <c r="B84" s="28"/>
+      <c r="C84" s="19"/>
       <c r="D84" s="1" t="s">
         <v>194</v>
       </c>
@@ -3636,9 +3640,9 @@
       <c r="I84" s="4"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="18"/>
-      <c r="B85" s="24"/>
-      <c r="C85" s="20">
+      <c r="A85" s="17"/>
+      <c r="B85" s="28"/>
+      <c r="C85" s="19">
         <v>42</v>
       </c>
       <c r="D85" s="2" t="s">
@@ -3657,9 +3661,9 @@
       <c r="I85" s="4"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="18"/>
-      <c r="B86" s="25"/>
-      <c r="C86" s="20"/>
+      <c r="A86" s="17"/>
+      <c r="B86" s="29"/>
+      <c r="C86" s="19"/>
       <c r="D86" s="2" t="s">
         <v>221</v>
       </c>
@@ -3676,13 +3680,13 @@
       <c r="I86" s="4"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="18" t="s">
+      <c r="A87" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="B87" s="26" t="s">
+      <c r="B87" s="21" t="s">
         <v>301</v>
       </c>
-      <c r="C87" s="20">
+      <c r="C87" s="19">
         <v>43</v>
       </c>
       <c r="D87" s="2" t="s">
@@ -3701,11 +3705,11 @@
       <c r="I87" s="4"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="18"/>
-      <c r="B88" s="19" t="s">
+      <c r="A88" s="17"/>
+      <c r="B88" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C88" s="20"/>
+      <c r="C88" s="19"/>
       <c r="D88" s="2" t="s">
         <v>226</v>
       </c>
@@ -3722,11 +3726,11 @@
       <c r="I88" s="4"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" s="18"/>
-      <c r="B89" s="19" t="s">
+      <c r="A89" s="17"/>
+      <c r="B89" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C89" s="20">
+      <c r="C89" s="19">
         <v>44</v>
       </c>
       <c r="D89" s="2" t="s">
@@ -3745,11 +3749,11 @@
       <c r="I89" s="4"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90" s="18"/>
-      <c r="B90" s="19" t="s">
+      <c r="A90" s="17"/>
+      <c r="B90" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C90" s="20"/>
+      <c r="C90" s="19"/>
       <c r="D90" s="2" t="s">
         <v>230</v>
       </c>
@@ -3766,13 +3770,13 @@
       <c r="I90" s="4"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91" s="18" t="s">
+      <c r="A91" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="B91" s="26" t="s">
+      <c r="B91" s="21" t="s">
         <v>302</v>
       </c>
-      <c r="C91" s="20">
+      <c r="C91" s="19">
         <v>45</v>
       </c>
       <c r="D91" s="2" t="s">
@@ -3791,11 +3795,11 @@
       <c r="I91" s="4"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A92" s="18"/>
-      <c r="B92" s="19" t="s">
+      <c r="A92" s="17"/>
+      <c r="B92" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C92" s="20"/>
+      <c r="C92" s="19"/>
       <c r="D92" s="2" t="s">
         <v>235</v>
       </c>
@@ -3812,11 +3816,11 @@
       <c r="I92" s="4"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" s="18"/>
-      <c r="B93" s="19" t="s">
+      <c r="A93" s="17"/>
+      <c r="B93" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C93" s="20">
+      <c r="C93" s="19">
         <v>46</v>
       </c>
       <c r="D93" s="2" t="s">
@@ -3835,11 +3839,11 @@
       <c r="I93" s="4"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94" s="18"/>
-      <c r="B94" s="19" t="s">
+      <c r="A94" s="17"/>
+      <c r="B94" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C94" s="20"/>
+      <c r="C94" s="19"/>
       <c r="D94" s="2" t="s">
         <v>239</v>
       </c>
@@ -3856,13 +3860,13 @@
       <c r="I94" s="4"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95" s="18" t="s">
+      <c r="A95" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="B95" s="26" t="s">
+      <c r="B95" s="21" t="s">
         <v>303</v>
       </c>
-      <c r="C95" s="20">
+      <c r="C95" s="19">
         <v>47</v>
       </c>
       <c r="D95" s="2" t="s">
@@ -3881,11 +3885,11 @@
       <c r="I95" s="4"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A96" s="18"/>
-      <c r="B96" s="19" t="s">
+      <c r="A96" s="17"/>
+      <c r="B96" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C96" s="20"/>
+      <c r="C96" s="19"/>
       <c r="D96" s="2" t="s">
         <v>244</v>
       </c>
@@ -3902,11 +3906,11 @@
       <c r="I96" s="4"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97" s="18"/>
-      <c r="B97" s="19" t="s">
+      <c r="A97" s="17"/>
+      <c r="B97" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C97" s="20">
+      <c r="C97" s="19">
         <v>48</v>
       </c>
       <c r="D97" s="2" t="s">
@@ -3925,11 +3929,11 @@
       <c r="I97" s="4"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98" s="18"/>
-      <c r="B98" s="19" t="s">
+      <c r="A98" s="17"/>
+      <c r="B98" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C98" s="20"/>
+      <c r="C98" s="19"/>
       <c r="D98" s="2" t="s">
         <v>248</v>
       </c>
@@ -3946,13 +3950,13 @@
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" s="18" t="s">
+      <c r="A99" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="B99" s="26" t="s">
+      <c r="B99" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="C99" s="20">
+      <c r="C99" s="19">
         <v>49</v>
       </c>
       <c r="D99" s="2" t="s">
@@ -3971,11 +3975,11 @@
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" s="18"/>
-      <c r="B100" s="19" t="s">
+      <c r="A100" s="17"/>
+      <c r="B100" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C100" s="20"/>
+      <c r="C100" s="19"/>
       <c r="D100" s="2" t="s">
         <v>253</v>
       </c>
@@ -3992,11 +3996,11 @@
       <c r="I100" s="4"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101" s="18"/>
-      <c r="B101" s="19" t="s">
+      <c r="A101" s="17"/>
+      <c r="B101" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C101" s="20">
+      <c r="C101" s="19">
         <v>50</v>
       </c>
       <c r="D101" s="2" t="s">
@@ -4015,11 +4019,11 @@
       <c r="I101" s="4"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A102" s="18"/>
-      <c r="B102" s="19" t="s">
+      <c r="A102" s="17"/>
+      <c r="B102" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C102" s="20"/>
+      <c r="C102" s="19"/>
       <c r="D102" s="2" t="s">
         <v>257</v>
       </c>
@@ -4036,13 +4040,13 @@
       <c r="I102" s="4"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A103" s="18" t="s">
+      <c r="A103" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="B103" s="26" t="s">
+      <c r="B103" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="C103" s="20">
+      <c r="C103" s="19">
         <v>51</v>
       </c>
       <c r="D103" s="2" t="s">
@@ -4061,11 +4065,11 @@
       <c r="I103" s="4"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" s="18"/>
-      <c r="B104" s="19" t="s">
+      <c r="A104" s="17"/>
+      <c r="B104" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C104" s="20"/>
+      <c r="C104" s="19"/>
       <c r="D104" s="2" t="s">
         <v>60</v>
       </c>
@@ -4082,13 +4086,13 @@
       <c r="I104" s="4"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A105" s="18" t="s">
+      <c r="A105" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="B105" s="19" t="s">
+      <c r="B105" s="22" t="s">
         <v>263</v>
       </c>
-      <c r="C105" s="20">
+      <c r="C105" s="19">
         <v>52</v>
       </c>
       <c r="D105" s="2" t="s">
@@ -4107,11 +4111,11 @@
       <c r="I105" s="4"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A106" s="18"/>
-      <c r="B106" s="19" t="s">
+      <c r="A106" s="17"/>
+      <c r="B106" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C106" s="20"/>
+      <c r="C106" s="19"/>
       <c r="D106" s="2" t="s">
         <v>24</v>
       </c>
@@ -4128,11 +4132,11 @@
       <c r="I106" s="4"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A107" s="18"/>
-      <c r="B107" s="19" t="s">
+      <c r="A107" s="17"/>
+      <c r="B107" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C107" s="20">
+      <c r="C107" s="19">
         <v>53</v>
       </c>
       <c r="D107" s="2" t="s">
@@ -4151,11 +4155,11 @@
       <c r="I107" s="4"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A108" s="18"/>
-      <c r="B108" s="19" t="s">
+      <c r="A108" s="17"/>
+      <c r="B108" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C108" s="20"/>
+      <c r="C108" s="19"/>
       <c r="D108" s="2" t="s">
         <v>136</v>
       </c>
@@ -4172,13 +4176,13 @@
       <c r="I108" s="4"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" s="18" t="s">
+      <c r="A109" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="B109" s="26" t="s">
+      <c r="B109" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="C109" s="20">
+      <c r="C109" s="19">
         <v>54</v>
       </c>
       <c r="D109" s="2" t="s">
@@ -4197,11 +4201,11 @@
       <c r="I109" s="4"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A110" s="18"/>
-      <c r="B110" s="19" t="s">
+      <c r="A110" s="17"/>
+      <c r="B110" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C110" s="20"/>
+      <c r="C110" s="19"/>
       <c r="D110" s="2" t="s">
         <v>269</v>
       </c>
@@ -4218,13 +4222,13 @@
       <c r="I110" s="4"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A111" s="18" t="s">
+      <c r="A111" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="B111" s="26" t="s">
+      <c r="B111" s="21" t="s">
         <v>307</v>
       </c>
-      <c r="C111" s="20">
+      <c r="C111" s="19">
         <v>55</v>
       </c>
       <c r="D111" s="2" t="s">
@@ -4243,11 +4247,11 @@
       <c r="I111" s="4"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A112" s="18"/>
-      <c r="B112" s="19" t="s">
+      <c r="A112" s="17"/>
+      <c r="B112" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C112" s="20"/>
+      <c r="C112" s="19"/>
       <c r="D112" s="2" t="s">
         <v>274</v>
       </c>
@@ -4264,13 +4268,13 @@
       <c r="I112" s="4"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A113" s="18" t="s">
+      <c r="A113" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="B113" s="19" t="s">
+      <c r="B113" s="22" t="s">
         <v>277</v>
       </c>
-      <c r="C113" s="20">
+      <c r="C113" s="19">
         <v>56</v>
       </c>
       <c r="D113" s="2" t="s">
@@ -4289,11 +4293,11 @@
       <c r="I113" s="4"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A114" s="18"/>
-      <c r="B114" s="19" t="s">
+      <c r="A114" s="17"/>
+      <c r="B114" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C114" s="20"/>
+      <c r="C114" s="19"/>
       <c r="D114" s="2" t="s">
         <v>280</v>
       </c>
@@ -4310,11 +4314,11 @@
       <c r="I114" s="4"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A115" s="18"/>
-      <c r="B115" s="19" t="s">
+      <c r="A115" s="17"/>
+      <c r="B115" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C115" s="20">
+      <c r="C115" s="19">
         <v>57</v>
       </c>
       <c r="D115" s="2" t="s">
@@ -4333,11 +4337,11 @@
       <c r="I115" s="4"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A116" s="18"/>
-      <c r="B116" s="19" t="s">
+      <c r="A116" s="17"/>
+      <c r="B116" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C116" s="20"/>
+      <c r="C116" s="19"/>
       <c r="D116" s="2" t="s">
         <v>284</v>
       </c>
@@ -4354,13 +4358,13 @@
       <c r="I116" s="4"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A117" s="18" t="s">
+      <c r="A117" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="B117" s="19" t="s">
+      <c r="B117" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="C117" s="20">
+      <c r="C117" s="19">
         <v>58</v>
       </c>
       <c r="D117" s="2" t="s">
@@ -4379,11 +4383,11 @@
       <c r="I117" s="4"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A118" s="18"/>
-      <c r="B118" s="19" t="s">
+      <c r="A118" s="17"/>
+      <c r="B118" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C118" s="20"/>
+      <c r="C118" s="19"/>
       <c r="D118" s="2" t="s">
         <v>290</v>
       </c>
@@ -4400,11 +4404,11 @@
       <c r="I118" s="4"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A119" s="18"/>
-      <c r="B119" s="19" t="s">
+      <c r="A119" s="17"/>
+      <c r="B119" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C119" s="20">
+      <c r="C119" s="19">
         <v>59</v>
       </c>
       <c r="D119" s="2" t="s">
@@ -4423,11 +4427,11 @@
       <c r="I119" s="4"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A120" s="18"/>
-      <c r="B120" s="19" t="s">
+      <c r="A120" s="17"/>
+      <c r="B120" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C120" s="20"/>
+      <c r="C120" s="19"/>
       <c r="D120" s="2" t="s">
         <v>292</v>
       </c>
@@ -4444,13 +4448,13 @@
       <c r="I120" s="4"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" s="18" t="s">
+      <c r="A121" s="17" t="s">
         <v>294</v>
       </c>
-      <c r="B121" s="19" t="s">
+      <c r="B121" s="22" t="s">
         <v>295</v>
       </c>
-      <c r="C121" s="20">
+      <c r="C121" s="19">
         <v>60</v>
       </c>
       <c r="D121" s="2" t="s">
@@ -4469,9 +4473,9 @@
       <c r="I121" s="4"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A122" s="18"/>
-      <c r="B122" s="19"/>
-      <c r="C122" s="20"/>
+      <c r="A122" s="17"/>
+      <c r="B122" s="22"/>
+      <c r="C122" s="19"/>
       <c r="D122" s="2" t="s">
         <v>298</v>
       </c>
@@ -4488,9 +4492,9 @@
       <c r="I122" s="4"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A123" s="18"/>
-      <c r="B123" s="19"/>
-      <c r="C123" s="20">
+      <c r="A123" s="17"/>
+      <c r="B123" s="22"/>
+      <c r="C123" s="19">
         <v>61</v>
       </c>
       <c r="D123" s="2" t="s">
@@ -4509,9 +4513,9 @@
       <c r="I123" s="4"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A124" s="18"/>
-      <c r="B124" s="19"/>
-      <c r="C124" s="20"/>
+      <c r="A124" s="17"/>
+      <c r="B124" s="22"/>
+      <c r="C124" s="19"/>
       <c r="D124" s="2" t="s">
         <v>310</v>
       </c>
@@ -4528,9 +4532,9 @@
       <c r="I124" s="4"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A125" s="18"/>
-      <c r="B125" s="19"/>
-      <c r="C125" s="20">
+      <c r="A125" s="17"/>
+      <c r="B125" s="22"/>
+      <c r="C125" s="19">
         <v>62</v>
       </c>
       <c r="D125" s="2" t="s">
@@ -4549,9 +4553,9 @@
       <c r="I125" s="4"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A126" s="18"/>
-      <c r="B126" s="19"/>
-      <c r="C126" s="20"/>
+      <c r="A126" s="17"/>
+      <c r="B126" s="22"/>
+      <c r="C126" s="19"/>
       <c r="D126" s="2" t="s">
         <v>314</v>
       </c>
@@ -4569,15 +4573,114 @@
     </row>
   </sheetData>
   <mergeCells count="141">
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A121:A126"/>
+    <mergeCell ref="B121:B126"/>
+    <mergeCell ref="C121:C122"/>
+    <mergeCell ref="C123:C124"/>
+    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C115:C116"/>
+    <mergeCell ref="C117:C118"/>
+    <mergeCell ref="C119:C120"/>
+    <mergeCell ref="B83:B86"/>
+    <mergeCell ref="C105:C106"/>
+    <mergeCell ref="C107:C108"/>
+    <mergeCell ref="C109:C110"/>
+    <mergeCell ref="C111:C112"/>
+    <mergeCell ref="C113:C114"/>
+    <mergeCell ref="C95:C96"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="C101:C102"/>
+    <mergeCell ref="C103:C104"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="C93:C94"/>
+    <mergeCell ref="A117:A120"/>
+    <mergeCell ref="B87:B90"/>
+    <mergeCell ref="B91:B94"/>
+    <mergeCell ref="B95:B98"/>
+    <mergeCell ref="B99:B102"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="B111:B112"/>
+    <mergeCell ref="B113:B116"/>
+    <mergeCell ref="B117:B120"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A113:A116"/>
+    <mergeCell ref="A83:A86"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="A91:A94"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="A99:A102"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="C83:C84"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C47:C48"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C19:C20"/>
@@ -4602,114 +4705,15 @@
     <mergeCell ref="A71:A74"/>
     <mergeCell ref="A61:A64"/>
     <mergeCell ref="A65:A68"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="C83:C84"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A83:A86"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="A91:A94"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="A99:A102"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B71:B74"/>
-    <mergeCell ref="B75:B78"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A117:A120"/>
-    <mergeCell ref="B87:B90"/>
-    <mergeCell ref="B91:B94"/>
-    <mergeCell ref="B95:B98"/>
-    <mergeCell ref="B99:B102"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="B109:B110"/>
-    <mergeCell ref="B111:B112"/>
-    <mergeCell ref="B113:B116"/>
-    <mergeCell ref="B117:B120"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A113:A116"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="C103:C104"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="A121:A126"/>
-    <mergeCell ref="B121:B126"/>
-    <mergeCell ref="C121:C122"/>
-    <mergeCell ref="C123:C124"/>
-    <mergeCell ref="C125:C126"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C115:C116"/>
-    <mergeCell ref="C117:C118"/>
-    <mergeCell ref="C119:C120"/>
-    <mergeCell ref="B83:B86"/>
-    <mergeCell ref="C105:C106"/>
-    <mergeCell ref="C107:C108"/>
-    <mergeCell ref="C109:C110"/>
-    <mergeCell ref="C111:C112"/>
-    <mergeCell ref="C113:C114"/>
-    <mergeCell ref="C95:C96"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A51:A52"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G126" xr:uid="{BD7D4049-E182-46D9-ABFE-ED680993C7C2}">
@@ -4772,9 +4776,10 @@
     <hyperlink ref="F55" r:id="rId53" xr:uid="{20B09360-02CC-402B-B54F-2ED5454AF3D0}"/>
     <hyperlink ref="F56" r:id="rId54" xr:uid="{75E007E6-8645-44B3-9C1C-804E5DF8CEAC}"/>
     <hyperlink ref="F57" r:id="rId55" xr:uid="{EEEFC227-AA75-4FA8-8770-51710CAEA2B9}"/>
+    <hyperlink ref="F58" r:id="rId56" xr:uid="{4C0BA54A-6492-48D4-AC2F-7E75F504E59B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId56"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId57"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
solve task '56. Merge Intervals'
</commit_message>
<xml_diff>
--- a/DSA studing (in acc. with Claude plan)/DSA_Leetcode_plan from Claude.xlsx
+++ b/DSA studing (in acc. with Claude plan)/DSA_Leetcode_plan from Claude.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Programming\Python\Leetcode\Leetcode practise\DSA studing (in acc. with Claude plan)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA09BCF-D7F6-4874-B357-D9130193B24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3ED5F9-1E6E-49C9-92D1-312FE4115DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1223,7 +1223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1268,32 +1268,20 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1309,6 +1297,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1600,7 +1603,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D62" sqref="D62"/>
+      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1616,31 +1619,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="23" t="s">
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="16" t="s">
         <v>318</v>
       </c>
       <c r="J1" s="9" t="s">
@@ -1654,36 +1657,36 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
       <c r="J2" s="10">
         <f>COUNTIF(G3:G126,"решена")/124</f>
-        <v>0.43548387096774194</v>
+        <v>0.44354838709677419</v>
       </c>
       <c r="K2" s="11">
         <f>SUM(H3:H126)/(COUNTIF(G3:G126,"решена") + COUNTIF(G3:G126,"не решена"))</f>
-        <v>2.25</v>
+        <v>2.2456140350877192</v>
       </c>
       <c r="L2" s="10">
         <f>SUM(I3:I126)/SUM(H3:H126)</f>
-        <v>0.73015873015873012</v>
+        <v>0.7265625</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="29">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -1709,9 +1712,9 @@
       <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="18"/>
+      <c r="A4" s="28"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="29"/>
       <c r="D4" s="6" t="s">
         <v>11</v>
       </c>
@@ -1732,9 +1735,9 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="18">
+      <c r="A5" s="28"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="29">
         <v>2</v>
       </c>
       <c r="D5" s="6" t="s">
@@ -1757,9 +1760,9 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="18"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="29"/>
       <c r="D6" s="6" t="s">
         <v>15</v>
       </c>
@@ -1780,13 +1783,13 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="27" t="s">
         <v>324</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="29">
         <v>3</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -1809,9 +1812,9 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="16"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="18"/>
+      <c r="A8" s="28"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="29"/>
       <c r="D8" s="6" t="s">
         <v>20</v>
       </c>
@@ -1832,9 +1835,9 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="18">
+      <c r="A9" s="28"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="29">
         <v>4</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -1857,9 +1860,9 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="18"/>
+      <c r="A10" s="28"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="29"/>
       <c r="D10" s="6" t="s">
         <v>24</v>
       </c>
@@ -1880,13 +1883,13 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="27" t="s">
         <v>197</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="29">
         <v>5</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -1909,9 +1912,9 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="18"/>
+      <c r="A12" s="28"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="29"/>
       <c r="D12" s="6" t="s">
         <v>29</v>
       </c>
@@ -1932,9 +1935,9 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="18">
+      <c r="A13" s="28"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="29">
         <v>6</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -1957,9 +1960,9 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="18"/>
+      <c r="A14" s="28"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="29"/>
       <c r="D14" s="6" t="s">
         <v>33</v>
       </c>
@@ -1980,13 +1983,13 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="26" t="s">
         <v>198</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="29">
         <v>7</v>
       </c>
       <c r="D15" s="6" t="s">
@@ -2009,9 +2012,9 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="18"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="29"/>
       <c r="D16" s="6" t="s">
         <v>38</v>
       </c>
@@ -2032,9 +2035,9 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="18">
+      <c r="A17" s="18"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="29">
         <v>8</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -2057,9 +2060,9 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="18"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="29"/>
       <c r="D18" s="6" t="s">
         <v>42</v>
       </c>
@@ -2080,13 +2083,13 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="26" t="s">
         <v>199</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="29">
         <v>9</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -2109,9 +2112,9 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="18"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="29"/>
       <c r="D20" s="6" t="s">
         <v>47</v>
       </c>
@@ -2132,9 +2135,9 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="19">
+      <c r="A21" s="18"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="20">
         <v>10</v>
       </c>
       <c r="D21" s="6" t="s">
@@ -2157,9 +2160,9 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="19"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="13" t="s">
         <v>51</v>
       </c>
@@ -2180,13 +2183,13 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="29">
         <v>11</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -2209,9 +2212,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="18"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="29"/>
       <c r="D24" s="6" t="s">
         <v>56</v>
       </c>
@@ -2232,9 +2235,9 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="18">
+      <c r="A25" s="18"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="29">
         <v>12</v>
       </c>
       <c r="D25" s="6" t="s">
@@ -2257,9 +2260,9 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="18"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="29"/>
       <c r="D26" s="6" t="s">
         <v>60</v>
       </c>
@@ -2280,13 +2283,13 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C27" s="29">
         <v>13</v>
       </c>
       <c r="D27" s="6" t="s">
@@ -2309,9 +2312,9 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="16"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="18"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="29"/>
       <c r="D28" s="6" t="s">
         <v>65</v>
       </c>
@@ -2332,9 +2335,9 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="16"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="18">
+      <c r="A29" s="28"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="29">
         <v>14</v>
       </c>
       <c r="D29" s="6" t="s">
@@ -2357,9 +2360,9 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="16"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="18"/>
+      <c r="A30" s="28"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="29"/>
       <c r="D30" s="6" t="s">
         <v>69</v>
       </c>
@@ -2380,13 +2383,13 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31" s="29">
         <v>15</v>
       </c>
       <c r="D31" s="6" t="s">
@@ -2409,9 +2412,9 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="16"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="18"/>
+      <c r="A32" s="28"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="29"/>
       <c r="D32" s="6" t="s">
         <v>74</v>
       </c>
@@ -2432,9 +2435,9 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="16"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="18">
+      <c r="A33" s="28"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="29">
         <v>16</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -2457,9 +2460,9 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="16"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="18"/>
+      <c r="A34" s="28"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="29"/>
       <c r="D34" s="6" t="s">
         <v>78</v>
       </c>
@@ -2480,13 +2483,13 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="C35" s="18">
+      <c r="C35" s="29">
         <v>17</v>
       </c>
       <c r="D35" s="6" t="s">
@@ -2509,9 +2512,9 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="16"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="18"/>
+      <c r="A36" s="28"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="29"/>
       <c r="D36" s="6" t="s">
         <v>83</v>
       </c>
@@ -2532,13 +2535,13 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="27" t="s">
         <v>203</v>
       </c>
-      <c r="C37" s="18">
+      <c r="C37" s="29">
         <v>18</v>
       </c>
       <c r="D37" s="6" t="s">
@@ -2561,9 +2564,9 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="16"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="18"/>
+      <c r="A38" s="28"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="29"/>
       <c r="D38" s="6" t="s">
         <v>88</v>
       </c>
@@ -2584,9 +2587,9 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="16"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="18">
+      <c r="A39" s="28"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="29">
         <v>19</v>
       </c>
       <c r="D39" s="6" t="s">
@@ -2609,9 +2612,9 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="16"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="18"/>
+      <c r="A40" s="28"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="29"/>
       <c r="D40" s="6" t="s">
         <v>92</v>
       </c>
@@ -2632,13 +2635,13 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="27" t="s">
         <v>204</v>
       </c>
-      <c r="C41" s="18">
+      <c r="C41" s="29">
         <v>20</v>
       </c>
       <c r="D41" s="6" t="s">
@@ -2661,9 +2664,9 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="16"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="18"/>
+      <c r="A42" s="28"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="29"/>
       <c r="D42" s="6" t="s">
         <v>97</v>
       </c>
@@ -2684,9 +2687,9 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="16"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="18">
+      <c r="A43" s="28"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="29">
         <v>21</v>
       </c>
       <c r="D43" s="6" t="s">
@@ -2709,9 +2712,9 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="16"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="18"/>
+      <c r="A44" s="28"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="29"/>
       <c r="D44" s="6" t="s">
         <v>101</v>
       </c>
@@ -2732,13 +2735,13 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="B45" s="20" t="s">
+      <c r="B45" s="27" t="s">
         <v>205</v>
       </c>
-      <c r="C45" s="18">
+      <c r="C45" s="29">
         <v>22</v>
       </c>
       <c r="D45" s="6" t="s">
@@ -2761,9 +2764,9 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="16"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="18"/>
+      <c r="A46" s="28"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="29"/>
       <c r="D46" s="6" t="s">
         <v>106</v>
       </c>
@@ -2784,13 +2787,13 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="16" t="s">
+      <c r="A47" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="C47" s="18">
+      <c r="C47" s="29">
         <v>23</v>
       </c>
       <c r="D47" s="6" t="s">
@@ -2813,9 +2816,9 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="16"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="18"/>
+      <c r="A48" s="28"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="29"/>
       <c r="D48" s="6" t="s">
         <v>111</v>
       </c>
@@ -2836,9 +2839,9 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="16"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="18">
+      <c r="A49" s="28"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="29">
         <v>24</v>
       </c>
       <c r="D49" s="6" t="s">
@@ -2861,9 +2864,9 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="16"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="18"/>
+      <c r="A50" s="28"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="29"/>
       <c r="D50" s="6" t="s">
         <v>115</v>
       </c>
@@ -2884,13 +2887,13 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="B51" s="27" t="s">
         <v>207</v>
       </c>
-      <c r="C51" s="18">
+      <c r="C51" s="29">
         <v>25</v>
       </c>
       <c r="D51" s="6" t="s">
@@ -2913,9 +2916,9 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="16"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="18"/>
+      <c r="A52" s="28"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="29"/>
       <c r="D52" s="6" t="s">
         <v>120</v>
       </c>
@@ -2936,13 +2939,13 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="16" t="s">
+      <c r="A53" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="27" t="s">
         <v>208</v>
       </c>
-      <c r="C53" s="18">
+      <c r="C53" s="29">
         <v>26</v>
       </c>
       <c r="D53" s="6" t="s">
@@ -2965,9 +2968,9 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="16"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="18"/>
+      <c r="A54" s="28"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="29"/>
       <c r="D54" s="6" t="s">
         <v>125</v>
       </c>
@@ -2988,9 +2991,9 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="16"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="19">
+      <c r="A55" s="28"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="20">
         <v>27</v>
       </c>
       <c r="D55" s="6" t="s">
@@ -3013,9 +3016,9 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="16"/>
-      <c r="B56" s="20"/>
-      <c r="C56" s="19"/>
+      <c r="A56" s="28"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="20"/>
       <c r="D56" s="13" t="s">
         <v>129</v>
       </c>
@@ -3036,13 +3039,13 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="17" t="s">
+      <c r="A57" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="B57" s="21" t="s">
+      <c r="B57" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="C57" s="18">
+      <c r="C57" s="29">
         <v>28</v>
       </c>
       <c r="D57" s="6" t="s">
@@ -3065,9 +3068,9 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="17"/>
-      <c r="B58" s="21"/>
-      <c r="C58" s="18"/>
+      <c r="A58" s="28"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="29"/>
       <c r="D58" s="6" t="s">
         <v>134</v>
       </c>
@@ -3088,37 +3091,41 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="17"/>
-      <c r="B59" s="21"/>
-      <c r="C59" s="19">
+      <c r="A59" s="28"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="20">
         <v>29</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="E59" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F59" s="1" t="s">
+      <c r="E59" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F59" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="G59" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
+      <c r="G59" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="H59" s="5">
+        <v>2</v>
+      </c>
+      <c r="I59" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="17"/>
-      <c r="B60" s="21"/>
-      <c r="C60" s="19"/>
+      <c r="A60" s="28"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="20"/>
       <c r="D60" s="1" t="s">
         <v>138</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F60" s="1" t="s">
+      <c r="F60" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G60" s="4" t="s">
@@ -3128,13 +3135,13 @@
       <c r="I60" s="4"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="17" t="s">
+      <c r="A61" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="B61" s="21" t="s">
+      <c r="B61" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="C61" s="19">
+      <c r="C61" s="20">
         <v>30</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -3153,9 +3160,9 @@
       <c r="I61" s="4"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="17"/>
-      <c r="B62" s="21"/>
-      <c r="C62" s="19"/>
+      <c r="A62" s="18"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="20"/>
       <c r="D62" s="1" t="s">
         <v>143</v>
       </c>
@@ -3172,9 +3179,9 @@
       <c r="I62" s="4"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="17"/>
-      <c r="B63" s="21"/>
-      <c r="C63" s="19">
+      <c r="A63" s="18"/>
+      <c r="B63" s="26"/>
+      <c r="C63" s="20">
         <v>31</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -3193,9 +3200,9 @@
       <c r="I63" s="4"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="17"/>
-      <c r="B64" s="21"/>
-      <c r="C64" s="19"/>
+      <c r="A64" s="18"/>
+      <c r="B64" s="26"/>
+      <c r="C64" s="20"/>
       <c r="D64" s="1" t="s">
         <v>147</v>
       </c>
@@ -3212,13 +3219,13 @@
       <c r="I64" s="4"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="17" t="s">
+      <c r="A65" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="B65" s="21" t="s">
+      <c r="B65" s="26" t="s">
         <v>211</v>
       </c>
-      <c r="C65" s="19">
+      <c r="C65" s="20">
         <v>32</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -3237,9 +3244,9 @@
       <c r="I65" s="4"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="17"/>
-      <c r="B66" s="21"/>
-      <c r="C66" s="19"/>
+      <c r="A66" s="18"/>
+      <c r="B66" s="26"/>
+      <c r="C66" s="20"/>
       <c r="D66" s="1" t="s">
         <v>152</v>
       </c>
@@ -3256,9 +3263,9 @@
       <c r="I66" s="4"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="17"/>
-      <c r="B67" s="21"/>
-      <c r="C67" s="19">
+      <c r="A67" s="18"/>
+      <c r="B67" s="26"/>
+      <c r="C67" s="20">
         <v>33</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -3277,9 +3284,9 @@
       <c r="I67" s="4"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="17"/>
-      <c r="B68" s="21"/>
-      <c r="C68" s="19"/>
+      <c r="A68" s="18"/>
+      <c r="B68" s="26"/>
+      <c r="C68" s="20"/>
       <c r="D68" s="1" t="s">
         <v>156</v>
       </c>
@@ -3296,13 +3303,13 @@
       <c r="I68" s="4"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="17" t="s">
+      <c r="A69" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="B69" s="21" t="s">
+      <c r="B69" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="C69" s="19">
+      <c r="C69" s="20">
         <v>34</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -3321,9 +3328,9 @@
       <c r="I69" s="4"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="17"/>
-      <c r="B70" s="21"/>
-      <c r="C70" s="19"/>
+      <c r="A70" s="18"/>
+      <c r="B70" s="26"/>
+      <c r="C70" s="20"/>
       <c r="D70" s="1" t="s">
         <v>161</v>
       </c>
@@ -3340,13 +3347,13 @@
       <c r="I70" s="4"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="17" t="s">
+      <c r="A71" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="B71" s="21" t="s">
+      <c r="B71" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="C71" s="19">
+      <c r="C71" s="20">
         <v>35</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -3365,9 +3372,9 @@
       <c r="I71" s="4"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="17"/>
-      <c r="B72" s="21"/>
-      <c r="C72" s="19"/>
+      <c r="A72" s="18"/>
+      <c r="B72" s="26"/>
+      <c r="C72" s="20"/>
       <c r="D72" s="1" t="s">
         <v>166</v>
       </c>
@@ -3384,9 +3391,9 @@
       <c r="I72" s="4"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="17"/>
-      <c r="B73" s="21"/>
-      <c r="C73" s="19">
+      <c r="A73" s="18"/>
+      <c r="B73" s="26"/>
+      <c r="C73" s="20">
         <v>36</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -3405,9 +3412,9 @@
       <c r="I73" s="4"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="17"/>
-      <c r="B74" s="21"/>
-      <c r="C74" s="19"/>
+      <c r="A74" s="18"/>
+      <c r="B74" s="26"/>
+      <c r="C74" s="20"/>
       <c r="D74" s="1" t="s">
         <v>170</v>
       </c>
@@ -3424,13 +3431,13 @@
       <c r="I74" s="4"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="17" t="s">
+      <c r="A75" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="B75" s="21" t="s">
+      <c r="B75" s="26" t="s">
         <v>214</v>
       </c>
-      <c r="C75" s="19">
+      <c r="C75" s="20">
         <v>37</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -3449,9 +3456,9 @@
       <c r="I75" s="4"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="17"/>
-      <c r="B76" s="21"/>
-      <c r="C76" s="19"/>
+      <c r="A76" s="18"/>
+      <c r="B76" s="26"/>
+      <c r="C76" s="20"/>
       <c r="D76" s="1" t="s">
         <v>175</v>
       </c>
@@ -3468,9 +3475,9 @@
       <c r="I76" s="4"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="17"/>
-      <c r="B77" s="21"/>
-      <c r="C77" s="19">
+      <c r="A77" s="18"/>
+      <c r="B77" s="26"/>
+      <c r="C77" s="20">
         <v>38</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -3489,9 +3496,9 @@
       <c r="I77" s="4"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="17"/>
-      <c r="B78" s="21"/>
-      <c r="C78" s="19"/>
+      <c r="A78" s="18"/>
+      <c r="B78" s="26"/>
+      <c r="C78" s="20"/>
       <c r="D78" s="1" t="s">
         <v>179</v>
       </c>
@@ -3508,13 +3515,13 @@
       <c r="I78" s="4"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="17" t="s">
+      <c r="A79" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="B79" s="21" t="s">
+      <c r="B79" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="C79" s="19">
+      <c r="C79" s="20">
         <v>39</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -3533,9 +3540,9 @@
       <c r="I79" s="4"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="17"/>
-      <c r="B80" s="21"/>
-      <c r="C80" s="19"/>
+      <c r="A80" s="18"/>
+      <c r="B80" s="26"/>
+      <c r="C80" s="20"/>
       <c r="D80" s="1" t="s">
         <v>184</v>
       </c>
@@ -3552,13 +3559,13 @@
       <c r="I80" s="4"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="17" t="s">
+      <c r="A81" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="B81" s="21" t="s">
+      <c r="B81" s="26" t="s">
         <v>216</v>
       </c>
-      <c r="C81" s="19">
+      <c r="C81" s="20">
         <v>40</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -3577,9 +3584,9 @@
       <c r="I81" s="4"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="17"/>
-      <c r="B82" s="21"/>
-      <c r="C82" s="19"/>
+      <c r="A82" s="18"/>
+      <c r="B82" s="26"/>
+      <c r="C82" s="20"/>
       <c r="D82" s="1" t="s">
         <v>189</v>
       </c>
@@ -3596,13 +3603,13 @@
       <c r="I82" s="4"/>
     </row>
     <row r="83" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="17" t="s">
+      <c r="A83" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="B83" s="27" t="s">
+      <c r="B83" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="C83" s="19">
+      <c r="C83" s="20">
         <v>41</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -3621,9 +3628,9 @@
       <c r="I83" s="4"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="17"/>
-      <c r="B84" s="28"/>
-      <c r="C84" s="19"/>
+      <c r="A84" s="18"/>
+      <c r="B84" s="24"/>
+      <c r="C84" s="20"/>
       <c r="D84" s="1" t="s">
         <v>194</v>
       </c>
@@ -3640,9 +3647,9 @@
       <c r="I84" s="4"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="17"/>
-      <c r="B85" s="28"/>
-      <c r="C85" s="19">
+      <c r="A85" s="18"/>
+      <c r="B85" s="24"/>
+      <c r="C85" s="20">
         <v>42</v>
       </c>
       <c r="D85" s="2" t="s">
@@ -3661,9 +3668,9 @@
       <c r="I85" s="4"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="17"/>
-      <c r="B86" s="29"/>
-      <c r="C86" s="19"/>
+      <c r="A86" s="18"/>
+      <c r="B86" s="25"/>
+      <c r="C86" s="20"/>
       <c r="D86" s="2" t="s">
         <v>221</v>
       </c>
@@ -3680,13 +3687,13 @@
       <c r="I86" s="4"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="17" t="s">
+      <c r="A87" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="B87" s="21" t="s">
+      <c r="B87" s="26" t="s">
         <v>301</v>
       </c>
-      <c r="C87" s="19">
+      <c r="C87" s="20">
         <v>43</v>
       </c>
       <c r="D87" s="2" t="s">
@@ -3705,11 +3712,11 @@
       <c r="I87" s="4"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="17"/>
-      <c r="B88" s="22" t="s">
+      <c r="A88" s="18"/>
+      <c r="B88" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C88" s="19"/>
+      <c r="C88" s="20"/>
       <c r="D88" s="2" t="s">
         <v>226</v>
       </c>
@@ -3726,11 +3733,11 @@
       <c r="I88" s="4"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" s="17"/>
-      <c r="B89" s="22" t="s">
+      <c r="A89" s="18"/>
+      <c r="B89" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C89" s="19">
+      <c r="C89" s="20">
         <v>44</v>
       </c>
       <c r="D89" s="2" t="s">
@@ -3749,11 +3756,11 @@
       <c r="I89" s="4"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90" s="17"/>
-      <c r="B90" s="22" t="s">
+      <c r="A90" s="18"/>
+      <c r="B90" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C90" s="19"/>
+      <c r="C90" s="20"/>
       <c r="D90" s="2" t="s">
         <v>230</v>
       </c>
@@ -3770,13 +3777,13 @@
       <c r="I90" s="4"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91" s="17" t="s">
+      <c r="A91" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="B91" s="21" t="s">
+      <c r="B91" s="26" t="s">
         <v>302</v>
       </c>
-      <c r="C91" s="19">
+      <c r="C91" s="20">
         <v>45</v>
       </c>
       <c r="D91" s="2" t="s">
@@ -3795,11 +3802,11 @@
       <c r="I91" s="4"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A92" s="17"/>
-      <c r="B92" s="22" t="s">
+      <c r="A92" s="18"/>
+      <c r="B92" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C92" s="19"/>
+      <c r="C92" s="20"/>
       <c r="D92" s="2" t="s">
         <v>235</v>
       </c>
@@ -3816,11 +3823,11 @@
       <c r="I92" s="4"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" s="17"/>
-      <c r="B93" s="22" t="s">
+      <c r="A93" s="18"/>
+      <c r="B93" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C93" s="19">
+      <c r="C93" s="20">
         <v>46</v>
       </c>
       <c r="D93" s="2" t="s">
@@ -3839,11 +3846,11 @@
       <c r="I93" s="4"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94" s="17"/>
-      <c r="B94" s="22" t="s">
+      <c r="A94" s="18"/>
+      <c r="B94" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C94" s="19"/>
+      <c r="C94" s="20"/>
       <c r="D94" s="2" t="s">
         <v>239</v>
       </c>
@@ -3860,13 +3867,13 @@
       <c r="I94" s="4"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95" s="17" t="s">
+      <c r="A95" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="B95" s="21" t="s">
+      <c r="B95" s="26" t="s">
         <v>303</v>
       </c>
-      <c r="C95" s="19">
+      <c r="C95" s="20">
         <v>47</v>
       </c>
       <c r="D95" s="2" t="s">
@@ -3885,11 +3892,11 @@
       <c r="I95" s="4"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A96" s="17"/>
-      <c r="B96" s="22" t="s">
+      <c r="A96" s="18"/>
+      <c r="B96" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C96" s="19"/>
+      <c r="C96" s="20"/>
       <c r="D96" s="2" t="s">
         <v>244</v>
       </c>
@@ -3906,11 +3913,11 @@
       <c r="I96" s="4"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97" s="17"/>
-      <c r="B97" s="22" t="s">
+      <c r="A97" s="18"/>
+      <c r="B97" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C97" s="19">
+      <c r="C97" s="20">
         <v>48</v>
       </c>
       <c r="D97" s="2" t="s">
@@ -3929,11 +3936,11 @@
       <c r="I97" s="4"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98" s="17"/>
-      <c r="B98" s="22" t="s">
+      <c r="A98" s="18"/>
+      <c r="B98" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C98" s="19"/>
+      <c r="C98" s="20"/>
       <c r="D98" s="2" t="s">
         <v>248</v>
       </c>
@@ -3950,13 +3957,13 @@
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" s="17" t="s">
+      <c r="A99" s="18" t="s">
         <v>250</v>
       </c>
-      <c r="B99" s="21" t="s">
+      <c r="B99" s="26" t="s">
         <v>304</v>
       </c>
-      <c r="C99" s="19">
+      <c r="C99" s="20">
         <v>49</v>
       </c>
       <c r="D99" s="2" t="s">
@@ -3975,11 +3982,11 @@
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" s="17"/>
-      <c r="B100" s="22" t="s">
+      <c r="A100" s="18"/>
+      <c r="B100" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C100" s="19"/>
+      <c r="C100" s="20"/>
       <c r="D100" s="2" t="s">
         <v>253</v>
       </c>
@@ -3996,11 +4003,11 @@
       <c r="I100" s="4"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101" s="17"/>
-      <c r="B101" s="22" t="s">
+      <c r="A101" s="18"/>
+      <c r="B101" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C101" s="19">
+      <c r="C101" s="20">
         <v>50</v>
       </c>
       <c r="D101" s="2" t="s">
@@ -4019,11 +4026,11 @@
       <c r="I101" s="4"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A102" s="17"/>
-      <c r="B102" s="22" t="s">
+      <c r="A102" s="18"/>
+      <c r="B102" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C102" s="19"/>
+      <c r="C102" s="20"/>
       <c r="D102" s="2" t="s">
         <v>257</v>
       </c>
@@ -4040,13 +4047,13 @@
       <c r="I102" s="4"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A103" s="17" t="s">
+      <c r="A103" s="18" t="s">
         <v>259</v>
       </c>
-      <c r="B103" s="21" t="s">
+      <c r="B103" s="26" t="s">
         <v>305</v>
       </c>
-      <c r="C103" s="19">
+      <c r="C103" s="20">
         <v>51</v>
       </c>
       <c r="D103" s="2" t="s">
@@ -4065,11 +4072,11 @@
       <c r="I103" s="4"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" s="17"/>
-      <c r="B104" s="22" t="s">
+      <c r="A104" s="18"/>
+      <c r="B104" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C104" s="19"/>
+      <c r="C104" s="20"/>
       <c r="D104" s="2" t="s">
         <v>60</v>
       </c>
@@ -4086,13 +4093,13 @@
       <c r="I104" s="4"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A105" s="17" t="s">
+      <c r="A105" s="18" t="s">
         <v>262</v>
       </c>
-      <c r="B105" s="22" t="s">
+      <c r="B105" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="C105" s="19">
+      <c r="C105" s="20">
         <v>52</v>
       </c>
       <c r="D105" s="2" t="s">
@@ -4111,11 +4118,11 @@
       <c r="I105" s="4"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A106" s="17"/>
-      <c r="B106" s="22" t="s">
+      <c r="A106" s="18"/>
+      <c r="B106" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C106" s="19"/>
+      <c r="C106" s="20"/>
       <c r="D106" s="2" t="s">
         <v>24</v>
       </c>
@@ -4132,11 +4139,11 @@
       <c r="I106" s="4"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A107" s="17"/>
-      <c r="B107" s="22" t="s">
+      <c r="A107" s="18"/>
+      <c r="B107" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C107" s="19">
+      <c r="C107" s="20">
         <v>53</v>
       </c>
       <c r="D107" s="2" t="s">
@@ -4155,11 +4162,11 @@
       <c r="I107" s="4"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A108" s="17"/>
-      <c r="B108" s="22" t="s">
+      <c r="A108" s="18"/>
+      <c r="B108" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C108" s="19"/>
+      <c r="C108" s="20"/>
       <c r="D108" s="2" t="s">
         <v>136</v>
       </c>
@@ -4176,13 +4183,13 @@
       <c r="I108" s="4"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" s="17" t="s">
+      <c r="A109" s="18" t="s">
         <v>266</v>
       </c>
-      <c r="B109" s="21" t="s">
+      <c r="B109" s="26" t="s">
         <v>306</v>
       </c>
-      <c r="C109" s="19">
+      <c r="C109" s="20">
         <v>54</v>
       </c>
       <c r="D109" s="2" t="s">
@@ -4201,11 +4208,11 @@
       <c r="I109" s="4"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A110" s="17"/>
-      <c r="B110" s="22" t="s">
+      <c r="A110" s="18"/>
+      <c r="B110" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C110" s="19"/>
+      <c r="C110" s="20"/>
       <c r="D110" s="2" t="s">
         <v>269</v>
       </c>
@@ -4222,13 +4229,13 @@
       <c r="I110" s="4"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A111" s="17" t="s">
+      <c r="A111" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="B111" s="21" t="s">
+      <c r="B111" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="C111" s="19">
+      <c r="C111" s="20">
         <v>55</v>
       </c>
       <c r="D111" s="2" t="s">
@@ -4247,11 +4254,11 @@
       <c r="I111" s="4"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A112" s="17"/>
-      <c r="B112" s="22" t="s">
+      <c r="A112" s="18"/>
+      <c r="B112" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C112" s="19"/>
+      <c r="C112" s="20"/>
       <c r="D112" s="2" t="s">
         <v>274</v>
       </c>
@@ -4268,13 +4275,13 @@
       <c r="I112" s="4"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A113" s="17" t="s">
+      <c r="A113" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="B113" s="22" t="s">
+      <c r="B113" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="C113" s="19">
+      <c r="C113" s="20">
         <v>56</v>
       </c>
       <c r="D113" s="2" t="s">
@@ -4293,11 +4300,11 @@
       <c r="I113" s="4"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A114" s="17"/>
-      <c r="B114" s="22" t="s">
+      <c r="A114" s="18"/>
+      <c r="B114" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C114" s="19"/>
+      <c r="C114" s="20"/>
       <c r="D114" s="2" t="s">
         <v>280</v>
       </c>
@@ -4314,11 +4321,11 @@
       <c r="I114" s="4"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A115" s="17"/>
-      <c r="B115" s="22" t="s">
+      <c r="A115" s="18"/>
+      <c r="B115" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C115" s="19">
+      <c r="C115" s="20">
         <v>57</v>
       </c>
       <c r="D115" s="2" t="s">
@@ -4337,11 +4344,11 @@
       <c r="I115" s="4"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A116" s="17"/>
-      <c r="B116" s="22" t="s">
+      <c r="A116" s="18"/>
+      <c r="B116" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C116" s="19"/>
+      <c r="C116" s="20"/>
       <c r="D116" s="2" t="s">
         <v>284</v>
       </c>
@@ -4358,13 +4365,13 @@
       <c r="I116" s="4"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A117" s="17" t="s">
+      <c r="A117" s="18" t="s">
         <v>286</v>
       </c>
-      <c r="B117" s="22" t="s">
+      <c r="B117" s="19" t="s">
         <v>287</v>
       </c>
-      <c r="C117" s="19">
+      <c r="C117" s="20">
         <v>58</v>
       </c>
       <c r="D117" s="2" t="s">
@@ -4383,11 +4390,11 @@
       <c r="I117" s="4"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A118" s="17"/>
-      <c r="B118" s="22" t="s">
+      <c r="A118" s="18"/>
+      <c r="B118" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C118" s="19"/>
+      <c r="C118" s="20"/>
       <c r="D118" s="2" t="s">
         <v>290</v>
       </c>
@@ -4404,11 +4411,11 @@
       <c r="I118" s="4"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A119" s="17"/>
-      <c r="B119" s="22" t="s">
+      <c r="A119" s="18"/>
+      <c r="B119" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C119" s="19">
+      <c r="C119" s="20">
         <v>59</v>
       </c>
       <c r="D119" s="2" t="s">
@@ -4427,11 +4434,11 @@
       <c r="I119" s="4"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A120" s="17"/>
-      <c r="B120" s="22" t="s">
+      <c r="A120" s="18"/>
+      <c r="B120" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C120" s="19"/>
+      <c r="C120" s="20"/>
       <c r="D120" s="2" t="s">
         <v>292</v>
       </c>
@@ -4448,13 +4455,13 @@
       <c r="I120" s="4"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" s="17" t="s">
+      <c r="A121" s="18" t="s">
         <v>294</v>
       </c>
-      <c r="B121" s="22" t="s">
+      <c r="B121" s="19" t="s">
         <v>295</v>
       </c>
-      <c r="C121" s="19">
+      <c r="C121" s="20">
         <v>60</v>
       </c>
       <c r="D121" s="2" t="s">
@@ -4473,9 +4480,9 @@
       <c r="I121" s="4"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A122" s="17"/>
-      <c r="B122" s="22"/>
-      <c r="C122" s="19"/>
+      <c r="A122" s="18"/>
+      <c r="B122" s="19"/>
+      <c r="C122" s="20"/>
       <c r="D122" s="2" t="s">
         <v>298</v>
       </c>
@@ -4492,9 +4499,9 @@
       <c r="I122" s="4"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A123" s="17"/>
-      <c r="B123" s="22"/>
-      <c r="C123" s="19">
+      <c r="A123" s="18"/>
+      <c r="B123" s="19"/>
+      <c r="C123" s="20">
         <v>61</v>
       </c>
       <c r="D123" s="2" t="s">
@@ -4513,9 +4520,9 @@
       <c r="I123" s="4"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A124" s="17"/>
-      <c r="B124" s="22"/>
-      <c r="C124" s="19"/>
+      <c r="A124" s="18"/>
+      <c r="B124" s="19"/>
+      <c r="C124" s="20"/>
       <c r="D124" s="2" t="s">
         <v>310</v>
       </c>
@@ -4532,9 +4539,9 @@
       <c r="I124" s="4"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A125" s="17"/>
-      <c r="B125" s="22"/>
-      <c r="C125" s="19">
+      <c r="A125" s="18"/>
+      <c r="B125" s="19"/>
+      <c r="C125" s="20">
         <v>62</v>
       </c>
       <c r="D125" s="2" t="s">
@@ -4553,9 +4560,9 @@
       <c r="I125" s="4"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A126" s="17"/>
-      <c r="B126" s="22"/>
-      <c r="C126" s="19"/>
+      <c r="A126" s="18"/>
+      <c r="B126" s="19"/>
+      <c r="C126" s="20"/>
       <c r="D126" s="2" t="s">
         <v>314</v>
       </c>
@@ -4573,6 +4580,123 @@
     </row>
   </sheetData>
   <mergeCells count="141">
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="A71:A74"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="C83:C84"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="A83:A86"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="A91:A94"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="A99:A102"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A117:A120"/>
+    <mergeCell ref="B87:B90"/>
+    <mergeCell ref="B91:B94"/>
+    <mergeCell ref="B95:B98"/>
+    <mergeCell ref="B99:B102"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="B111:B112"/>
+    <mergeCell ref="B113:B116"/>
+    <mergeCell ref="B117:B120"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A113:A116"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="C101:C102"/>
+    <mergeCell ref="C103:C104"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="C93:C94"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
@@ -4597,123 +4721,6 @@
     <mergeCell ref="C111:C112"/>
     <mergeCell ref="C113:C114"/>
     <mergeCell ref="C95:C96"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="C103:C104"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="A117:A120"/>
-    <mergeCell ref="B87:B90"/>
-    <mergeCell ref="B91:B94"/>
-    <mergeCell ref="B95:B98"/>
-    <mergeCell ref="B99:B102"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="B109:B110"/>
-    <mergeCell ref="B111:B112"/>
-    <mergeCell ref="B113:B116"/>
-    <mergeCell ref="B117:B120"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A113:A116"/>
-    <mergeCell ref="A83:A86"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="A91:A94"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="A99:A102"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B71:B74"/>
-    <mergeCell ref="B75:B78"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="C83:C84"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A75:A78"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="A71:A74"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A51:A52"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G126" xr:uid="{BD7D4049-E182-46D9-ABFE-ED680993C7C2}">
@@ -4777,9 +4784,11 @@
     <hyperlink ref="F56" r:id="rId54" xr:uid="{75E007E6-8645-44B3-9C1C-804E5DF8CEAC}"/>
     <hyperlink ref="F57" r:id="rId55" xr:uid="{EEEFC227-AA75-4FA8-8770-51710CAEA2B9}"/>
     <hyperlink ref="F58" r:id="rId56" xr:uid="{4C0BA54A-6492-48D4-AC2F-7E75F504E59B}"/>
+    <hyperlink ref="F59" r:id="rId57" xr:uid="{7FF47B51-3E09-4769-9361-616326B362F0}"/>
+    <hyperlink ref="F60" r:id="rId58" xr:uid="{9CECBBD6-2F14-4F88-B6F4-C08AF3014E4F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId57"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId59"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
solve task '179. Largest Number'
</commit_message>
<xml_diff>
--- a/DSA studing (in acc. with Claude plan)/DSA_Leetcode_plan from Claude.xlsx
+++ b/DSA studing (in acc. with Claude plan)/DSA_Leetcode_plan from Claude.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Programming\Python\Leetcode\Leetcode practise\DSA studing (in acc. with Claude plan)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3ED5F9-1E6E-49C9-92D1-312FE4115DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C456D4-7C31-4AE9-B2F9-86D5AF2BF5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1223,7 +1223,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1268,20 +1268,32 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1297,21 +1309,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1602,8 +1599,8 @@
   <dimension ref="A1:L126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
+      <pane ySplit="2" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I79" sqref="I79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1619,31 +1616,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="16" t="s">
+      <c r="B1" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="23" t="s">
         <v>316</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="23" t="s">
         <v>317</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="23" t="s">
         <v>318</v>
       </c>
       <c r="J1" s="9" t="s">
@@ -1657,36 +1654,36 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
       <c r="J2" s="10">
         <f>COUNTIF(G3:G126,"решена")/124</f>
-        <v>0.44354838709677419</v>
+        <v>0.45161290322580644</v>
       </c>
       <c r="K2" s="11">
         <f>SUM(H3:H126)/(COUNTIF(G3:G126,"решена") + COUNTIF(G3:G126,"не решена"))</f>
-        <v>2.2456140350877192</v>
+        <v>2.3103448275862069</v>
       </c>
       <c r="L2" s="10">
         <f>SUM(I3:I126)/SUM(H3:H126)</f>
-        <v>0.7265625</v>
+        <v>0.73134328358208955</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="18">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -1712,9 +1709,9 @@
       <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="29"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="6" t="s">
         <v>11</v>
       </c>
@@ -1735,9 +1732,9 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="28"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="29">
+      <c r="A5" s="16"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="18">
         <v>2</v>
       </c>
       <c r="D5" s="6" t="s">
@@ -1760,9 +1757,9 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="28"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="29"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="18"/>
       <c r="D6" s="6" t="s">
         <v>15</v>
       </c>
@@ -1783,13 +1780,13 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="20" t="s">
         <v>324</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="18">
         <v>3</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -1812,9 +1809,9 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="29"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="18"/>
       <c r="D8" s="6" t="s">
         <v>20</v>
       </c>
@@ -1835,9 +1832,9 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="29">
+      <c r="A9" s="16"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="18">
         <v>4</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -1860,9 +1857,9 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="28"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="29"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="6" t="s">
         <v>24</v>
       </c>
@@ -1883,13 +1880,13 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="18">
         <v>5</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -1912,9 +1909,9 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="28"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="29"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="18"/>
       <c r="D12" s="6" t="s">
         <v>29</v>
       </c>
@@ -1935,9 +1932,9 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="28"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="29">
+      <c r="A13" s="16"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="18">
         <v>6</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -1960,9 +1957,9 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="28"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="29"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="6" t="s">
         <v>33</v>
       </c>
@@ -1983,13 +1980,13 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="C15" s="29">
+      <c r="C15" s="18">
         <v>7</v>
       </c>
       <c r="D15" s="6" t="s">
@@ -2012,9 +2009,9 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="18"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="29"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="6" t="s">
         <v>38</v>
       </c>
@@ -2035,9 +2032,9 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="29">
+      <c r="A17" s="17"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="18">
         <v>8</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -2060,9 +2057,9 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="29"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="18"/>
       <c r="D18" s="6" t="s">
         <v>42</v>
       </c>
@@ -2083,13 +2080,13 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="C19" s="29">
+      <c r="C19" s="18">
         <v>9</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -2112,9 +2109,9 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="29"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="18"/>
       <c r="D20" s="6" t="s">
         <v>47</v>
       </c>
@@ -2135,9 +2132,9 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="18"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="20">
+      <c r="A21" s="17"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="19">
         <v>10</v>
       </c>
       <c r="D21" s="6" t="s">
@@ -2160,9 +2157,9 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="20"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="19"/>
       <c r="D22" s="13" t="s">
         <v>51</v>
       </c>
@@ -2183,13 +2180,13 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="C23" s="29">
+      <c r="C23" s="18">
         <v>11</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -2212,9 +2209,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="18"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="29"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="18"/>
       <c r="D24" s="6" t="s">
         <v>56</v>
       </c>
@@ -2235,9 +2232,9 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="29">
+      <c r="A25" s="17"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="18">
         <v>12</v>
       </c>
       <c r="D25" s="6" t="s">
@@ -2260,9 +2257,9 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="18"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="29"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="18"/>
       <c r="D26" s="6" t="s">
         <v>60</v>
       </c>
@@ -2283,13 +2280,13 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="28" t="s">
+      <c r="A27" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="C27" s="29">
+      <c r="C27" s="18">
         <v>13</v>
       </c>
       <c r="D27" s="6" t="s">
@@ -2312,9 +2309,9 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="28"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="29"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="18"/>
       <c r="D28" s="6" t="s">
         <v>65</v>
       </c>
@@ -2335,9 +2332,9 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="28"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="29">
+      <c r="A29" s="16"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="18">
         <v>14</v>
       </c>
       <c r="D29" s="6" t="s">
@@ -2360,9 +2357,9 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="28"/>
-      <c r="B30" s="27"/>
-      <c r="C30" s="29"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="18"/>
       <c r="D30" s="6" t="s">
         <v>69</v>
       </c>
@@ -2383,13 +2380,13 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="28" t="s">
+      <c r="A31" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="27" t="s">
+      <c r="B31" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="C31" s="29">
+      <c r="C31" s="18">
         <v>15</v>
       </c>
       <c r="D31" s="6" t="s">
@@ -2412,9 +2409,9 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="28"/>
-      <c r="B32" s="27"/>
-      <c r="C32" s="29"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="18"/>
       <c r="D32" s="6" t="s">
         <v>74</v>
       </c>
@@ -2435,9 +2432,9 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="28"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="29">
+      <c r="A33" s="16"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="18">
         <v>16</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -2460,9 +2457,9 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="28"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="29"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="18"/>
       <c r="D34" s="6" t="s">
         <v>78</v>
       </c>
@@ -2483,13 +2480,13 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="28" t="s">
+      <c r="A35" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="C35" s="29">
+      <c r="C35" s="18">
         <v>17</v>
       </c>
       <c r="D35" s="6" t="s">
@@ -2512,9 +2509,9 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="28"/>
-      <c r="B36" s="27"/>
-      <c r="C36" s="29"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="18"/>
       <c r="D36" s="6" t="s">
         <v>83</v>
       </c>
@@ -2535,13 +2532,13 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="28" t="s">
+      <c r="A37" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="27" t="s">
+      <c r="B37" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="C37" s="29">
+      <c r="C37" s="18">
         <v>18</v>
       </c>
       <c r="D37" s="6" t="s">
@@ -2564,9 +2561,9 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="28"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="29"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="18"/>
       <c r="D38" s="6" t="s">
         <v>88</v>
       </c>
@@ -2587,9 +2584,9 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="28"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="29">
+      <c r="A39" s="16"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="18">
         <v>19</v>
       </c>
       <c r="D39" s="6" t="s">
@@ -2612,9 +2609,9 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="28"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="29"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="18"/>
       <c r="D40" s="6" t="s">
         <v>92</v>
       </c>
@@ -2635,13 +2632,13 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="28" t="s">
+      <c r="A41" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B41" s="27" t="s">
+      <c r="B41" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="C41" s="29">
+      <c r="C41" s="18">
         <v>20</v>
       </c>
       <c r="D41" s="6" t="s">
@@ -2664,9 +2661,9 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="28"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="29"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="18"/>
       <c r="D42" s="6" t="s">
         <v>97</v>
       </c>
@@ -2687,9 +2684,9 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="28"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="29">
+      <c r="A43" s="16"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="18">
         <v>21</v>
       </c>
       <c r="D43" s="6" t="s">
@@ -2712,9 +2709,9 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="28"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="29"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="18"/>
       <c r="D44" s="6" t="s">
         <v>101</v>
       </c>
@@ -2735,13 +2732,13 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="28" t="s">
+      <c r="A45" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="B45" s="27" t="s">
+      <c r="B45" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="C45" s="29">
+      <c r="C45" s="18">
         <v>22</v>
       </c>
       <c r="D45" s="6" t="s">
@@ -2764,9 +2761,9 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="28"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="29"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="18"/>
       <c r="D46" s="6" t="s">
         <v>106</v>
       </c>
@@ -2787,13 +2784,13 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="28" t="s">
+      <c r="A47" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B47" s="27" t="s">
+      <c r="B47" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="C47" s="29">
+      <c r="C47" s="18">
         <v>23</v>
       </c>
       <c r="D47" s="6" t="s">
@@ -2816,9 +2813,9 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="28"/>
-      <c r="B48" s="27"/>
-      <c r="C48" s="29"/>
+      <c r="A48" s="16"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="18"/>
       <c r="D48" s="6" t="s">
         <v>111</v>
       </c>
@@ -2839,9 +2836,9 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="28"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="29">
+      <c r="A49" s="16"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="18">
         <v>24</v>
       </c>
       <c r="D49" s="6" t="s">
@@ -2864,9 +2861,9 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="28"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="29"/>
+      <c r="A50" s="16"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="18"/>
       <c r="D50" s="6" t="s">
         <v>115</v>
       </c>
@@ -2887,13 +2884,13 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="28" t="s">
+      <c r="A51" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B51" s="27" t="s">
+      <c r="B51" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="C51" s="29">
+      <c r="C51" s="18">
         <v>25</v>
       </c>
       <c r="D51" s="6" t="s">
@@ -2916,9 +2913,9 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="28"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="29"/>
+      <c r="A52" s="16"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="18"/>
       <c r="D52" s="6" t="s">
         <v>120</v>
       </c>
@@ -2939,13 +2936,13 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="28" t="s">
+      <c r="A53" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B53" s="27" t="s">
+      <c r="B53" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="C53" s="29">
+      <c r="C53" s="18">
         <v>26</v>
       </c>
       <c r="D53" s="6" t="s">
@@ -2968,9 +2965,9 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="28"/>
-      <c r="B54" s="27"/>
-      <c r="C54" s="29"/>
+      <c r="A54" s="16"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="18"/>
       <c r="D54" s="6" t="s">
         <v>125</v>
       </c>
@@ -2991,9 +2988,9 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="28"/>
-      <c r="B55" s="27"/>
-      <c r="C55" s="20">
+      <c r="A55" s="16"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="19">
         <v>27</v>
       </c>
       <c r="D55" s="6" t="s">
@@ -3016,9 +3013,9 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="28"/>
-      <c r="B56" s="27"/>
-      <c r="C56" s="20"/>
+      <c r="A56" s="16"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="19"/>
       <c r="D56" s="13" t="s">
         <v>129</v>
       </c>
@@ -3039,13 +3036,13 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="28" t="s">
+      <c r="A57" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="B57" s="27" t="s">
+      <c r="B57" s="20" t="s">
         <v>209</v>
       </c>
-      <c r="C57" s="29">
+      <c r="C57" s="18">
         <v>28</v>
       </c>
       <c r="D57" s="6" t="s">
@@ -3068,9 +3065,9 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="28"/>
-      <c r="B58" s="27"/>
-      <c r="C58" s="29"/>
+      <c r="A58" s="16"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="18"/>
       <c r="D58" s="6" t="s">
         <v>134</v>
       </c>
@@ -3091,9 +3088,9 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="28"/>
-      <c r="B59" s="27"/>
-      <c r="C59" s="20">
+      <c r="A59" s="16"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="18">
         <v>29</v>
       </c>
       <c r="D59" s="6" t="s">
@@ -3116,32 +3113,36 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="28"/>
-      <c r="B60" s="27"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="1" t="s">
+      <c r="A60" s="16"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F60" s="30" t="s">
+      <c r="E60" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F60" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="G60" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4"/>
+      <c r="G60" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="H60" s="5">
+        <v>6</v>
+      </c>
+      <c r="I60" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="18" t="s">
+      <c r="A61" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="B61" s="26" t="s">
+      <c r="B61" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="C61" s="20">
+      <c r="C61" s="19">
         <v>30</v>
       </c>
       <c r="D61" s="1" t="s">
@@ -3160,9 +3161,9 @@
       <c r="I61" s="4"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="18"/>
-      <c r="B62" s="26"/>
-      <c r="C62" s="20"/>
+      <c r="A62" s="17"/>
+      <c r="B62" s="21"/>
+      <c r="C62" s="19"/>
       <c r="D62" s="1" t="s">
         <v>143</v>
       </c>
@@ -3179,9 +3180,9 @@
       <c r="I62" s="4"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="18"/>
-      <c r="B63" s="26"/>
-      <c r="C63" s="20">
+      <c r="A63" s="17"/>
+      <c r="B63" s="21"/>
+      <c r="C63" s="19">
         <v>31</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -3200,9 +3201,9 @@
       <c r="I63" s="4"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="18"/>
-      <c r="B64" s="26"/>
-      <c r="C64" s="20"/>
+      <c r="A64" s="17"/>
+      <c r="B64" s="21"/>
+      <c r="C64" s="19"/>
       <c r="D64" s="1" t="s">
         <v>147</v>
       </c>
@@ -3219,13 +3220,13 @@
       <c r="I64" s="4"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="18" t="s">
+      <c r="A65" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="B65" s="26" t="s">
+      <c r="B65" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="C65" s="20">
+      <c r="C65" s="19">
         <v>32</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -3244,9 +3245,9 @@
       <c r="I65" s="4"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="18"/>
-      <c r="B66" s="26"/>
-      <c r="C66" s="20"/>
+      <c r="A66" s="17"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="19"/>
       <c r="D66" s="1" t="s">
         <v>152</v>
       </c>
@@ -3263,9 +3264,9 @@
       <c r="I66" s="4"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="18"/>
-      <c r="B67" s="26"/>
-      <c r="C67" s="20">
+      <c r="A67" s="17"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="19">
         <v>33</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -3284,9 +3285,9 @@
       <c r="I67" s="4"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="18"/>
-      <c r="B68" s="26"/>
-      <c r="C68" s="20"/>
+      <c r="A68" s="17"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="19"/>
       <c r="D68" s="1" t="s">
         <v>156</v>
       </c>
@@ -3303,13 +3304,13 @@
       <c r="I68" s="4"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="18" t="s">
+      <c r="A69" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="B69" s="26" t="s">
+      <c r="B69" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="C69" s="20">
+      <c r="C69" s="19">
         <v>34</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -3328,9 +3329,9 @@
       <c r="I69" s="4"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="18"/>
-      <c r="B70" s="26"/>
-      <c r="C70" s="20"/>
+      <c r="A70" s="17"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="19"/>
       <c r="D70" s="1" t="s">
         <v>161</v>
       </c>
@@ -3347,13 +3348,13 @@
       <c r="I70" s="4"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="18" t="s">
+      <c r="A71" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="B71" s="26" t="s">
+      <c r="B71" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="C71" s="20">
+      <c r="C71" s="19">
         <v>35</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -3372,9 +3373,9 @@
       <c r="I71" s="4"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="18"/>
-      <c r="B72" s="26"/>
-      <c r="C72" s="20"/>
+      <c r="A72" s="17"/>
+      <c r="B72" s="21"/>
+      <c r="C72" s="19"/>
       <c r="D72" s="1" t="s">
         <v>166</v>
       </c>
@@ -3391,9 +3392,9 @@
       <c r="I72" s="4"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="18"/>
-      <c r="B73" s="26"/>
-      <c r="C73" s="20">
+      <c r="A73" s="17"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="19">
         <v>36</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -3412,9 +3413,9 @@
       <c r="I73" s="4"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="18"/>
-      <c r="B74" s="26"/>
-      <c r="C74" s="20"/>
+      <c r="A74" s="17"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="19"/>
       <c r="D74" s="1" t="s">
         <v>170</v>
       </c>
@@ -3431,13 +3432,13 @@
       <c r="I74" s="4"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="18" t="s">
+      <c r="A75" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="B75" s="26" t="s">
+      <c r="B75" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="C75" s="20">
+      <c r="C75" s="19">
         <v>37</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -3456,9 +3457,9 @@
       <c r="I75" s="4"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="18"/>
-      <c r="B76" s="26"/>
-      <c r="C76" s="20"/>
+      <c r="A76" s="17"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="19"/>
       <c r="D76" s="1" t="s">
         <v>175</v>
       </c>
@@ -3475,9 +3476,9 @@
       <c r="I76" s="4"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="18"/>
-      <c r="B77" s="26"/>
-      <c r="C77" s="20">
+      <c r="A77" s="17"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="19">
         <v>38</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -3496,9 +3497,9 @@
       <c r="I77" s="4"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="18"/>
-      <c r="B78" s="26"/>
-      <c r="C78" s="20"/>
+      <c r="A78" s="17"/>
+      <c r="B78" s="21"/>
+      <c r="C78" s="19"/>
       <c r="D78" s="1" t="s">
         <v>179</v>
       </c>
@@ -3515,13 +3516,13 @@
       <c r="I78" s="4"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="18" t="s">
+      <c r="A79" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="B79" s="26" t="s">
+      <c r="B79" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="C79" s="20">
+      <c r="C79" s="19">
         <v>39</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -3540,9 +3541,9 @@
       <c r="I79" s="4"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="18"/>
-      <c r="B80" s="26"/>
-      <c r="C80" s="20"/>
+      <c r="A80" s="17"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="19"/>
       <c r="D80" s="1" t="s">
         <v>184</v>
       </c>
@@ -3559,13 +3560,13 @@
       <c r="I80" s="4"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="18" t="s">
+      <c r="A81" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="B81" s="26" t="s">
+      <c r="B81" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="C81" s="20">
+      <c r="C81" s="19">
         <v>40</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -3584,9 +3585,9 @@
       <c r="I81" s="4"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="18"/>
-      <c r="B82" s="26"/>
-      <c r="C82" s="20"/>
+      <c r="A82" s="17"/>
+      <c r="B82" s="21"/>
+      <c r="C82" s="19"/>
       <c r="D82" s="1" t="s">
         <v>189</v>
       </c>
@@ -3603,13 +3604,13 @@
       <c r="I82" s="4"/>
     </row>
     <row r="83" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="18" t="s">
+      <c r="A83" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="B83" s="23" t="s">
+      <c r="B83" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="C83" s="20">
+      <c r="C83" s="19">
         <v>41</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -3628,9 +3629,9 @@
       <c r="I83" s="4"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="18"/>
-      <c r="B84" s="24"/>
-      <c r="C84" s="20"/>
+      <c r="A84" s="17"/>
+      <c r="B84" s="28"/>
+      <c r="C84" s="19"/>
       <c r="D84" s="1" t="s">
         <v>194</v>
       </c>
@@ -3647,9 +3648,9 @@
       <c r="I84" s="4"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="18"/>
-      <c r="B85" s="24"/>
-      <c r="C85" s="20">
+      <c r="A85" s="17"/>
+      <c r="B85" s="28"/>
+      <c r="C85" s="19">
         <v>42</v>
       </c>
       <c r="D85" s="2" t="s">
@@ -3668,9 +3669,9 @@
       <c r="I85" s="4"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="18"/>
-      <c r="B86" s="25"/>
-      <c r="C86" s="20"/>
+      <c r="A86" s="17"/>
+      <c r="B86" s="29"/>
+      <c r="C86" s="19"/>
       <c r="D86" s="2" t="s">
         <v>221</v>
       </c>
@@ -3687,13 +3688,13 @@
       <c r="I86" s="4"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="18" t="s">
+      <c r="A87" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="B87" s="26" t="s">
+      <c r="B87" s="21" t="s">
         <v>301</v>
       </c>
-      <c r="C87" s="20">
+      <c r="C87" s="19">
         <v>43</v>
       </c>
       <c r="D87" s="2" t="s">
@@ -3712,11 +3713,11 @@
       <c r="I87" s="4"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="18"/>
-      <c r="B88" s="19" t="s">
+      <c r="A88" s="17"/>
+      <c r="B88" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C88" s="20"/>
+      <c r="C88" s="19"/>
       <c r="D88" s="2" t="s">
         <v>226</v>
       </c>
@@ -3733,11 +3734,11 @@
       <c r="I88" s="4"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" s="18"/>
-      <c r="B89" s="19" t="s">
+      <c r="A89" s="17"/>
+      <c r="B89" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C89" s="20">
+      <c r="C89" s="19">
         <v>44</v>
       </c>
       <c r="D89" s="2" t="s">
@@ -3756,11 +3757,11 @@
       <c r="I89" s="4"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90" s="18"/>
-      <c r="B90" s="19" t="s">
+      <c r="A90" s="17"/>
+      <c r="B90" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C90" s="20"/>
+      <c r="C90" s="19"/>
       <c r="D90" s="2" t="s">
         <v>230</v>
       </c>
@@ -3777,13 +3778,13 @@
       <c r="I90" s="4"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91" s="18" t="s">
+      <c r="A91" s="17" t="s">
         <v>232</v>
       </c>
-      <c r="B91" s="26" t="s">
+      <c r="B91" s="21" t="s">
         <v>302</v>
       </c>
-      <c r="C91" s="20">
+      <c r="C91" s="19">
         <v>45</v>
       </c>
       <c r="D91" s="2" t="s">
@@ -3802,11 +3803,11 @@
       <c r="I91" s="4"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A92" s="18"/>
-      <c r="B92" s="19" t="s">
+      <c r="A92" s="17"/>
+      <c r="B92" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C92" s="20"/>
+      <c r="C92" s="19"/>
       <c r="D92" s="2" t="s">
         <v>235</v>
       </c>
@@ -3823,11 +3824,11 @@
       <c r="I92" s="4"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" s="18"/>
-      <c r="B93" s="19" t="s">
+      <c r="A93" s="17"/>
+      <c r="B93" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C93" s="20">
+      <c r="C93" s="19">
         <v>46</v>
       </c>
       <c r="D93" s="2" t="s">
@@ -3846,11 +3847,11 @@
       <c r="I93" s="4"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94" s="18"/>
-      <c r="B94" s="19" t="s">
+      <c r="A94" s="17"/>
+      <c r="B94" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C94" s="20"/>
+      <c r="C94" s="19"/>
       <c r="D94" s="2" t="s">
         <v>239</v>
       </c>
@@ -3867,13 +3868,13 @@
       <c r="I94" s="4"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95" s="18" t="s">
+      <c r="A95" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="B95" s="26" t="s">
+      <c r="B95" s="21" t="s">
         <v>303</v>
       </c>
-      <c r="C95" s="20">
+      <c r="C95" s="19">
         <v>47</v>
       </c>
       <c r="D95" s="2" t="s">
@@ -3892,11 +3893,11 @@
       <c r="I95" s="4"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A96" s="18"/>
-      <c r="B96" s="19" t="s">
+      <c r="A96" s="17"/>
+      <c r="B96" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C96" s="20"/>
+      <c r="C96" s="19"/>
       <c r="D96" s="2" t="s">
         <v>244</v>
       </c>
@@ -3913,11 +3914,11 @@
       <c r="I96" s="4"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97" s="18"/>
-      <c r="B97" s="19" t="s">
+      <c r="A97" s="17"/>
+      <c r="B97" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C97" s="20">
+      <c r="C97" s="19">
         <v>48</v>
       </c>
       <c r="D97" s="2" t="s">
@@ -3936,11 +3937,11 @@
       <c r="I97" s="4"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98" s="18"/>
-      <c r="B98" s="19" t="s">
+      <c r="A98" s="17"/>
+      <c r="B98" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C98" s="20"/>
+      <c r="C98" s="19"/>
       <c r="D98" s="2" t="s">
         <v>248</v>
       </c>
@@ -3957,13 +3958,13 @@
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" s="18" t="s">
+      <c r="A99" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="B99" s="26" t="s">
+      <c r="B99" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="C99" s="20">
+      <c r="C99" s="19">
         <v>49</v>
       </c>
       <c r="D99" s="2" t="s">
@@ -3982,11 +3983,11 @@
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" s="18"/>
-      <c r="B100" s="19" t="s">
+      <c r="A100" s="17"/>
+      <c r="B100" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C100" s="20"/>
+      <c r="C100" s="19"/>
       <c r="D100" s="2" t="s">
         <v>253</v>
       </c>
@@ -4003,11 +4004,11 @@
       <c r="I100" s="4"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101" s="18"/>
-      <c r="B101" s="19" t="s">
+      <c r="A101" s="17"/>
+      <c r="B101" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C101" s="20">
+      <c r="C101" s="19">
         <v>50</v>
       </c>
       <c r="D101" s="2" t="s">
@@ -4026,11 +4027,11 @@
       <c r="I101" s="4"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A102" s="18"/>
-      <c r="B102" s="19" t="s">
+      <c r="A102" s="17"/>
+      <c r="B102" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C102" s="20"/>
+      <c r="C102" s="19"/>
       <c r="D102" s="2" t="s">
         <v>257</v>
       </c>
@@ -4047,13 +4048,13 @@
       <c r="I102" s="4"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A103" s="18" t="s">
+      <c r="A103" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="B103" s="26" t="s">
+      <c r="B103" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="C103" s="20">
+      <c r="C103" s="19">
         <v>51</v>
       </c>
       <c r="D103" s="2" t="s">
@@ -4072,11 +4073,11 @@
       <c r="I103" s="4"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" s="18"/>
-      <c r="B104" s="19" t="s">
+      <c r="A104" s="17"/>
+      <c r="B104" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C104" s="20"/>
+      <c r="C104" s="19"/>
       <c r="D104" s="2" t="s">
         <v>60</v>
       </c>
@@ -4093,13 +4094,13 @@
       <c r="I104" s="4"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A105" s="18" t="s">
+      <c r="A105" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="B105" s="19" t="s">
+      <c r="B105" s="22" t="s">
         <v>263</v>
       </c>
-      <c r="C105" s="20">
+      <c r="C105" s="19">
         <v>52</v>
       </c>
       <c r="D105" s="2" t="s">
@@ -4118,11 +4119,11 @@
       <c r="I105" s="4"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A106" s="18"/>
-      <c r="B106" s="19" t="s">
+      <c r="A106" s="17"/>
+      <c r="B106" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C106" s="20"/>
+      <c r="C106" s="19"/>
       <c r="D106" s="2" t="s">
         <v>24</v>
       </c>
@@ -4139,11 +4140,11 @@
       <c r="I106" s="4"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A107" s="18"/>
-      <c r="B107" s="19" t="s">
+      <c r="A107" s="17"/>
+      <c r="B107" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C107" s="20">
+      <c r="C107" s="19">
         <v>53</v>
       </c>
       <c r="D107" s="2" t="s">
@@ -4162,11 +4163,11 @@
       <c r="I107" s="4"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A108" s="18"/>
-      <c r="B108" s="19" t="s">
+      <c r="A108" s="17"/>
+      <c r="B108" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C108" s="20"/>
+      <c r="C108" s="19"/>
       <c r="D108" s="2" t="s">
         <v>136</v>
       </c>
@@ -4183,13 +4184,13 @@
       <c r="I108" s="4"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" s="18" t="s">
+      <c r="A109" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="B109" s="26" t="s">
+      <c r="B109" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="C109" s="20">
+      <c r="C109" s="19">
         <v>54</v>
       </c>
       <c r="D109" s="2" t="s">
@@ -4208,11 +4209,11 @@
       <c r="I109" s="4"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A110" s="18"/>
-      <c r="B110" s="19" t="s">
+      <c r="A110" s="17"/>
+      <c r="B110" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C110" s="20"/>
+      <c r="C110" s="19"/>
       <c r="D110" s="2" t="s">
         <v>269</v>
       </c>
@@ -4229,13 +4230,13 @@
       <c r="I110" s="4"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A111" s="18" t="s">
+      <c r="A111" s="17" t="s">
         <v>271</v>
       </c>
-      <c r="B111" s="26" t="s">
+      <c r="B111" s="21" t="s">
         <v>307</v>
       </c>
-      <c r="C111" s="20">
+      <c r="C111" s="19">
         <v>55</v>
       </c>
       <c r="D111" s="2" t="s">
@@ -4254,11 +4255,11 @@
       <c r="I111" s="4"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A112" s="18"/>
-      <c r="B112" s="19" t="s">
+      <c r="A112" s="17"/>
+      <c r="B112" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C112" s="20"/>
+      <c r="C112" s="19"/>
       <c r="D112" s="2" t="s">
         <v>274</v>
       </c>
@@ -4275,13 +4276,13 @@
       <c r="I112" s="4"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A113" s="18" t="s">
+      <c r="A113" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="B113" s="19" t="s">
+      <c r="B113" s="22" t="s">
         <v>277</v>
       </c>
-      <c r="C113" s="20">
+      <c r="C113" s="19">
         <v>56</v>
       </c>
       <c r="D113" s="2" t="s">
@@ -4300,11 +4301,11 @@
       <c r="I113" s="4"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A114" s="18"/>
-      <c r="B114" s="19" t="s">
+      <c r="A114" s="17"/>
+      <c r="B114" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C114" s="20"/>
+      <c r="C114" s="19"/>
       <c r="D114" s="2" t="s">
         <v>280</v>
       </c>
@@ -4321,11 +4322,11 @@
       <c r="I114" s="4"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A115" s="18"/>
-      <c r="B115" s="19" t="s">
+      <c r="A115" s="17"/>
+      <c r="B115" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C115" s="20">
+      <c r="C115" s="19">
         <v>57</v>
       </c>
       <c r="D115" s="2" t="s">
@@ -4344,11 +4345,11 @@
       <c r="I115" s="4"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A116" s="18"/>
-      <c r="B116" s="19" t="s">
+      <c r="A116" s="17"/>
+      <c r="B116" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C116" s="20"/>
+      <c r="C116" s="19"/>
       <c r="D116" s="2" t="s">
         <v>284</v>
       </c>
@@ -4365,13 +4366,13 @@
       <c r="I116" s="4"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A117" s="18" t="s">
+      <c r="A117" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="B117" s="19" t="s">
+      <c r="B117" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="C117" s="20">
+      <c r="C117" s="19">
         <v>58</v>
       </c>
       <c r="D117" s="2" t="s">
@@ -4390,11 +4391,11 @@
       <c r="I117" s="4"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A118" s="18"/>
-      <c r="B118" s="19" t="s">
+      <c r="A118" s="17"/>
+      <c r="B118" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C118" s="20"/>
+      <c r="C118" s="19"/>
       <c r="D118" s="2" t="s">
         <v>290</v>
       </c>
@@ -4411,11 +4412,11 @@
       <c r="I118" s="4"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A119" s="18"/>
-      <c r="B119" s="19" t="s">
+      <c r="A119" s="17"/>
+      <c r="B119" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C119" s="20">
+      <c r="C119" s="19">
         <v>59</v>
       </c>
       <c r="D119" s="2" t="s">
@@ -4434,11 +4435,11 @@
       <c r="I119" s="4"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A120" s="18"/>
-      <c r="B120" s="19" t="s">
+      <c r="A120" s="17"/>
+      <c r="B120" s="22" t="s">
         <v>220</v>
       </c>
-      <c r="C120" s="20"/>
+      <c r="C120" s="19"/>
       <c r="D120" s="2" t="s">
         <v>292</v>
       </c>
@@ -4455,13 +4456,13 @@
       <c r="I120" s="4"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" s="18" t="s">
+      <c r="A121" s="17" t="s">
         <v>294</v>
       </c>
-      <c r="B121" s="19" t="s">
+      <c r="B121" s="22" t="s">
         <v>295</v>
       </c>
-      <c r="C121" s="20">
+      <c r="C121" s="19">
         <v>60</v>
       </c>
       <c r="D121" s="2" t="s">
@@ -4480,9 +4481,9 @@
       <c r="I121" s="4"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A122" s="18"/>
-      <c r="B122" s="19"/>
-      <c r="C122" s="20"/>
+      <c r="A122" s="17"/>
+      <c r="B122" s="22"/>
+      <c r="C122" s="19"/>
       <c r="D122" s="2" t="s">
         <v>298</v>
       </c>
@@ -4499,9 +4500,9 @@
       <c r="I122" s="4"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A123" s="18"/>
-      <c r="B123" s="19"/>
-      <c r="C123" s="20">
+      <c r="A123" s="17"/>
+      <c r="B123" s="22"/>
+      <c r="C123" s="19">
         <v>61</v>
       </c>
       <c r="D123" s="2" t="s">
@@ -4520,9 +4521,9 @@
       <c r="I123" s="4"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A124" s="18"/>
-      <c r="B124" s="19"/>
-      <c r="C124" s="20"/>
+      <c r="A124" s="17"/>
+      <c r="B124" s="22"/>
+      <c r="C124" s="19"/>
       <c r="D124" s="2" t="s">
         <v>310</v>
       </c>
@@ -4539,9 +4540,9 @@
       <c r="I124" s="4"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A125" s="18"/>
-      <c r="B125" s="19"/>
-      <c r="C125" s="20">
+      <c r="A125" s="17"/>
+      <c r="B125" s="22"/>
+      <c r="C125" s="19">
         <v>62</v>
       </c>
       <c r="D125" s="2" t="s">
@@ -4560,9 +4561,9 @@
       <c r="I125" s="4"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A126" s="18"/>
-      <c r="B126" s="19"/>
-      <c r="C126" s="20"/>
+      <c r="A126" s="17"/>
+      <c r="B126" s="22"/>
+      <c r="C126" s="19"/>
       <c r="D126" s="2" t="s">
         <v>314</v>
       </c>
@@ -4580,15 +4581,114 @@
     </row>
   </sheetData>
   <mergeCells count="141">
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A121:A126"/>
+    <mergeCell ref="B121:B126"/>
+    <mergeCell ref="C121:C122"/>
+    <mergeCell ref="C123:C124"/>
+    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C115:C116"/>
+    <mergeCell ref="C117:C118"/>
+    <mergeCell ref="C119:C120"/>
+    <mergeCell ref="B83:B86"/>
+    <mergeCell ref="C105:C106"/>
+    <mergeCell ref="C107:C108"/>
+    <mergeCell ref="C109:C110"/>
+    <mergeCell ref="C111:C112"/>
+    <mergeCell ref="C113:C114"/>
+    <mergeCell ref="C95:C96"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="C101:C102"/>
+    <mergeCell ref="C103:C104"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="C93:C94"/>
+    <mergeCell ref="A117:A120"/>
+    <mergeCell ref="B87:B90"/>
+    <mergeCell ref="B91:B94"/>
+    <mergeCell ref="B95:B98"/>
+    <mergeCell ref="B99:B102"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="B111:B112"/>
+    <mergeCell ref="B113:B116"/>
+    <mergeCell ref="B117:B120"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A113:A116"/>
+    <mergeCell ref="A83:A86"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="A91:A94"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="A99:A102"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="C83:C84"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C47:C48"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C19:C20"/>
@@ -4613,114 +4713,15 @@
     <mergeCell ref="A71:A74"/>
     <mergeCell ref="A61:A64"/>
     <mergeCell ref="A65:A68"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="C83:C84"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A83:A86"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="A91:A94"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="A99:A102"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B71:B74"/>
-    <mergeCell ref="B75:B78"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A117:A120"/>
-    <mergeCell ref="B87:B90"/>
-    <mergeCell ref="B91:B94"/>
-    <mergeCell ref="B95:B98"/>
-    <mergeCell ref="B99:B102"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="B109:B110"/>
-    <mergeCell ref="B111:B112"/>
-    <mergeCell ref="B113:B116"/>
-    <mergeCell ref="B117:B120"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A113:A116"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="C103:C104"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="A121:A126"/>
-    <mergeCell ref="B121:B126"/>
-    <mergeCell ref="C121:C122"/>
-    <mergeCell ref="C123:C124"/>
-    <mergeCell ref="C125:C126"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C115:C116"/>
-    <mergeCell ref="C117:C118"/>
-    <mergeCell ref="C119:C120"/>
-    <mergeCell ref="B83:B86"/>
-    <mergeCell ref="C105:C106"/>
-    <mergeCell ref="C107:C108"/>
-    <mergeCell ref="C109:C110"/>
-    <mergeCell ref="C111:C112"/>
-    <mergeCell ref="C113:C114"/>
-    <mergeCell ref="C95:C96"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A51:A52"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G126" xr:uid="{BD7D4049-E182-46D9-ABFE-ED680993C7C2}">

</xml_diff>

<commit_message>
solve taks '704. Binary Search'
</commit_message>
<xml_diff>
--- a/DSA studing (in acc. with Claude plan)/DSA_Leetcode_plan from Claude.xlsx
+++ b/DSA studing (in acc. with Claude plan)/DSA_Leetcode_plan from Claude.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Programming\Python\Leetcode\Leetcode practise\DSA studing (in acc. with Claude plan)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C456D4-7C31-4AE9-B2F9-86D5AF2BF5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D685F28E-929E-49F2-A4AD-29470FB34C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,6 +31,9 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -707,11 +710,6 @@
 https://www.geeksforgeeks.org/python-list-sort-method-and-sorted-function/</t>
   </si>
   <si>
-    <t>https://realpython.com/binary-search-python/
-https://www.geeksforgeeks.org/binary-search-in-python/
-https://www.programiz.com/dsa/binary-search</t>
-  </si>
-  <si>
     <t>https://realpython.com/python-thinking-recursively/
 https://www.geeksforgeeks.org/dynamic-programming/
 https://www.programiz.com/dsa/dynamic-programming</t>
@@ -1088,6 +1086,11 @@
   </si>
   <si>
     <t>не решена</t>
+  </si>
+  <si>
+    <t>https://realpython.com/binary-search-python/
+https://www.geeksforgeeks.org/python/python-program-for-binary-search/
+https://www.programiz.com/dsa/binary-search</t>
   </si>
 </sst>
 </file>
@@ -1223,7 +1226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1268,38 +1271,20 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1309,6 +1294,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1599,8 +1596,8 @@
   <dimension ref="A1:L126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I79" sqref="I79"/>
+      <pane ySplit="2" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B53" sqref="B53:B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1616,74 +1613,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="23" t="s">
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="16" t="s">
+        <v>315</v>
+      </c>
+      <c r="H1" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="I1" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="I1" s="23" t="s">
-        <v>318</v>
-      </c>
       <c r="J1" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>322</v>
       </c>
-      <c r="L1" s="9" t="s">
-        <v>323</v>
-      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
       <c r="J2" s="10">
         <f>COUNTIF(G3:G126,"решена")/124</f>
-        <v>0.45161290322580644</v>
+        <v>0.45967741935483869</v>
       </c>
       <c r="K2" s="11">
         <f>SUM(H3:H126)/(COUNTIF(G3:G126,"решена") + COUNTIF(G3:G126,"не решена"))</f>
-        <v>2.3103448275862069</v>
+        <v>2.3389830508474576</v>
       </c>
       <c r="L2" s="10">
         <f>SUM(I3:I126)/SUM(H3:H126)</f>
-        <v>0.73134328358208955</v>
+        <v>0.73188405797101452</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="27">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -1696,7 +1693,7 @@
         <v>10</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H3" s="5">
         <v>5</v>
@@ -1709,9 +1706,9 @@
       <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="18"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="6" t="s">
         <v>11</v>
       </c>
@@ -1722,7 +1719,7 @@
         <v>12</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H4" s="5">
         <v>1</v>
@@ -1732,9 +1729,9 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="18">
+      <c r="A5" s="26"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="27">
         <v>2</v>
       </c>
       <c r="D5" s="6" t="s">
@@ -1747,7 +1744,7 @@
         <v>14</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H5" s="5">
         <v>3</v>
@@ -1757,9 +1754,9 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="18"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="6" t="s">
         <v>15</v>
       </c>
@@ -1770,7 +1767,7 @@
         <v>16</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H6" s="5">
         <v>2</v>
@@ -1780,13 +1777,13 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>324</v>
-      </c>
-      <c r="C7" s="18">
+      <c r="B7" s="25" t="s">
+        <v>323</v>
+      </c>
+      <c r="C7" s="27">
         <v>3</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -1799,7 +1796,7 @@
         <v>19</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H7" s="5">
         <v>2</v>
@@ -1809,9 +1806,9 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="16"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="18"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="6" t="s">
         <v>20</v>
       </c>
@@ -1822,7 +1819,7 @@
         <v>21</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H8" s="5">
         <v>1</v>
@@ -1832,9 +1829,9 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="18">
+      <c r="A9" s="26"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="27">
         <v>4</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -1847,7 +1844,7 @@
         <v>23</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H9" s="5">
         <v>1</v>
@@ -1857,9 +1854,9 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="18"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="6" t="s">
         <v>24</v>
       </c>
@@ -1870,7 +1867,7 @@
         <v>25</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H10" s="5">
         <v>3</v>
@@ -1880,13 +1877,13 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="27">
         <v>5</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -1899,7 +1896,7 @@
         <v>28</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H11" s="5">
         <v>1</v>
@@ -1909,9 +1906,9 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="18"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="6" t="s">
         <v>29</v>
       </c>
@@ -1922,7 +1919,7 @@
         <v>30</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H12" s="5">
         <v>2</v>
@@ -1932,9 +1929,9 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="18">
+      <c r="A13" s="26"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="27">
         <v>6</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -1947,7 +1944,7 @@
         <v>32</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H13" s="5">
         <v>2</v>
@@ -1957,9 +1954,9 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="18"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="6" t="s">
         <v>33</v>
       </c>
@@ -1970,7 +1967,7 @@
         <v>34</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H14" s="5">
         <v>5</v>
@@ -1980,13 +1977,13 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="27">
         <v>7</v>
       </c>
       <c r="D15" s="6" t="s">
@@ -1999,7 +1996,7 @@
         <v>37</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H15" s="5">
         <v>2</v>
@@ -2009,9 +2006,9 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="18"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="6" t="s">
         <v>38</v>
       </c>
@@ -2022,7 +2019,7 @@
         <v>39</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H16" s="5">
         <v>2</v>
@@ -2032,9 +2029,9 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="18">
+      <c r="A17" s="18"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="27">
         <v>8</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -2047,7 +2044,7 @@
         <v>41</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H17" s="5">
         <v>3</v>
@@ -2057,9 +2054,9 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="18"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="6" t="s">
         <v>42</v>
       </c>
@@ -2070,7 +2067,7 @@
         <v>43</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H18" s="5">
         <v>6</v>
@@ -2080,13 +2077,13 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="27">
         <v>9</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -2099,7 +2096,7 @@
         <v>46</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H19" s="5">
         <v>1</v>
@@ -2109,9 +2106,9 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="18"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="6" t="s">
         <v>47</v>
       </c>
@@ -2122,7 +2119,7 @@
         <v>48</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H20" s="5">
         <v>1</v>
@@ -2132,9 +2129,9 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="19">
+      <c r="A21" s="18"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="27">
         <v>10</v>
       </c>
       <c r="D21" s="6" t="s">
@@ -2147,7 +2144,7 @@
         <v>50</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H21" s="5">
         <v>2</v>
@@ -2157,9 +2154,9 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="19"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="13" t="s">
         <v>51</v>
       </c>
@@ -2170,7 +2167,7 @@
         <v>52</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H22" s="15">
         <v>0</v>
@@ -2180,13 +2177,13 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="27">
         <v>11</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -2199,7 +2196,7 @@
         <v>55</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H23" s="5">
         <v>2</v>
@@ -2209,9 +2206,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="18"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="6" t="s">
         <v>56</v>
       </c>
@@ -2222,7 +2219,7 @@
         <v>57</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H24" s="5">
         <v>2</v>
@@ -2232,9 +2229,9 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="18">
+      <c r="A25" s="18"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="27">
         <v>12</v>
       </c>
       <c r="D25" s="6" t="s">
@@ -2247,7 +2244,7 @@
         <v>59</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H25" s="5">
         <v>2</v>
@@ -2257,9 +2254,9 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="18"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="6" t="s">
         <v>60</v>
       </c>
@@ -2270,7 +2267,7 @@
         <v>61</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H26" s="5">
         <v>2</v>
@@ -2280,13 +2277,13 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C27" s="27">
         <v>13</v>
       </c>
       <c r="D27" s="6" t="s">
@@ -2299,7 +2296,7 @@
         <v>64</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H27" s="5">
         <v>2</v>
@@ -2309,9 +2306,9 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="16"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="18"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="6" t="s">
         <v>65</v>
       </c>
@@ -2322,7 +2319,7 @@
         <v>66</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H28" s="5">
         <v>4</v>
@@ -2332,9 +2329,9 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="16"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="18">
+      <c r="A29" s="26"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="27">
         <v>14</v>
       </c>
       <c r="D29" s="6" t="s">
@@ -2347,7 +2344,7 @@
         <v>68</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H29" s="5">
         <v>1</v>
@@ -2357,9 +2354,9 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="16"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="18"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="27"/>
       <c r="D30" s="6" t="s">
         <v>69</v>
       </c>
@@ -2370,7 +2367,7 @@
         <v>70</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H30" s="5">
         <v>1</v>
@@ -2380,13 +2377,13 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31" s="27">
         <v>15</v>
       </c>
       <c r="D31" s="6" t="s">
@@ -2399,7 +2396,7 @@
         <v>73</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H31" s="5">
         <v>1</v>
@@ -2409,9 +2406,9 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="16"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="18"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="27"/>
       <c r="D32" s="6" t="s">
         <v>74</v>
       </c>
@@ -2422,7 +2419,7 @@
         <v>75</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H32" s="5">
         <v>1</v>
@@ -2432,9 +2429,9 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="16"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="18">
+      <c r="A33" s="26"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="27">
         <v>16</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -2447,7 +2444,7 @@
         <v>77</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H33" s="5">
         <v>2</v>
@@ -2457,9 +2454,9 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="16"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="18"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="6" t="s">
         <v>78</v>
       </c>
@@ -2470,7 +2467,7 @@
         <v>79</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H34" s="5">
         <v>2</v>
@@ -2480,13 +2477,13 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="C35" s="18">
+      <c r="C35" s="27">
         <v>17</v>
       </c>
       <c r="D35" s="6" t="s">
@@ -2499,7 +2496,7 @@
         <v>82</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H35" s="5">
         <v>4</v>
@@ -2509,9 +2506,9 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="16"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="18"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="27"/>
       <c r="D36" s="6" t="s">
         <v>83</v>
       </c>
@@ -2522,7 +2519,7 @@
         <v>84</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H36" s="5">
         <v>1</v>
@@ -2532,13 +2529,13 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="25" t="s">
         <v>203</v>
       </c>
-      <c r="C37" s="18">
+      <c r="C37" s="27">
         <v>18</v>
       </c>
       <c r="D37" s="6" t="s">
@@ -2551,7 +2548,7 @@
         <v>87</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H37" s="5">
         <v>3</v>
@@ -2561,9 +2558,9 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="16"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="18"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="27"/>
       <c r="D38" s="6" t="s">
         <v>88</v>
       </c>
@@ -2574,7 +2571,7 @@
         <v>89</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H38" s="5">
         <v>2</v>
@@ -2584,9 +2581,9 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="16"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="18">
+      <c r="A39" s="26"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="27">
         <v>19</v>
       </c>
       <c r="D39" s="6" t="s">
@@ -2599,7 +2596,7 @@
         <v>91</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H39" s="5">
         <v>1</v>
@@ -2609,9 +2606,9 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="16"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="18"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="27"/>
       <c r="D40" s="6" t="s">
         <v>92</v>
       </c>
@@ -2622,7 +2619,7 @@
         <v>93</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H40" s="5">
         <v>1</v>
@@ -2632,13 +2629,13 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="25" t="s">
         <v>204</v>
       </c>
-      <c r="C41" s="18">
+      <c r="C41" s="27">
         <v>20</v>
       </c>
       <c r="D41" s="6" t="s">
@@ -2651,7 +2648,7 @@
         <v>96</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H41" s="5">
         <v>1</v>
@@ -2661,9 +2658,9 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="16"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="18"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="27"/>
       <c r="D42" s="6" t="s">
         <v>97</v>
       </c>
@@ -2674,7 +2671,7 @@
         <v>98</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H42" s="5">
         <v>2</v>
@@ -2684,9 +2681,9 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="16"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="18">
+      <c r="A43" s="26"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="27">
         <v>21</v>
       </c>
       <c r="D43" s="6" t="s">
@@ -2699,7 +2696,7 @@
         <v>100</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H43" s="5">
         <v>2</v>
@@ -2709,9 +2706,9 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="16"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="18"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="27"/>
       <c r="D44" s="6" t="s">
         <v>101</v>
       </c>
@@ -2722,7 +2719,7 @@
         <v>102</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H44" s="5">
         <v>1</v>
@@ -2732,13 +2729,13 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B45" s="20" t="s">
+      <c r="B45" s="25" t="s">
         <v>205</v>
       </c>
-      <c r="C45" s="18">
+      <c r="C45" s="27">
         <v>22</v>
       </c>
       <c r="D45" s="6" t="s">
@@ -2751,7 +2748,7 @@
         <v>105</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H45" s="5">
         <v>1</v>
@@ -2761,9 +2758,9 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="16"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="18"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="27"/>
       <c r="D46" s="6" t="s">
         <v>106</v>
       </c>
@@ -2774,7 +2771,7 @@
         <v>107</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H46" s="5">
         <v>5</v>
@@ -2784,13 +2781,13 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="16" t="s">
+      <c r="A47" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="C47" s="18">
+      <c r="C47" s="27">
         <v>23</v>
       </c>
       <c r="D47" s="6" t="s">
@@ -2803,7 +2800,7 @@
         <v>110</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H47" s="5">
         <v>3</v>
@@ -2813,9 +2810,9 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="16"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="18"/>
+      <c r="A48" s="26"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="27"/>
       <c r="D48" s="6" t="s">
         <v>111</v>
       </c>
@@ -2826,7 +2823,7 @@
         <v>112</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H48" s="5">
         <v>2</v>
@@ -2836,9 +2833,9 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="16"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="18">
+      <c r="A49" s="26"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="27">
         <v>24</v>
       </c>
       <c r="D49" s="6" t="s">
@@ -2851,7 +2848,7 @@
         <v>114</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H49" s="5">
         <v>1</v>
@@ -2861,9 +2858,9 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="16"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="18"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="27"/>
       <c r="D50" s="6" t="s">
         <v>115</v>
       </c>
@@ -2874,7 +2871,7 @@
         <v>116</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H50" s="5">
         <v>1</v>
@@ -2884,13 +2881,13 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="B51" s="25" t="s">
         <v>207</v>
       </c>
-      <c r="C51" s="18">
+      <c r="C51" s="27">
         <v>25</v>
       </c>
       <c r="D51" s="6" t="s">
@@ -2903,7 +2900,7 @@
         <v>119</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H51" s="5">
         <v>1</v>
@@ -2913,9 +2910,9 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="16"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="18"/>
+      <c r="A52" s="26"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="27"/>
       <c r="D52" s="6" t="s">
         <v>120</v>
       </c>
@@ -2926,7 +2923,7 @@
         <v>121</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H52" s="5">
         <v>3</v>
@@ -2936,13 +2933,13 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="16" t="s">
+      <c r="A53" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="C53" s="18">
+      <c r="C53" s="27">
         <v>26</v>
       </c>
       <c r="D53" s="6" t="s">
@@ -2955,7 +2952,7 @@
         <v>124</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H53" s="5">
         <v>5</v>
@@ -2965,9 +2962,9 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="16"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="18"/>
+      <c r="A54" s="26"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="27"/>
       <c r="D54" s="6" t="s">
         <v>125</v>
       </c>
@@ -2978,7 +2975,7 @@
         <v>126</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H54" s="5">
         <v>6</v>
@@ -2988,9 +2985,9 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="16"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="19">
+      <c r="A55" s="26"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="27">
         <v>27</v>
       </c>
       <c r="D55" s="6" t="s">
@@ -3003,7 +3000,7 @@
         <v>128</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H55" s="5">
         <v>3</v>
@@ -3013,9 +3010,9 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="16"/>
-      <c r="B56" s="20"/>
-      <c r="C56" s="19"/>
+      <c r="A56" s="26"/>
+      <c r="B56" s="25"/>
+      <c r="C56" s="27"/>
       <c r="D56" s="13" t="s">
         <v>129</v>
       </c>
@@ -3026,7 +3023,7 @@
         <v>130</v>
       </c>
       <c r="G56" s="15" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H56" s="15">
         <v>3</v>
@@ -3036,13 +3033,13 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="16" t="s">
+      <c r="A57" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="B57" s="20" t="s">
+      <c r="B57" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="C57" s="18">
+      <c r="C57" s="27">
         <v>28</v>
       </c>
       <c r="D57" s="6" t="s">
@@ -3055,7 +3052,7 @@
         <v>133</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H57" s="5">
         <v>5</v>
@@ -3065,9 +3062,9 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="16"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="18"/>
+      <c r="A58" s="26"/>
+      <c r="B58" s="25"/>
+      <c r="C58" s="27"/>
       <c r="D58" s="6" t="s">
         <v>134</v>
       </c>
@@ -3078,7 +3075,7 @@
         <v>135</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H58" s="5">
         <v>2</v>
@@ -3088,9 +3085,9 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="16"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="18">
+      <c r="A59" s="26"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="27">
         <v>29</v>
       </c>
       <c r="D59" s="6" t="s">
@@ -3103,7 +3100,7 @@
         <v>137</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H59" s="5">
         <v>2</v>
@@ -3113,9 +3110,9 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="16"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="18"/>
+      <c r="A60" s="26"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="27"/>
       <c r="D60" s="6" t="s">
         <v>138</v>
       </c>
@@ -3126,7 +3123,7 @@
         <v>139</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H60" s="5">
         <v>6</v>
@@ -3136,34 +3133,38 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="17" t="s">
+      <c r="A61" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="B61" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="C61" s="19">
+      <c r="B61" s="25" t="s">
+        <v>325</v>
+      </c>
+      <c r="C61" s="20">
         <v>30</v>
       </c>
-      <c r="D61" s="1" t="s">
+      <c r="D61" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="E61" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F61" s="1" t="s">
+      <c r="E61" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F61" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="G61" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
+      <c r="G61" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="H61" s="5">
+        <v>4</v>
+      </c>
+      <c r="I61" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="17"/>
-      <c r="B62" s="21"/>
-      <c r="C62" s="19"/>
+      <c r="A62" s="18"/>
+      <c r="B62" s="25"/>
+      <c r="C62" s="20"/>
       <c r="D62" s="1" t="s">
         <v>143</v>
       </c>
@@ -3174,15 +3175,15 @@
         <v>144</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="17"/>
-      <c r="B63" s="21"/>
-      <c r="C63" s="19">
+      <c r="A63" s="18"/>
+      <c r="B63" s="25"/>
+      <c r="C63" s="20">
         <v>31</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -3195,15 +3196,15 @@
         <v>146</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="17"/>
-      <c r="B64" s="21"/>
-      <c r="C64" s="19"/>
+      <c r="A64" s="18"/>
+      <c r="B64" s="25"/>
+      <c r="C64" s="20"/>
       <c r="D64" s="1" t="s">
         <v>147</v>
       </c>
@@ -3214,19 +3215,19 @@
         <v>148</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="17" t="s">
+      <c r="A65" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="B65" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="C65" s="19">
+      <c r="B65" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="C65" s="20">
         <v>32</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -3239,15 +3240,15 @@
         <v>151</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="17"/>
-      <c r="B66" s="21"/>
-      <c r="C66" s="19"/>
+      <c r="A66" s="18"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="20"/>
       <c r="D66" s="1" t="s">
         <v>152</v>
       </c>
@@ -3258,15 +3259,15 @@
         <v>153</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="17"/>
-      <c r="B67" s="21"/>
-      <c r="C67" s="19">
+      <c r="A67" s="18"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="20">
         <v>33</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -3279,15 +3280,15 @@
         <v>155</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="17"/>
-      <c r="B68" s="21"/>
-      <c r="C68" s="19"/>
+      <c r="A68" s="18"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="20"/>
       <c r="D68" s="1" t="s">
         <v>156</v>
       </c>
@@ -3298,19 +3299,19 @@
         <v>157</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="17" t="s">
+      <c r="A69" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="B69" s="21" t="s">
-        <v>212</v>
-      </c>
-      <c r="C69" s="19">
+      <c r="B69" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="C69" s="20">
         <v>34</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -3323,15 +3324,15 @@
         <v>160</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="17"/>
-      <c r="B70" s="21"/>
-      <c r="C70" s="19"/>
+      <c r="A70" s="18"/>
+      <c r="B70" s="24"/>
+      <c r="C70" s="20"/>
       <c r="D70" s="1" t="s">
         <v>161</v>
       </c>
@@ -3342,19 +3343,19 @@
         <v>162</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="17" t="s">
+      <c r="A71" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="B71" s="21" t="s">
-        <v>213</v>
-      </c>
-      <c r="C71" s="19">
+      <c r="B71" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="C71" s="20">
         <v>35</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -3367,15 +3368,15 @@
         <v>165</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="17"/>
-      <c r="B72" s="21"/>
-      <c r="C72" s="19"/>
+      <c r="A72" s="18"/>
+      <c r="B72" s="24"/>
+      <c r="C72" s="20"/>
       <c r="D72" s="1" t="s">
         <v>166</v>
       </c>
@@ -3386,15 +3387,15 @@
         <v>167</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="17"/>
-      <c r="B73" s="21"/>
-      <c r="C73" s="19">
+      <c r="A73" s="18"/>
+      <c r="B73" s="24"/>
+      <c r="C73" s="20">
         <v>36</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -3407,15 +3408,15 @@
         <v>169</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="17"/>
-      <c r="B74" s="21"/>
-      <c r="C74" s="19"/>
+      <c r="A74" s="18"/>
+      <c r="B74" s="24"/>
+      <c r="C74" s="20"/>
       <c r="D74" s="1" t="s">
         <v>170</v>
       </c>
@@ -3426,19 +3427,19 @@
         <v>171</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="17" t="s">
+      <c r="A75" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="B75" s="21" t="s">
-        <v>214</v>
-      </c>
-      <c r="C75" s="19">
+      <c r="B75" s="24" t="s">
+        <v>213</v>
+      </c>
+      <c r="C75" s="20">
         <v>37</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -3451,15 +3452,15 @@
         <v>174</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="17"/>
-      <c r="B76" s="21"/>
-      <c r="C76" s="19"/>
+      <c r="A76" s="18"/>
+      <c r="B76" s="24"/>
+      <c r="C76" s="20"/>
       <c r="D76" s="1" t="s">
         <v>175</v>
       </c>
@@ -3470,15 +3471,15 @@
         <v>176</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="17"/>
-      <c r="B77" s="21"/>
-      <c r="C77" s="19">
+      <c r="A77" s="18"/>
+      <c r="B77" s="24"/>
+      <c r="C77" s="20">
         <v>38</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -3491,15 +3492,15 @@
         <v>178</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="17"/>
-      <c r="B78" s="21"/>
-      <c r="C78" s="19"/>
+      <c r="A78" s="18"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="20"/>
       <c r="D78" s="1" t="s">
         <v>179</v>
       </c>
@@ -3510,19 +3511,19 @@
         <v>180</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="17" t="s">
+      <c r="A79" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="B79" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="C79" s="19">
+      <c r="B79" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="C79" s="20">
         <v>39</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -3535,15 +3536,15 @@
         <v>183</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="17"/>
-      <c r="B80" s="21"/>
-      <c r="C80" s="19"/>
+      <c r="A80" s="18"/>
+      <c r="B80" s="24"/>
+      <c r="C80" s="20"/>
       <c r="D80" s="1" t="s">
         <v>184</v>
       </c>
@@ -3554,19 +3555,19 @@
         <v>185</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="17" t="s">
+      <c r="A81" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="B81" s="21" t="s">
-        <v>216</v>
-      </c>
-      <c r="C81" s="19">
+      <c r="B81" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="C81" s="20">
         <v>40</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -3579,15 +3580,15 @@
         <v>188</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="17"/>
-      <c r="B82" s="21"/>
-      <c r="C82" s="19"/>
+      <c r="A82" s="18"/>
+      <c r="B82" s="24"/>
+      <c r="C82" s="20"/>
       <c r="D82" s="1" t="s">
         <v>189</v>
       </c>
@@ -3598,19 +3599,19 @@
         <v>190</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
     </row>
     <row r="83" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="17" t="s">
+      <c r="A83" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="B83" s="27" t="s">
-        <v>217</v>
-      </c>
-      <c r="C83" s="19">
+      <c r="B83" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="C83" s="20">
         <v>41</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -3623,15 +3624,15 @@
         <v>193</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="17"/>
-      <c r="B84" s="28"/>
-      <c r="C84" s="19"/>
+      <c r="A84" s="18"/>
+      <c r="B84" s="22"/>
+      <c r="C84" s="20"/>
       <c r="D84" s="1" t="s">
         <v>194</v>
       </c>
@@ -3642,442 +3643,442 @@
         <v>195</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="17"/>
-      <c r="B85" s="28"/>
-      <c r="C85" s="19">
+      <c r="A85" s="18"/>
+      <c r="B85" s="22"/>
+      <c r="C85" s="20">
         <v>42</v>
       </c>
       <c r="D85" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F85" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="E85" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>219</v>
-      </c>
       <c r="G85" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="17"/>
-      <c r="B86" s="29"/>
-      <c r="C86" s="19"/>
+      <c r="A86" s="18"/>
+      <c r="B86" s="23"/>
+      <c r="C86" s="20"/>
       <c r="D86" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F86" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="E86" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="G86" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H86" s="4"/>
       <c r="I86" s="4"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="17" t="s">
+      <c r="A87" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="B87" s="24" t="s">
+        <v>300</v>
+      </c>
+      <c r="C87" s="20">
+        <v>43</v>
+      </c>
+      <c r="D87" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B87" s="21" t="s">
-        <v>301</v>
-      </c>
-      <c r="C87" s="19">
-        <v>43</v>
-      </c>
-      <c r="D87" s="2" t="s">
+      <c r="E87" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F87" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E87" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>225</v>
-      </c>
       <c r="G87" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="17"/>
-      <c r="B88" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C88" s="19"/>
+      <c r="A88" s="18"/>
+      <c r="B88" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C88" s="20"/>
       <c r="D88" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F88" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="E88" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>227</v>
-      </c>
       <c r="G88" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" s="17"/>
-      <c r="B89" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C89" s="19">
+      <c r="A89" s="18"/>
+      <c r="B89" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C89" s="20">
         <v>44</v>
       </c>
       <c r="D89" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F89" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="E89" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>229</v>
-      </c>
       <c r="G89" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90" s="17"/>
-      <c r="B90" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C90" s="19"/>
+      <c r="A90" s="18"/>
+      <c r="B90" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C90" s="20"/>
       <c r="D90" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F90" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E90" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>231</v>
-      </c>
       <c r="G90" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91" s="17" t="s">
+      <c r="A91" s="18" t="s">
+        <v>231</v>
+      </c>
+      <c r="B91" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="C91" s="20">
+        <v>45</v>
+      </c>
+      <c r="D91" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="B91" s="21" t="s">
-        <v>302</v>
-      </c>
-      <c r="C91" s="19">
-        <v>45</v>
-      </c>
-      <c r="D91" s="2" t="s">
+      <c r="E91" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F91" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="E91" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F91" s="2" t="s">
-        <v>234</v>
-      </c>
       <c r="G91" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A92" s="17"/>
-      <c r="B92" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C92" s="19"/>
+      <c r="A92" s="18"/>
+      <c r="B92" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C92" s="20"/>
       <c r="D92" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F92" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="E92" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>236</v>
-      </c>
       <c r="G92" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H92" s="4"/>
       <c r="I92" s="4"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" s="17"/>
-      <c r="B93" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C93" s="19">
+      <c r="A93" s="18"/>
+      <c r="B93" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C93" s="20">
         <v>46</v>
       </c>
       <c r="D93" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F93" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="E93" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>238</v>
-      </c>
       <c r="G93" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94" s="17"/>
-      <c r="B94" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C94" s="19"/>
+      <c r="A94" s="18"/>
+      <c r="B94" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C94" s="20"/>
       <c r="D94" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F94" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="E94" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F94" s="2" t="s">
-        <v>240</v>
-      </c>
       <c r="G94" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H94" s="4"/>
       <c r="I94" s="4"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95" s="17" t="s">
+      <c r="A95" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="B95" s="24" t="s">
+        <v>302</v>
+      </c>
+      <c r="C95" s="20">
+        <v>47</v>
+      </c>
+      <c r="D95" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B95" s="21" t="s">
-        <v>303</v>
-      </c>
-      <c r="C95" s="19">
-        <v>47</v>
-      </c>
-      <c r="D95" s="2" t="s">
+      <c r="E95" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F95" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="E95" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F95" s="2" t="s">
-        <v>243</v>
-      </c>
       <c r="G95" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H95" s="4"/>
       <c r="I95" s="4"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A96" s="17"/>
-      <c r="B96" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C96" s="19"/>
+      <c r="A96" s="18"/>
+      <c r="B96" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C96" s="20"/>
       <c r="D96" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F96" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="E96" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>245</v>
-      </c>
       <c r="G96" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H96" s="4"/>
       <c r="I96" s="4"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97" s="17"/>
-      <c r="B97" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C97" s="19">
+      <c r="A97" s="18"/>
+      <c r="B97" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C97" s="20">
         <v>48</v>
       </c>
       <c r="D97" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F97" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="E97" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>247</v>
-      </c>
       <c r="G97" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H97" s="4"/>
       <c r="I97" s="4"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98" s="17"/>
-      <c r="B98" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C98" s="19"/>
+      <c r="A98" s="18"/>
+      <c r="B98" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C98" s="20"/>
       <c r="D98" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F98" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="E98" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F98" s="2" t="s">
-        <v>249</v>
-      </c>
       <c r="G98" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H98" s="4"/>
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" s="17" t="s">
+      <c r="A99" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="B99" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="C99" s="20">
+        <v>49</v>
+      </c>
+      <c r="D99" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B99" s="21" t="s">
-        <v>304</v>
-      </c>
-      <c r="C99" s="19">
-        <v>49</v>
-      </c>
-      <c r="D99" s="2" t="s">
+      <c r="E99" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F99" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E99" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>252</v>
-      </c>
       <c r="G99" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H99" s="4"/>
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" s="17"/>
-      <c r="B100" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C100" s="19"/>
+      <c r="A100" s="18"/>
+      <c r="B100" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C100" s="20"/>
       <c r="D100" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F100" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="E100" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>254</v>
-      </c>
       <c r="G100" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H100" s="4"/>
       <c r="I100" s="4"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101" s="17"/>
-      <c r="B101" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C101" s="19">
+      <c r="A101" s="18"/>
+      <c r="B101" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C101" s="20">
         <v>50</v>
       </c>
       <c r="D101" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F101" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="E101" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>256</v>
-      </c>
       <c r="G101" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H101" s="4"/>
       <c r="I101" s="4"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A102" s="17"/>
-      <c r="B102" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C102" s="19"/>
+      <c r="A102" s="18"/>
+      <c r="B102" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C102" s="20"/>
       <c r="D102" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F102" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="E102" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>258</v>
-      </c>
       <c r="G102" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H102" s="4"/>
       <c r="I102" s="4"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A103" s="17" t="s">
+      <c r="A103" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="B103" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="C103" s="20">
+        <v>51</v>
+      </c>
+      <c r="D103" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B103" s="21" t="s">
-        <v>305</v>
-      </c>
-      <c r="C103" s="19">
-        <v>51</v>
-      </c>
-      <c r="D103" s="2" t="s">
+      <c r="E103" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F103" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="E103" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F103" s="2" t="s">
-        <v>261</v>
-      </c>
       <c r="G103" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H103" s="4"/>
       <c r="I103" s="4"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" s="17"/>
-      <c r="B104" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C104" s="19"/>
+      <c r="A104" s="18"/>
+      <c r="B104" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C104" s="20"/>
       <c r="D104" s="2" t="s">
         <v>60</v>
       </c>
@@ -4088,42 +4089,42 @@
         <v>61</v>
       </c>
       <c r="G104" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H104" s="4"/>
       <c r="I104" s="4"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A105" s="17" t="s">
+      <c r="A105" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="B105" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="B105" s="22" t="s">
+      <c r="C105" s="20">
+        <v>52</v>
+      </c>
+      <c r="D105" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="C105" s="19">
-        <v>52</v>
-      </c>
-      <c r="D105" s="2" t="s">
+      <c r="E105" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F105" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="E105" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>265</v>
-      </c>
       <c r="G105" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H105" s="4"/>
       <c r="I105" s="4"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A106" s="17"/>
-      <c r="B106" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C106" s="19"/>
+      <c r="A106" s="18"/>
+      <c r="B106" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C106" s="20"/>
       <c r="D106" s="2" t="s">
         <v>24</v>
       </c>
@@ -4134,17 +4135,17 @@
         <v>25</v>
       </c>
       <c r="G106" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H106" s="4"/>
       <c r="I106" s="4"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A107" s="17"/>
-      <c r="B107" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C107" s="19">
+      <c r="A107" s="18"/>
+      <c r="B107" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C107" s="20">
         <v>53</v>
       </c>
       <c r="D107" s="2" t="s">
@@ -4157,17 +4158,17 @@
         <v>133</v>
       </c>
       <c r="G107" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H107" s="4"/>
       <c r="I107" s="4"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A108" s="17"/>
-      <c r="B108" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C108" s="19"/>
+      <c r="A108" s="18"/>
+      <c r="B108" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C108" s="20"/>
       <c r="D108" s="2" t="s">
         <v>136</v>
       </c>
@@ -4178,245 +4179,245 @@
         <v>137</v>
       </c>
       <c r="G108" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H108" s="4"/>
       <c r="I108" s="4"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" s="17" t="s">
+      <c r="A109" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="B109" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="C109" s="20">
+        <v>54</v>
+      </c>
+      <c r="D109" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="B109" s="21" t="s">
-        <v>306</v>
-      </c>
-      <c r="C109" s="19">
-        <v>54</v>
-      </c>
-      <c r="D109" s="2" t="s">
+      <c r="E109" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F109" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="E109" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F109" s="2" t="s">
-        <v>268</v>
-      </c>
       <c r="G109" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H109" s="4"/>
       <c r="I109" s="4"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A110" s="17"/>
-      <c r="B110" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C110" s="19"/>
+      <c r="A110" s="18"/>
+      <c r="B110" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C110" s="20"/>
       <c r="D110" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F110" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="E110" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F110" s="2" t="s">
-        <v>270</v>
-      </c>
       <c r="G110" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H110" s="4"/>
       <c r="I110" s="4"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A111" s="17" t="s">
+      <c r="A111" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="B111" s="24" t="s">
+        <v>306</v>
+      </c>
+      <c r="C111" s="20">
+        <v>55</v>
+      </c>
+      <c r="D111" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="B111" s="21" t="s">
-        <v>307</v>
-      </c>
-      <c r="C111" s="19">
-        <v>55</v>
-      </c>
-      <c r="D111" s="2" t="s">
+      <c r="E111" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F111" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="E111" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F111" s="2" t="s">
-        <v>273</v>
-      </c>
       <c r="G111" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H111" s="4"/>
       <c r="I111" s="4"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A112" s="17"/>
-      <c r="B112" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C112" s="19"/>
+      <c r="A112" s="18"/>
+      <c r="B112" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C112" s="20"/>
       <c r="D112" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F112" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="E112" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F112" s="2" t="s">
-        <v>275</v>
-      </c>
       <c r="G112" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H112" s="4"/>
       <c r="I112" s="4"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A113" s="17" t="s">
+      <c r="A113" s="18" t="s">
+        <v>275</v>
+      </c>
+      <c r="B113" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="B113" s="22" t="s">
+      <c r="C113" s="20">
+        <v>56</v>
+      </c>
+      <c r="D113" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C113" s="19">
-        <v>56</v>
-      </c>
-      <c r="D113" s="2" t="s">
+      <c r="E113" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F113" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="E113" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F113" s="2" t="s">
-        <v>279</v>
-      </c>
       <c r="G113" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H113" s="4"/>
       <c r="I113" s="4"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A114" s="17"/>
-      <c r="B114" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C114" s="19"/>
+      <c r="A114" s="18"/>
+      <c r="B114" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C114" s="20"/>
       <c r="D114" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F114" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="E114" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F114" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="G114" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H114" s="4"/>
       <c r="I114" s="4"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A115" s="17"/>
-      <c r="B115" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C115" s="19">
+      <c r="A115" s="18"/>
+      <c r="B115" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C115" s="20">
         <v>57</v>
       </c>
       <c r="D115" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F115" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="E115" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>283</v>
-      </c>
       <c r="G115" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H115" s="4"/>
       <c r="I115" s="4"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A116" s="17"/>
-      <c r="B116" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C116" s="19"/>
+      <c r="A116" s="18"/>
+      <c r="B116" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C116" s="20"/>
       <c r="D116" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F116" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="E116" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F116" s="2" t="s">
-        <v>285</v>
-      </c>
       <c r="G116" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H116" s="4"/>
       <c r="I116" s="4"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A117" s="17" t="s">
+      <c r="A117" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="B117" s="19" t="s">
         <v>286</v>
       </c>
-      <c r="B117" s="22" t="s">
+      <c r="C117" s="20">
+        <v>58</v>
+      </c>
+      <c r="D117" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="C117" s="19">
-        <v>58</v>
-      </c>
-      <c r="D117" s="2" t="s">
+      <c r="E117" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F117" s="2" t="s">
         <v>288</v>
       </c>
-      <c r="E117" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F117" s="2" t="s">
-        <v>289</v>
-      </c>
       <c r="G117" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H117" s="4"/>
       <c r="I117" s="4"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A118" s="17"/>
-      <c r="B118" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C118" s="19"/>
+      <c r="A118" s="18"/>
+      <c r="B118" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C118" s="20"/>
       <c r="D118" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F118" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="E118" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F118" s="2" t="s">
-        <v>291</v>
-      </c>
       <c r="G118" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H118" s="4"/>
       <c r="I118" s="4"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A119" s="17"/>
-      <c r="B119" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C119" s="19">
+      <c r="A119" s="18"/>
+      <c r="B119" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C119" s="20">
         <v>59</v>
       </c>
       <c r="D119" s="2" t="s">
@@ -4429,158 +4430,275 @@
         <v>34</v>
       </c>
       <c r="G119" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H119" s="4"/>
       <c r="I119" s="4"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A120" s="17"/>
-      <c r="B120" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C120" s="19"/>
+      <c r="A120" s="18"/>
+      <c r="B120" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C120" s="20"/>
       <c r="D120" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F120" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="E120" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F120" s="2" t="s">
-        <v>293</v>
-      </c>
       <c r="G120" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H120" s="4"/>
       <c r="I120" s="4"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" s="17" t="s">
+      <c r="A121" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="B121" s="19" t="s">
         <v>294</v>
       </c>
-      <c r="B121" s="22" t="s">
+      <c r="C121" s="20">
+        <v>60</v>
+      </c>
+      <c r="D121" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="C121" s="19">
-        <v>60</v>
-      </c>
-      <c r="D121" s="2" t="s">
+      <c r="E121" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F121" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="E121" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F121" s="2" t="s">
-        <v>297</v>
-      </c>
       <c r="G121" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H121" s="4"/>
       <c r="I121" s="4"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A122" s="17"/>
-      <c r="B122" s="22"/>
-      <c r="C122" s="19"/>
+      <c r="A122" s="18"/>
+      <c r="B122" s="19"/>
+      <c r="C122" s="20"/>
       <c r="D122" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E122" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="E122" s="2" t="s">
+      <c r="F122" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="F122" s="2" t="s">
-        <v>300</v>
-      </c>
       <c r="G122" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H122" s="4"/>
       <c r="I122" s="4"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A123" s="17"/>
-      <c r="B123" s="22"/>
-      <c r="C123" s="19">
+      <c r="A123" s="18"/>
+      <c r="B123" s="19"/>
+      <c r="C123" s="20">
         <v>61</v>
       </c>
       <c r="D123" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F123" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="E123" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="F123" s="2" t="s">
-        <v>309</v>
-      </c>
       <c r="G123" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H123" s="4"/>
       <c r="I123" s="4"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A124" s="17"/>
-      <c r="B124" s="22"/>
-      <c r="C124" s="19"/>
+      <c r="A124" s="18"/>
+      <c r="B124" s="19"/>
+      <c r="C124" s="20"/>
       <c r="D124" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F124" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="E124" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="F124" s="2" t="s">
-        <v>311</v>
-      </c>
       <c r="G124" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H124" s="4"/>
       <c r="I124" s="4"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A125" s="17"/>
-      <c r="B125" s="22"/>
-      <c r="C125" s="19">
+      <c r="A125" s="18"/>
+      <c r="B125" s="19"/>
+      <c r="C125" s="20">
         <v>62</v>
       </c>
       <c r="D125" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F125" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="E125" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="F125" s="2" t="s">
-        <v>313</v>
-      </c>
       <c r="G125" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H125" s="4"/>
       <c r="I125" s="4"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A126" s="17"/>
-      <c r="B126" s="22"/>
-      <c r="C126" s="19"/>
+      <c r="A126" s="18"/>
+      <c r="B126" s="19"/>
+      <c r="C126" s="20"/>
       <c r="D126" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F126" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="E126" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="F126" s="2" t="s">
-        <v>315</v>
-      </c>
       <c r="G126" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H126" s="4"/>
       <c r="I126" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="141">
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="A71:A74"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="C83:C84"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="A83:A86"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="A91:A94"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="A99:A102"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A117:A120"/>
+    <mergeCell ref="B87:B90"/>
+    <mergeCell ref="B91:B94"/>
+    <mergeCell ref="B95:B98"/>
+    <mergeCell ref="B99:B102"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="B111:B112"/>
+    <mergeCell ref="B113:B116"/>
+    <mergeCell ref="B117:B120"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A113:A116"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="C101:C102"/>
+    <mergeCell ref="C103:C104"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="C93:C94"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
@@ -4605,123 +4723,6 @@
     <mergeCell ref="C111:C112"/>
     <mergeCell ref="C113:C114"/>
     <mergeCell ref="C95:C96"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="C103:C104"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="A117:A120"/>
-    <mergeCell ref="B87:B90"/>
-    <mergeCell ref="B91:B94"/>
-    <mergeCell ref="B95:B98"/>
-    <mergeCell ref="B99:B102"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="B109:B110"/>
-    <mergeCell ref="B111:B112"/>
-    <mergeCell ref="B113:B116"/>
-    <mergeCell ref="B117:B120"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A113:A116"/>
-    <mergeCell ref="A83:A86"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="A91:A94"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="A99:A102"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B71:B74"/>
-    <mergeCell ref="B75:B78"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="C83:C84"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A75:A78"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="A71:A74"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A51:A52"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G126" xr:uid="{BD7D4049-E182-46D9-ABFE-ED680993C7C2}">
@@ -4787,9 +4788,10 @@
     <hyperlink ref="F58" r:id="rId56" xr:uid="{4C0BA54A-6492-48D4-AC2F-7E75F504E59B}"/>
     <hyperlink ref="F59" r:id="rId57" xr:uid="{7FF47B51-3E09-4769-9361-616326B362F0}"/>
     <hyperlink ref="F60" r:id="rId58" xr:uid="{9CECBBD6-2F14-4F88-B6F4-C08AF3014E4F}"/>
+    <hyperlink ref="F61" r:id="rId59" xr:uid="{F9AF7E56-A77D-4520-87E8-16AD5AF5E883}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId59"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId60"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
solve task '35. Search Insert Position'
</commit_message>
<xml_diff>
--- a/DSA studing (in acc. with Claude plan)/DSA_Leetcode_plan from Claude.xlsx
+++ b/DSA studing (in acc. with Claude plan)/DSA_Leetcode_plan from Claude.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Programming\Python\Leetcode\Leetcode practise\DSA studing (in acc. with Claude plan)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D685F28E-929E-49F2-A4AD-29470FB34C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F16590-8C6E-4890-8F73-8CFE6200EE79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1271,20 +1271,32 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1294,18 +1306,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1597,7 +1597,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B53" sqref="B53:B56"/>
+      <selection pane="bottomLeft" activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1613,31 +1613,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="16" t="s">
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="23" t="s">
         <v>315</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="23" t="s">
         <v>316</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="23" t="s">
         <v>317</v>
       </c>
       <c r="J1" s="9" t="s">
@@ -1651,36 +1651,36 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
       <c r="J2" s="10">
         <f>COUNTIF(G3:G126,"решена")/124</f>
-        <v>0.45967741935483869</v>
+        <v>0.46774193548387094</v>
       </c>
       <c r="K2" s="11">
         <f>SUM(H3:H126)/(COUNTIF(G3:G126,"решена") + COUNTIF(G3:G126,"не решена"))</f>
-        <v>2.3389830508474576</v>
+        <v>2.35</v>
       </c>
       <c r="L2" s="10">
         <f>SUM(I3:I126)/SUM(H3:H126)</f>
-        <v>0.73188405797101452</v>
+        <v>0.73758865248226946</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="20" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="18">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -1706,9 +1706,9 @@
       <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="26"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="27"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="6" t="s">
         <v>11</v>
       </c>
@@ -1729,9 +1729,9 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="27">
+      <c r="A5" s="16"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="18">
         <v>2</v>
       </c>
       <c r="D5" s="6" t="s">
@@ -1754,9 +1754,9 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="26"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="27"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="18"/>
       <c r="D6" s="6" t="s">
         <v>15</v>
       </c>
@@ -1777,13 +1777,13 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="18">
         <v>3</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -1806,9 +1806,9 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="27"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="18"/>
       <c r="D8" s="6" t="s">
         <v>20</v>
       </c>
@@ -1829,9 +1829,9 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="27">
+      <c r="A9" s="16"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="18">
         <v>4</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -1854,9 +1854,9 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="26"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="27"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="18"/>
       <c r="D10" s="6" t="s">
         <v>24</v>
       </c>
@@ -1877,13 +1877,13 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="18">
         <v>5</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -1906,9 +1906,9 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="26"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="27"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="18"/>
       <c r="D12" s="6" t="s">
         <v>29</v>
       </c>
@@ -1929,9 +1929,9 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="27">
+      <c r="A13" s="16"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="18">
         <v>6</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -1954,9 +1954,9 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="27"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="6" t="s">
         <v>33</v>
       </c>
@@ -1977,13 +1977,13 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="18">
         <v>7</v>
       </c>
       <c r="D15" s="6" t="s">
@@ -2006,9 +2006,9 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="18"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="27"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="18"/>
       <c r="D16" s="6" t="s">
         <v>38</v>
       </c>
@@ -2029,9 +2029,9 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="27">
+      <c r="A17" s="17"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="18">
         <v>8</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -2054,9 +2054,9 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="18"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="27"/>
+      <c r="A18" s="17"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="18"/>
       <c r="D18" s="6" t="s">
         <v>42</v>
       </c>
@@ -2077,13 +2077,13 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="C19" s="27">
+      <c r="C19" s="18">
         <v>9</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -2106,9 +2106,9 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="27"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="18"/>
       <c r="D20" s="6" t="s">
         <v>47</v>
       </c>
@@ -2129,9 +2129,9 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="18"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="27">
+      <c r="A21" s="17"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="18">
         <v>10</v>
       </c>
       <c r="D21" s="6" t="s">
@@ -2154,9 +2154,9 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="18"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="27"/>
+      <c r="A22" s="17"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="18"/>
       <c r="D22" s="13" t="s">
         <v>51</v>
       </c>
@@ -2177,13 +2177,13 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="21" t="s">
         <v>200</v>
       </c>
-      <c r="C23" s="27">
+      <c r="C23" s="18">
         <v>11</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -2206,9 +2206,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="18"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="27"/>
+      <c r="A24" s="17"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="18"/>
       <c r="D24" s="6" t="s">
         <v>56</v>
       </c>
@@ -2229,9 +2229,9 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="27">
+      <c r="A25" s="17"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="18">
         <v>12</v>
       </c>
       <c r="D25" s="6" t="s">
@@ -2254,9 +2254,9 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="18"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="27"/>
+      <c r="A26" s="17"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="18"/>
       <c r="D26" s="6" t="s">
         <v>60</v>
       </c>
@@ -2277,13 +2277,13 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="20" t="s">
         <v>201</v>
       </c>
-      <c r="C27" s="27">
+      <c r="C27" s="18">
         <v>13</v>
       </c>
       <c r="D27" s="6" t="s">
@@ -2306,9 +2306,9 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="26"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="27"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="18"/>
       <c r="D28" s="6" t="s">
         <v>65</v>
       </c>
@@ -2329,9 +2329,9 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="26"/>
-      <c r="B29" s="25"/>
-      <c r="C29" s="27">
+      <c r="A29" s="16"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="18">
         <v>14</v>
       </c>
       <c r="D29" s="6" t="s">
@@ -2354,9 +2354,9 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="26"/>
-      <c r="B30" s="25"/>
-      <c r="C30" s="27"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="18"/>
       <c r="D30" s="6" t="s">
         <v>69</v>
       </c>
@@ -2377,13 +2377,13 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="26" t="s">
+      <c r="A31" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="C31" s="27">
+      <c r="C31" s="18">
         <v>15</v>
       </c>
       <c r="D31" s="6" t="s">
@@ -2406,9 +2406,9 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="26"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="27"/>
+      <c r="A32" s="16"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="18"/>
       <c r="D32" s="6" t="s">
         <v>74</v>
       </c>
@@ -2429,9 +2429,9 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="26"/>
-      <c r="B33" s="25"/>
-      <c r="C33" s="27">
+      <c r="A33" s="16"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="18">
         <v>16</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -2454,9 +2454,9 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="26"/>
-      <c r="B34" s="25"/>
-      <c r="C34" s="27"/>
+      <c r="A34" s="16"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="18"/>
       <c r="D34" s="6" t="s">
         <v>78</v>
       </c>
@@ -2477,13 +2477,13 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="26" t="s">
+      <c r="A35" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="20" t="s">
         <v>202</v>
       </c>
-      <c r="C35" s="27">
+      <c r="C35" s="18">
         <v>17</v>
       </c>
       <c r="D35" s="6" t="s">
@@ -2506,9 +2506,9 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="26"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="27"/>
+      <c r="A36" s="16"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="18"/>
       <c r="D36" s="6" t="s">
         <v>83</v>
       </c>
@@ -2529,13 +2529,13 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="26" t="s">
+      <c r="A37" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="25" t="s">
+      <c r="B37" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="C37" s="27">
+      <c r="C37" s="18">
         <v>18</v>
       </c>
       <c r="D37" s="6" t="s">
@@ -2558,9 +2558,9 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="26"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="27"/>
+      <c r="A38" s="16"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="18"/>
       <c r="D38" s="6" t="s">
         <v>88</v>
       </c>
@@ -2581,9 +2581,9 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="26"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="27">
+      <c r="A39" s="16"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="18">
         <v>19</v>
       </c>
       <c r="D39" s="6" t="s">
@@ -2606,9 +2606,9 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="26"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="27"/>
+      <c r="A40" s="16"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="18"/>
       <c r="D40" s="6" t="s">
         <v>92</v>
       </c>
@@ -2629,13 +2629,13 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="26" t="s">
+      <c r="A41" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B41" s="25" t="s">
+      <c r="B41" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="C41" s="27">
+      <c r="C41" s="18">
         <v>20</v>
       </c>
       <c r="D41" s="6" t="s">
@@ -2658,9 +2658,9 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="26"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="27"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="18"/>
       <c r="D42" s="6" t="s">
         <v>97</v>
       </c>
@@ -2681,9 +2681,9 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="26"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="27">
+      <c r="A43" s="16"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="18">
         <v>21</v>
       </c>
       <c r="D43" s="6" t="s">
@@ -2706,9 +2706,9 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="26"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="27"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="18"/>
       <c r="D44" s="6" t="s">
         <v>101</v>
       </c>
@@ -2729,13 +2729,13 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="26" t="s">
+      <c r="A45" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="B45" s="25" t="s">
+      <c r="B45" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="C45" s="27">
+      <c r="C45" s="18">
         <v>22</v>
       </c>
       <c r="D45" s="6" t="s">
@@ -2758,9 +2758,9 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="26"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="27"/>
+      <c r="A46" s="16"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="18"/>
       <c r="D46" s="6" t="s">
         <v>106</v>
       </c>
@@ -2781,13 +2781,13 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="26" t="s">
+      <c r="A47" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="20" t="s">
         <v>206</v>
       </c>
-      <c r="C47" s="27">
+      <c r="C47" s="18">
         <v>23</v>
       </c>
       <c r="D47" s="6" t="s">
@@ -2810,9 +2810,9 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="26"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="27"/>
+      <c r="A48" s="16"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="18"/>
       <c r="D48" s="6" t="s">
         <v>111</v>
       </c>
@@ -2833,9 +2833,9 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="26"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="27">
+      <c r="A49" s="16"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="18">
         <v>24</v>
       </c>
       <c r="D49" s="6" t="s">
@@ -2858,9 +2858,9 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="26"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="27"/>
+      <c r="A50" s="16"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="18"/>
       <c r="D50" s="6" t="s">
         <v>115</v>
       </c>
@@ -2881,13 +2881,13 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="26" t="s">
+      <c r="A51" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="B51" s="25" t="s">
+      <c r="B51" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="C51" s="27">
+      <c r="C51" s="18">
         <v>25</v>
       </c>
       <c r="D51" s="6" t="s">
@@ -2910,9 +2910,9 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="26"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="27"/>
+      <c r="A52" s="16"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="18"/>
       <c r="D52" s="6" t="s">
         <v>120</v>
       </c>
@@ -2933,13 +2933,13 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="26" t="s">
+      <c r="A53" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B53" s="25" t="s">
+      <c r="B53" s="20" t="s">
         <v>208</v>
       </c>
-      <c r="C53" s="27">
+      <c r="C53" s="18">
         <v>26</v>
       </c>
       <c r="D53" s="6" t="s">
@@ -2962,9 +2962,9 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="26"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="27"/>
+      <c r="A54" s="16"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="18"/>
       <c r="D54" s="6" t="s">
         <v>125</v>
       </c>
@@ -2985,9 +2985,9 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="26"/>
-      <c r="B55" s="25"/>
-      <c r="C55" s="27">
+      <c r="A55" s="16"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="18">
         <v>27</v>
       </c>
       <c r="D55" s="6" t="s">
@@ -3010,9 +3010,9 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="26"/>
-      <c r="B56" s="25"/>
-      <c r="C56" s="27"/>
+      <c r="A56" s="16"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="18"/>
       <c r="D56" s="13" t="s">
         <v>129</v>
       </c>
@@ -3033,13 +3033,13 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="26" t="s">
+      <c r="A57" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="B57" s="25" t="s">
+      <c r="B57" s="20" t="s">
         <v>209</v>
       </c>
-      <c r="C57" s="27">
+      <c r="C57" s="18">
         <v>28</v>
       </c>
       <c r="D57" s="6" t="s">
@@ -3062,9 +3062,9 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="26"/>
-      <c r="B58" s="25"/>
-      <c r="C58" s="27"/>
+      <c r="A58" s="16"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="18"/>
       <c r="D58" s="6" t="s">
         <v>134</v>
       </c>
@@ -3085,9 +3085,9 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="26"/>
-      <c r="B59" s="25"/>
-      <c r="C59" s="27">
+      <c r="A59" s="16"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="18">
         <v>29</v>
       </c>
       <c r="D59" s="6" t="s">
@@ -3110,9 +3110,9 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="26"/>
-      <c r="B60" s="25"/>
-      <c r="C60" s="27"/>
+      <c r="A60" s="16"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="18"/>
       <c r="D60" s="6" t="s">
         <v>138</v>
       </c>
@@ -3133,13 +3133,13 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="18" t="s">
+      <c r="A61" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="B61" s="25" t="s">
+      <c r="B61" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="C61" s="20">
+      <c r="C61" s="18">
         <v>30</v>
       </c>
       <c r="D61" s="6" t="s">
@@ -3162,28 +3162,32 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="18"/>
-      <c r="B62" s="25"/>
-      <c r="C62" s="20"/>
-      <c r="D62" s="1" t="s">
+      <c r="A62" s="16"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F62" s="1" t="s">
+      <c r="E62" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F62" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="G62" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
+      <c r="G62" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="H62" s="5">
+        <v>3</v>
+      </c>
+      <c r="I62" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="18"/>
-      <c r="B63" s="25"/>
-      <c r="C63" s="20">
+      <c r="A63" s="16"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="19">
         <v>31</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -3202,9 +3206,9 @@
       <c r="I63" s="4"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="18"/>
-      <c r="B64" s="25"/>
-      <c r="C64" s="20"/>
+      <c r="A64" s="16"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="19"/>
       <c r="D64" s="1" t="s">
         <v>147</v>
       </c>
@@ -3221,13 +3225,13 @@
       <c r="I64" s="4"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="18" t="s">
+      <c r="A65" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="B65" s="24" t="s">
+      <c r="B65" s="21" t="s">
         <v>210</v>
       </c>
-      <c r="C65" s="20">
+      <c r="C65" s="19">
         <v>32</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -3246,9 +3250,9 @@
       <c r="I65" s="4"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="18"/>
-      <c r="B66" s="24"/>
-      <c r="C66" s="20"/>
+      <c r="A66" s="17"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="19"/>
       <c r="D66" s="1" t="s">
         <v>152</v>
       </c>
@@ -3265,9 +3269,9 @@
       <c r="I66" s="4"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="18"/>
-      <c r="B67" s="24"/>
-      <c r="C67" s="20">
+      <c r="A67" s="17"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="19">
         <v>33</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -3286,9 +3290,9 @@
       <c r="I67" s="4"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="18"/>
-      <c r="B68" s="24"/>
-      <c r="C68" s="20"/>
+      <c r="A68" s="17"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="19"/>
       <c r="D68" s="1" t="s">
         <v>156</v>
       </c>
@@ -3305,13 +3309,13 @@
       <c r="I68" s="4"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="18" t="s">
+      <c r="A69" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="B69" s="24" t="s">
+      <c r="B69" s="21" t="s">
         <v>211</v>
       </c>
-      <c r="C69" s="20">
+      <c r="C69" s="19">
         <v>34</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -3330,9 +3334,9 @@
       <c r="I69" s="4"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="18"/>
-      <c r="B70" s="24"/>
-      <c r="C70" s="20"/>
+      <c r="A70" s="17"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="19"/>
       <c r="D70" s="1" t="s">
         <v>161</v>
       </c>
@@ -3349,13 +3353,13 @@
       <c r="I70" s="4"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="18" t="s">
+      <c r="A71" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="B71" s="24" t="s">
+      <c r="B71" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="C71" s="20">
+      <c r="C71" s="19">
         <v>35</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -3374,9 +3378,9 @@
       <c r="I71" s="4"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="18"/>
-      <c r="B72" s="24"/>
-      <c r="C72" s="20"/>
+      <c r="A72" s="17"/>
+      <c r="B72" s="21"/>
+      <c r="C72" s="19"/>
       <c r="D72" s="1" t="s">
         <v>166</v>
       </c>
@@ -3393,9 +3397,9 @@
       <c r="I72" s="4"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="18"/>
-      <c r="B73" s="24"/>
-      <c r="C73" s="20">
+      <c r="A73" s="17"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="19">
         <v>36</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -3414,9 +3418,9 @@
       <c r="I73" s="4"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="18"/>
-      <c r="B74" s="24"/>
-      <c r="C74" s="20"/>
+      <c r="A74" s="17"/>
+      <c r="B74" s="21"/>
+      <c r="C74" s="19"/>
       <c r="D74" s="1" t="s">
         <v>170</v>
       </c>
@@ -3433,13 +3437,13 @@
       <c r="I74" s="4"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="18" t="s">
+      <c r="A75" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="B75" s="24" t="s">
+      <c r="B75" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="C75" s="20">
+      <c r="C75" s="19">
         <v>37</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -3458,9 +3462,9 @@
       <c r="I75" s="4"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="18"/>
-      <c r="B76" s="24"/>
-      <c r="C76" s="20"/>
+      <c r="A76" s="17"/>
+      <c r="B76" s="21"/>
+      <c r="C76" s="19"/>
       <c r="D76" s="1" t="s">
         <v>175</v>
       </c>
@@ -3477,9 +3481,9 @@
       <c r="I76" s="4"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="18"/>
-      <c r="B77" s="24"/>
-      <c r="C77" s="20">
+      <c r="A77" s="17"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="19">
         <v>38</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -3498,9 +3502,9 @@
       <c r="I77" s="4"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="18"/>
-      <c r="B78" s="24"/>
-      <c r="C78" s="20"/>
+      <c r="A78" s="17"/>
+      <c r="B78" s="21"/>
+      <c r="C78" s="19"/>
       <c r="D78" s="1" t="s">
         <v>179</v>
       </c>
@@ -3517,13 +3521,13 @@
       <c r="I78" s="4"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="18" t="s">
+      <c r="A79" s="17" t="s">
         <v>181</v>
       </c>
-      <c r="B79" s="24" t="s">
+      <c r="B79" s="21" t="s">
         <v>214</v>
       </c>
-      <c r="C79" s="20">
+      <c r="C79" s="19">
         <v>39</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -3542,9 +3546,9 @@
       <c r="I79" s="4"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="18"/>
-      <c r="B80" s="24"/>
-      <c r="C80" s="20"/>
+      <c r="A80" s="17"/>
+      <c r="B80" s="21"/>
+      <c r="C80" s="19"/>
       <c r="D80" s="1" t="s">
         <v>184</v>
       </c>
@@ -3561,13 +3565,13 @@
       <c r="I80" s="4"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="18" t="s">
+      <c r="A81" s="17" t="s">
         <v>186</v>
       </c>
-      <c r="B81" s="24" t="s">
+      <c r="B81" s="21" t="s">
         <v>215</v>
       </c>
-      <c r="C81" s="20">
+      <c r="C81" s="19">
         <v>40</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -3586,9 +3590,9 @@
       <c r="I81" s="4"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="18"/>
-      <c r="B82" s="24"/>
-      <c r="C82" s="20"/>
+      <c r="A82" s="17"/>
+      <c r="B82" s="21"/>
+      <c r="C82" s="19"/>
       <c r="D82" s="1" t="s">
         <v>189</v>
       </c>
@@ -3605,13 +3609,13 @@
       <c r="I82" s="4"/>
     </row>
     <row r="83" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="18" t="s">
+      <c r="A83" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="B83" s="21" t="s">
+      <c r="B83" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="C83" s="20">
+      <c r="C83" s="19">
         <v>41</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -3630,9 +3634,9 @@
       <c r="I83" s="4"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="18"/>
-      <c r="B84" s="22"/>
-      <c r="C84" s="20"/>
+      <c r="A84" s="17"/>
+      <c r="B84" s="26"/>
+      <c r="C84" s="19"/>
       <c r="D84" s="1" t="s">
         <v>194</v>
       </c>
@@ -3649,9 +3653,9 @@
       <c r="I84" s="4"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="18"/>
-      <c r="B85" s="22"/>
-      <c r="C85" s="20">
+      <c r="A85" s="17"/>
+      <c r="B85" s="26"/>
+      <c r="C85" s="19">
         <v>42</v>
       </c>
       <c r="D85" s="2" t="s">
@@ -3670,9 +3674,9 @@
       <c r="I85" s="4"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="18"/>
-      <c r="B86" s="23"/>
-      <c r="C86" s="20"/>
+      <c r="A86" s="17"/>
+      <c r="B86" s="27"/>
+      <c r="C86" s="19"/>
       <c r="D86" s="2" t="s">
         <v>220</v>
       </c>
@@ -3689,13 +3693,13 @@
       <c r="I86" s="4"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="18" t="s">
+      <c r="A87" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="B87" s="24" t="s">
+      <c r="B87" s="21" t="s">
         <v>300</v>
       </c>
-      <c r="C87" s="20">
+      <c r="C87" s="19">
         <v>43</v>
       </c>
       <c r="D87" s="2" t="s">
@@ -3714,11 +3718,11 @@
       <c r="I87" s="4"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="18"/>
-      <c r="B88" s="19" t="s">
+      <c r="A88" s="17"/>
+      <c r="B88" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C88" s="20"/>
+      <c r="C88" s="19"/>
       <c r="D88" s="2" t="s">
         <v>225</v>
       </c>
@@ -3735,11 +3739,11 @@
       <c r="I88" s="4"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" s="18"/>
-      <c r="B89" s="19" t="s">
+      <c r="A89" s="17"/>
+      <c r="B89" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C89" s="20">
+      <c r="C89" s="19">
         <v>44</v>
       </c>
       <c r="D89" s="2" t="s">
@@ -3758,11 +3762,11 @@
       <c r="I89" s="4"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90" s="18"/>
-      <c r="B90" s="19" t="s">
+      <c r="A90" s="17"/>
+      <c r="B90" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C90" s="20"/>
+      <c r="C90" s="19"/>
       <c r="D90" s="2" t="s">
         <v>229</v>
       </c>
@@ -3779,13 +3783,13 @@
       <c r="I90" s="4"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91" s="18" t="s">
+      <c r="A91" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="B91" s="24" t="s">
+      <c r="B91" s="21" t="s">
         <v>301</v>
       </c>
-      <c r="C91" s="20">
+      <c r="C91" s="19">
         <v>45</v>
       </c>
       <c r="D91" s="2" t="s">
@@ -3804,11 +3808,11 @@
       <c r="I91" s="4"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A92" s="18"/>
-      <c r="B92" s="19" t="s">
+      <c r="A92" s="17"/>
+      <c r="B92" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C92" s="20"/>
+      <c r="C92" s="19"/>
       <c r="D92" s="2" t="s">
         <v>234</v>
       </c>
@@ -3825,11 +3829,11 @@
       <c r="I92" s="4"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" s="18"/>
-      <c r="B93" s="19" t="s">
+      <c r="A93" s="17"/>
+      <c r="B93" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C93" s="20">
+      <c r="C93" s="19">
         <v>46</v>
       </c>
       <c r="D93" s="2" t="s">
@@ -3848,11 +3852,11 @@
       <c r="I93" s="4"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94" s="18"/>
-      <c r="B94" s="19" t="s">
+      <c r="A94" s="17"/>
+      <c r="B94" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C94" s="20"/>
+      <c r="C94" s="19"/>
       <c r="D94" s="2" t="s">
         <v>238</v>
       </c>
@@ -3869,13 +3873,13 @@
       <c r="I94" s="4"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95" s="18" t="s">
+      <c r="A95" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="B95" s="24" t="s">
+      <c r="B95" s="21" t="s">
         <v>302</v>
       </c>
-      <c r="C95" s="20">
+      <c r="C95" s="19">
         <v>47</v>
       </c>
       <c r="D95" s="2" t="s">
@@ -3894,11 +3898,11 @@
       <c r="I95" s="4"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A96" s="18"/>
-      <c r="B96" s="19" t="s">
+      <c r="A96" s="17"/>
+      <c r="B96" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C96" s="20"/>
+      <c r="C96" s="19"/>
       <c r="D96" s="2" t="s">
         <v>243</v>
       </c>
@@ -3915,11 +3919,11 @@
       <c r="I96" s="4"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97" s="18"/>
-      <c r="B97" s="19" t="s">
+      <c r="A97" s="17"/>
+      <c r="B97" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C97" s="20">
+      <c r="C97" s="19">
         <v>48</v>
       </c>
       <c r="D97" s="2" t="s">
@@ -3938,11 +3942,11 @@
       <c r="I97" s="4"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98" s="18"/>
-      <c r="B98" s="19" t="s">
+      <c r="A98" s="17"/>
+      <c r="B98" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C98" s="20"/>
+      <c r="C98" s="19"/>
       <c r="D98" s="2" t="s">
         <v>247</v>
       </c>
@@ -3959,13 +3963,13 @@
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" s="18" t="s">
+      <c r="A99" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="B99" s="24" t="s">
+      <c r="B99" s="21" t="s">
         <v>303</v>
       </c>
-      <c r="C99" s="20">
+      <c r="C99" s="19">
         <v>49</v>
       </c>
       <c r="D99" s="2" t="s">
@@ -3984,11 +3988,11 @@
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" s="18"/>
-      <c r="B100" s="19" t="s">
+      <c r="A100" s="17"/>
+      <c r="B100" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C100" s="20"/>
+      <c r="C100" s="19"/>
       <c r="D100" s="2" t="s">
         <v>252</v>
       </c>
@@ -4005,11 +4009,11 @@
       <c r="I100" s="4"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101" s="18"/>
-      <c r="B101" s="19" t="s">
+      <c r="A101" s="17"/>
+      <c r="B101" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C101" s="20">
+      <c r="C101" s="19">
         <v>50</v>
       </c>
       <c r="D101" s="2" t="s">
@@ -4028,11 +4032,11 @@
       <c r="I101" s="4"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A102" s="18"/>
-      <c r="B102" s="19" t="s">
+      <c r="A102" s="17"/>
+      <c r="B102" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C102" s="20"/>
+      <c r="C102" s="19"/>
       <c r="D102" s="2" t="s">
         <v>256</v>
       </c>
@@ -4049,13 +4053,13 @@
       <c r="I102" s="4"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A103" s="18" t="s">
+      <c r="A103" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="B103" s="24" t="s">
+      <c r="B103" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="C103" s="20">
+      <c r="C103" s="19">
         <v>51</v>
       </c>
       <c r="D103" s="2" t="s">
@@ -4074,11 +4078,11 @@
       <c r="I103" s="4"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" s="18"/>
-      <c r="B104" s="19" t="s">
+      <c r="A104" s="17"/>
+      <c r="B104" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C104" s="20"/>
+      <c r="C104" s="19"/>
       <c r="D104" s="2" t="s">
         <v>60</v>
       </c>
@@ -4095,13 +4099,13 @@
       <c r="I104" s="4"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A105" s="18" t="s">
+      <c r="A105" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="B105" s="19" t="s">
+      <c r="B105" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="C105" s="20">
+      <c r="C105" s="19">
         <v>52</v>
       </c>
       <c r="D105" s="2" t="s">
@@ -4120,11 +4124,11 @@
       <c r="I105" s="4"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A106" s="18"/>
-      <c r="B106" s="19" t="s">
+      <c r="A106" s="17"/>
+      <c r="B106" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C106" s="20"/>
+      <c r="C106" s="19"/>
       <c r="D106" s="2" t="s">
         <v>24</v>
       </c>
@@ -4141,11 +4145,11 @@
       <c r="I106" s="4"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A107" s="18"/>
-      <c r="B107" s="19" t="s">
+      <c r="A107" s="17"/>
+      <c r="B107" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C107" s="20">
+      <c r="C107" s="19">
         <v>53</v>
       </c>
       <c r="D107" s="2" t="s">
@@ -4164,11 +4168,11 @@
       <c r="I107" s="4"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A108" s="18"/>
-      <c r="B108" s="19" t="s">
+      <c r="A108" s="17"/>
+      <c r="B108" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C108" s="20"/>
+      <c r="C108" s="19"/>
       <c r="D108" s="2" t="s">
         <v>136</v>
       </c>
@@ -4185,13 +4189,13 @@
       <c r="I108" s="4"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" s="18" t="s">
+      <c r="A109" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="B109" s="24" t="s">
+      <c r="B109" s="21" t="s">
         <v>305</v>
       </c>
-      <c r="C109" s="20">
+      <c r="C109" s="19">
         <v>54</v>
       </c>
       <c r="D109" s="2" t="s">
@@ -4210,11 +4214,11 @@
       <c r="I109" s="4"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A110" s="18"/>
-      <c r="B110" s="19" t="s">
+      <c r="A110" s="17"/>
+      <c r="B110" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C110" s="20"/>
+      <c r="C110" s="19"/>
       <c r="D110" s="2" t="s">
         <v>268</v>
       </c>
@@ -4231,13 +4235,13 @@
       <c r="I110" s="4"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A111" s="18" t="s">
+      <c r="A111" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="B111" s="24" t="s">
+      <c r="B111" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="C111" s="20">
+      <c r="C111" s="19">
         <v>55</v>
       </c>
       <c r="D111" s="2" t="s">
@@ -4256,11 +4260,11 @@
       <c r="I111" s="4"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A112" s="18"/>
-      <c r="B112" s="19" t="s">
+      <c r="A112" s="17"/>
+      <c r="B112" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C112" s="20"/>
+      <c r="C112" s="19"/>
       <c r="D112" s="2" t="s">
         <v>273</v>
       </c>
@@ -4277,13 +4281,13 @@
       <c r="I112" s="4"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A113" s="18" t="s">
+      <c r="A113" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="B113" s="19" t="s">
+      <c r="B113" s="22" t="s">
         <v>276</v>
       </c>
-      <c r="C113" s="20">
+      <c r="C113" s="19">
         <v>56</v>
       </c>
       <c r="D113" s="2" t="s">
@@ -4302,11 +4306,11 @@
       <c r="I113" s="4"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A114" s="18"/>
-      <c r="B114" s="19" t="s">
+      <c r="A114" s="17"/>
+      <c r="B114" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C114" s="20"/>
+      <c r="C114" s="19"/>
       <c r="D114" s="2" t="s">
         <v>279</v>
       </c>
@@ -4323,11 +4327,11 @@
       <c r="I114" s="4"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A115" s="18"/>
-      <c r="B115" s="19" t="s">
+      <c r="A115" s="17"/>
+      <c r="B115" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C115" s="20">
+      <c r="C115" s="19">
         <v>57</v>
       </c>
       <c r="D115" s="2" t="s">
@@ -4346,11 +4350,11 @@
       <c r="I115" s="4"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A116" s="18"/>
-      <c r="B116" s="19" t="s">
+      <c r="A116" s="17"/>
+      <c r="B116" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C116" s="20"/>
+      <c r="C116" s="19"/>
       <c r="D116" s="2" t="s">
         <v>283</v>
       </c>
@@ -4367,13 +4371,13 @@
       <c r="I116" s="4"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A117" s="18" t="s">
+      <c r="A117" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="B117" s="19" t="s">
+      <c r="B117" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="C117" s="20">
+      <c r="C117" s="19">
         <v>58</v>
       </c>
       <c r="D117" s="2" t="s">
@@ -4392,11 +4396,11 @@
       <c r="I117" s="4"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A118" s="18"/>
-      <c r="B118" s="19" t="s">
+      <c r="A118" s="17"/>
+      <c r="B118" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C118" s="20"/>
+      <c r="C118" s="19"/>
       <c r="D118" s="2" t="s">
         <v>289</v>
       </c>
@@ -4413,11 +4417,11 @@
       <c r="I118" s="4"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A119" s="18"/>
-      <c r="B119" s="19" t="s">
+      <c r="A119" s="17"/>
+      <c r="B119" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C119" s="20">
+      <c r="C119" s="19">
         <v>59</v>
       </c>
       <c r="D119" s="2" t="s">
@@ -4436,11 +4440,11 @@
       <c r="I119" s="4"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A120" s="18"/>
-      <c r="B120" s="19" t="s">
+      <c r="A120" s="17"/>
+      <c r="B120" s="22" t="s">
         <v>219</v>
       </c>
-      <c r="C120" s="20"/>
+      <c r="C120" s="19"/>
       <c r="D120" s="2" t="s">
         <v>291</v>
       </c>
@@ -4457,13 +4461,13 @@
       <c r="I120" s="4"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" s="18" t="s">
+      <c r="A121" s="17" t="s">
         <v>293</v>
       </c>
-      <c r="B121" s="19" t="s">
+      <c r="B121" s="22" t="s">
         <v>294</v>
       </c>
-      <c r="C121" s="20">
+      <c r="C121" s="19">
         <v>60</v>
       </c>
       <c r="D121" s="2" t="s">
@@ -4482,9 +4486,9 @@
       <c r="I121" s="4"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A122" s="18"/>
-      <c r="B122" s="19"/>
-      <c r="C122" s="20"/>
+      <c r="A122" s="17"/>
+      <c r="B122" s="22"/>
+      <c r="C122" s="19"/>
       <c r="D122" s="2" t="s">
         <v>297</v>
       </c>
@@ -4501,9 +4505,9 @@
       <c r="I122" s="4"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A123" s="18"/>
-      <c r="B123" s="19"/>
-      <c r="C123" s="20">
+      <c r="A123" s="17"/>
+      <c r="B123" s="22"/>
+      <c r="C123" s="19">
         <v>61</v>
       </c>
       <c r="D123" s="2" t="s">
@@ -4522,9 +4526,9 @@
       <c r="I123" s="4"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A124" s="18"/>
-      <c r="B124" s="19"/>
-      <c r="C124" s="20"/>
+      <c r="A124" s="17"/>
+      <c r="B124" s="22"/>
+      <c r="C124" s="19"/>
       <c r="D124" s="2" t="s">
         <v>309</v>
       </c>
@@ -4541,9 +4545,9 @@
       <c r="I124" s="4"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A125" s="18"/>
-      <c r="B125" s="19"/>
-      <c r="C125" s="20">
+      <c r="A125" s="17"/>
+      <c r="B125" s="22"/>
+      <c r="C125" s="19">
         <v>62</v>
       </c>
       <c r="D125" s="2" t="s">
@@ -4562,9 +4566,9 @@
       <c r="I125" s="4"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A126" s="18"/>
-      <c r="B126" s="19"/>
-      <c r="C126" s="20"/>
+      <c r="A126" s="17"/>
+      <c r="B126" s="22"/>
+      <c r="C126" s="19"/>
       <c r="D126" s="2" t="s">
         <v>313</v>
       </c>
@@ -4582,15 +4586,114 @@
     </row>
   </sheetData>
   <mergeCells count="141">
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A121:A126"/>
+    <mergeCell ref="B121:B126"/>
+    <mergeCell ref="C121:C122"/>
+    <mergeCell ref="C123:C124"/>
+    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C115:C116"/>
+    <mergeCell ref="C117:C118"/>
+    <mergeCell ref="C119:C120"/>
+    <mergeCell ref="B83:B86"/>
+    <mergeCell ref="C105:C106"/>
+    <mergeCell ref="C107:C108"/>
+    <mergeCell ref="C109:C110"/>
+    <mergeCell ref="C111:C112"/>
+    <mergeCell ref="C113:C114"/>
+    <mergeCell ref="C95:C96"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="C101:C102"/>
+    <mergeCell ref="C103:C104"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="C93:C94"/>
+    <mergeCell ref="A117:A120"/>
+    <mergeCell ref="B87:B90"/>
+    <mergeCell ref="B91:B94"/>
+    <mergeCell ref="B95:B98"/>
+    <mergeCell ref="B99:B102"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="B111:B112"/>
+    <mergeCell ref="B113:B116"/>
+    <mergeCell ref="B117:B120"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A113:A116"/>
+    <mergeCell ref="A83:A86"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="A91:A94"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="A99:A102"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="C83:C84"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C47:C48"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C19:C20"/>
@@ -4615,114 +4718,15 @@
     <mergeCell ref="A71:A74"/>
     <mergeCell ref="A61:A64"/>
     <mergeCell ref="A65:A68"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="C83:C84"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="A83:A86"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="A91:A94"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="A99:A102"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B71:B74"/>
-    <mergeCell ref="B75:B78"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A117:A120"/>
-    <mergeCell ref="B87:B90"/>
-    <mergeCell ref="B91:B94"/>
-    <mergeCell ref="B95:B98"/>
-    <mergeCell ref="B99:B102"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="B109:B110"/>
-    <mergeCell ref="B111:B112"/>
-    <mergeCell ref="B113:B116"/>
-    <mergeCell ref="B117:B120"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A113:A116"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="C103:C104"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="A121:A126"/>
-    <mergeCell ref="B121:B126"/>
-    <mergeCell ref="C121:C122"/>
-    <mergeCell ref="C123:C124"/>
-    <mergeCell ref="C125:C126"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C115:C116"/>
-    <mergeCell ref="C117:C118"/>
-    <mergeCell ref="C119:C120"/>
-    <mergeCell ref="B83:B86"/>
-    <mergeCell ref="C105:C106"/>
-    <mergeCell ref="C107:C108"/>
-    <mergeCell ref="C109:C110"/>
-    <mergeCell ref="C111:C112"/>
-    <mergeCell ref="C113:C114"/>
-    <mergeCell ref="C95:C96"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A51:A52"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G126" xr:uid="{BD7D4049-E182-46D9-ABFE-ED680993C7C2}">
@@ -4789,9 +4793,10 @@
     <hyperlink ref="F59" r:id="rId57" xr:uid="{7FF47B51-3E09-4769-9361-616326B362F0}"/>
     <hyperlink ref="F60" r:id="rId58" xr:uid="{9CECBBD6-2F14-4F88-B6F4-C08AF3014E4F}"/>
     <hyperlink ref="F61" r:id="rId59" xr:uid="{F9AF7E56-A77D-4520-87E8-16AD5AF5E883}"/>
+    <hyperlink ref="F62" r:id="rId60" xr:uid="{CD8C3D13-0D28-42DD-AC01-181A7BF0563D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId60"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId61"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
solve task '74. Search a 2D Matrix'
</commit_message>
<xml_diff>
--- a/DSA studing (in acc. with Claude plan)/DSA_Leetcode_plan from Claude.xlsx
+++ b/DSA studing (in acc. with Claude plan)/DSA_Leetcode_plan from Claude.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Programming\Python\Leetcode\Leetcode practise\DSA studing (in acc. with Claude plan)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08F16590-8C6E-4890-8F73-8CFE6200EE79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDD315D-E705-4367-9D5B-1C1160273198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1226,7 +1226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1271,32 +1271,20 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1306,6 +1294,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1596,8 +1599,8 @@
   <dimension ref="A1:L126"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F63" sqref="F63"/>
+      <pane ySplit="2" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1613,31 +1616,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="23" t="s">
+      <c r="B1" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="16" t="s">
         <v>315</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="16" t="s">
         <v>317</v>
       </c>
       <c r="J1" s="9" t="s">
@@ -1651,36 +1654,36 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
       <c r="J2" s="10">
         <f>COUNTIF(G3:G126,"решена")/124</f>
-        <v>0.46774193548387094</v>
+        <v>0.47580645161290325</v>
       </c>
       <c r="K2" s="11">
         <f>SUM(H3:H126)/(COUNTIF(G3:G126,"решена") + COUNTIF(G3:G126,"не решена"))</f>
-        <v>2.35</v>
+        <v>2.377049180327869</v>
       </c>
       <c r="L2" s="10">
         <f>SUM(I3:I126)/SUM(H3:H126)</f>
-        <v>0.73758865248226946</v>
+        <v>0.73793103448275865</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="27">
         <v>1</v>
       </c>
       <c r="D3" s="6" t="s">
@@ -1706,9 +1709,9 @@
       <c r="L3" s="7"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="16"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="18"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="6" t="s">
         <v>11</v>
       </c>
@@ -1729,9 +1732,9 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="16"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="18">
+      <c r="A5" s="26"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="27">
         <v>2</v>
       </c>
       <c r="D5" s="6" t="s">
@@ -1754,9 +1757,9 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="16"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="18"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="27"/>
       <c r="D6" s="6" t="s">
         <v>15</v>
       </c>
@@ -1777,13 +1780,13 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="25" t="s">
         <v>323</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="27">
         <v>3</v>
       </c>
       <c r="D7" s="6" t="s">
@@ -1806,9 +1809,9 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="16"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="18"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="6" t="s">
         <v>20</v>
       </c>
@@ -1829,9 +1832,9 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="18">
+      <c r="A9" s="26"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="27">
         <v>4</v>
       </c>
       <c r="D9" s="6" t="s">
@@ -1854,9 +1857,9 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="18"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="6" t="s">
         <v>24</v>
       </c>
@@ -1877,13 +1880,13 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="27">
         <v>5</v>
       </c>
       <c r="D11" s="6" t="s">
@@ -1906,9 +1909,9 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="16"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="18"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="27"/>
       <c r="D12" s="6" t="s">
         <v>29</v>
       </c>
@@ -1929,9 +1932,9 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="16"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="18">
+      <c r="A13" s="26"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="27">
         <v>6</v>
       </c>
       <c r="D13" s="6" t="s">
@@ -1954,9 +1957,9 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="18"/>
+      <c r="A14" s="26"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="27"/>
       <c r="D14" s="6" t="s">
         <v>33</v>
       </c>
@@ -1977,13 +1980,13 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="27">
         <v>7</v>
       </c>
       <c r="D15" s="6" t="s">
@@ -2006,9 +2009,9 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="18"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="27"/>
       <c r="D16" s="6" t="s">
         <v>38</v>
       </c>
@@ -2029,9 +2032,9 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="18">
+      <c r="A17" s="18"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="27">
         <v>8</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -2054,9 +2057,9 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="18"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="27"/>
       <c r="D18" s="6" t="s">
         <v>42</v>
       </c>
@@ -2077,13 +2080,13 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="24" t="s">
         <v>199</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="27">
         <v>9</v>
       </c>
       <c r="D19" s="6" t="s">
@@ -2106,9 +2109,9 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="18"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="6" t="s">
         <v>47</v>
       </c>
@@ -2129,9 +2132,9 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="17"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="18">
+      <c r="A21" s="18"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="27">
         <v>10</v>
       </c>
       <c r="D21" s="6" t="s">
@@ -2154,9 +2157,9 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="18"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="27"/>
       <c r="D22" s="13" t="s">
         <v>51</v>
       </c>
@@ -2177,13 +2180,13 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="27">
         <v>11</v>
       </c>
       <c r="D23" s="6" t="s">
@@ -2206,9 +2209,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="18"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="27"/>
       <c r="D24" s="6" t="s">
         <v>56</v>
       </c>
@@ -2229,9 +2232,9 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="17"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="18">
+      <c r="A25" s="18"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="27">
         <v>12</v>
       </c>
       <c r="D25" s="6" t="s">
@@ -2254,9 +2257,9 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="18"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="27"/>
       <c r="D26" s="6" t="s">
         <v>60</v>
       </c>
@@ -2277,13 +2280,13 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C27" s="27">
         <v>13</v>
       </c>
       <c r="D27" s="6" t="s">
@@ -2306,9 +2309,9 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="16"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="18"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="6" t="s">
         <v>65</v>
       </c>
@@ -2329,9 +2332,9 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="16"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="18">
+      <c r="A29" s="26"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="27">
         <v>14</v>
       </c>
       <c r="D29" s="6" t="s">
@@ -2354,9 +2357,9 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="16"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="18"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="27"/>
       <c r="D30" s="6" t="s">
         <v>69</v>
       </c>
@@ -2377,13 +2380,13 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="16" t="s">
+      <c r="A31" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="C31" s="18">
+      <c r="C31" s="27">
         <v>15</v>
       </c>
       <c r="D31" s="6" t="s">
@@ -2406,9 +2409,9 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="16"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="18"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="27"/>
       <c r="D32" s="6" t="s">
         <v>74</v>
       </c>
@@ -2429,9 +2432,9 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="16"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="18">
+      <c r="A33" s="26"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="27">
         <v>16</v>
       </c>
       <c r="D33" s="6" t="s">
@@ -2454,9 +2457,9 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="16"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="18"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="6" t="s">
         <v>78</v>
       </c>
@@ -2477,13 +2480,13 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="C35" s="18">
+      <c r="C35" s="27">
         <v>17</v>
       </c>
       <c r="D35" s="6" t="s">
@@ -2506,9 +2509,9 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="16"/>
-      <c r="B36" s="20"/>
-      <c r="C36" s="18"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="27"/>
       <c r="D36" s="6" t="s">
         <v>83</v>
       </c>
@@ -2529,13 +2532,13 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="25" t="s">
         <v>203</v>
       </c>
-      <c r="C37" s="18">
+      <c r="C37" s="27">
         <v>18</v>
       </c>
       <c r="D37" s="6" t="s">
@@ -2558,9 +2561,9 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="16"/>
-      <c r="B38" s="20"/>
-      <c r="C38" s="18"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="27"/>
       <c r="D38" s="6" t="s">
         <v>88</v>
       </c>
@@ -2581,9 +2584,9 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="16"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="18">
+      <c r="A39" s="26"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="27">
         <v>19</v>
       </c>
       <c r="D39" s="6" t="s">
@@ -2606,9 +2609,9 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="16"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="18"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="27"/>
       <c r="D40" s="6" t="s">
         <v>92</v>
       </c>
@@ -2629,13 +2632,13 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="25" t="s">
         <v>204</v>
       </c>
-      <c r="C41" s="18">
+      <c r="C41" s="27">
         <v>20</v>
       </c>
       <c r="D41" s="6" t="s">
@@ -2658,9 +2661,9 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="16"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="18"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="27"/>
       <c r="D42" s="6" t="s">
         <v>97</v>
       </c>
@@ -2681,9 +2684,9 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="16"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="18">
+      <c r="A43" s="26"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="27">
         <v>21</v>
       </c>
       <c r="D43" s="6" t="s">
@@ -2706,9 +2709,9 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="16"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="18"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="27"/>
       <c r="D44" s="6" t="s">
         <v>101</v>
       </c>
@@ -2729,13 +2732,13 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B45" s="20" t="s">
+      <c r="B45" s="25" t="s">
         <v>205</v>
       </c>
-      <c r="C45" s="18">
+      <c r="C45" s="27">
         <v>22</v>
       </c>
       <c r="D45" s="6" t="s">
@@ -2758,9 +2761,9 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="16"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="18"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="27"/>
       <c r="D46" s="6" t="s">
         <v>106</v>
       </c>
@@ -2781,13 +2784,13 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="16" t="s">
+      <c r="A47" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="C47" s="18">
+      <c r="C47" s="27">
         <v>23</v>
       </c>
       <c r="D47" s="6" t="s">
@@ -2810,9 +2813,9 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="16"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="18"/>
+      <c r="A48" s="26"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="27"/>
       <c r="D48" s="6" t="s">
         <v>111</v>
       </c>
@@ -2833,9 +2836,9 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="16"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="18">
+      <c r="A49" s="26"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="27">
         <v>24</v>
       </c>
       <c r="D49" s="6" t="s">
@@ -2858,9 +2861,9 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="16"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="18"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="27"/>
       <c r="D50" s="6" t="s">
         <v>115</v>
       </c>
@@ -2881,13 +2884,13 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="B51" s="25" t="s">
         <v>207</v>
       </c>
-      <c r="C51" s="18">
+      <c r="C51" s="27">
         <v>25</v>
       </c>
       <c r="D51" s="6" t="s">
@@ -2910,9 +2913,9 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="16"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="18"/>
+      <c r="A52" s="26"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="27"/>
       <c r="D52" s="6" t="s">
         <v>120</v>
       </c>
@@ -2933,13 +2936,13 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="16" t="s">
+      <c r="A53" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="C53" s="18">
+      <c r="C53" s="27">
         <v>26</v>
       </c>
       <c r="D53" s="6" t="s">
@@ -2962,9 +2965,9 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="16"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="18"/>
+      <c r="A54" s="26"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="27"/>
       <c r="D54" s="6" t="s">
         <v>125</v>
       </c>
@@ -2985,9 +2988,9 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="16"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="18">
+      <c r="A55" s="26"/>
+      <c r="B55" s="25"/>
+      <c r="C55" s="27">
         <v>27</v>
       </c>
       <c r="D55" s="6" t="s">
@@ -3010,9 +3013,9 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="16"/>
-      <c r="B56" s="20"/>
-      <c r="C56" s="18"/>
+      <c r="A56" s="26"/>
+      <c r="B56" s="25"/>
+      <c r="C56" s="27"/>
       <c r="D56" s="13" t="s">
         <v>129</v>
       </c>
@@ -3033,13 +3036,13 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="16" t="s">
+      <c r="A57" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="B57" s="20" t="s">
+      <c r="B57" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="C57" s="18">
+      <c r="C57" s="27">
         <v>28</v>
       </c>
       <c r="D57" s="6" t="s">
@@ -3062,9 +3065,9 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="16"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="18"/>
+      <c r="A58" s="26"/>
+      <c r="B58" s="25"/>
+      <c r="C58" s="27"/>
       <c r="D58" s="6" t="s">
         <v>134</v>
       </c>
@@ -3085,9 +3088,9 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="16"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="18">
+      <c r="A59" s="26"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="27">
         <v>29</v>
       </c>
       <c r="D59" s="6" t="s">
@@ -3110,9 +3113,9 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="16"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="18"/>
+      <c r="A60" s="26"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="27"/>
       <c r="D60" s="6" t="s">
         <v>138</v>
       </c>
@@ -3133,13 +3136,13 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="16" t="s">
+      <c r="A61" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="25" t="s">
         <v>325</v>
       </c>
-      <c r="C61" s="18">
+      <c r="C61" s="27">
         <v>30</v>
       </c>
       <c r="D61" s="6" t="s">
@@ -3162,9 +3165,9 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="16"/>
-      <c r="B62" s="20"/>
-      <c r="C62" s="18"/>
+      <c r="A62" s="26"/>
+      <c r="B62" s="25"/>
+      <c r="C62" s="27"/>
       <c r="D62" s="6" t="s">
         <v>143</v>
       </c>
@@ -3185,37 +3188,41 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="16"/>
-      <c r="B63" s="20"/>
-      <c r="C63" s="19">
+      <c r="A63" s="26"/>
+      <c r="B63" s="25"/>
+      <c r="C63" s="20">
         <v>31</v>
       </c>
-      <c r="D63" s="1" t="s">
+      <c r="D63" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="E63" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F63" s="1" t="s">
+      <c r="E63" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F63" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="G63" s="4" t="s">
-        <v>319</v>
-      </c>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
+      <c r="G63" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="H63" s="5">
+        <v>4</v>
+      </c>
+      <c r="I63" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="16"/>
-      <c r="B64" s="20"/>
-      <c r="C64" s="19"/>
+      <c r="A64" s="26"/>
+      <c r="B64" s="25"/>
+      <c r="C64" s="20"/>
       <c r="D64" s="1" t="s">
         <v>147</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F64" s="1" t="s">
+      <c r="F64" s="28" t="s">
         <v>148</v>
       </c>
       <c r="G64" s="4" t="s">
@@ -3225,13 +3232,13 @@
       <c r="I64" s="4"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="17" t="s">
+      <c r="A65" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="B65" s="21" t="s">
+      <c r="B65" s="24" t="s">
         <v>210</v>
       </c>
-      <c r="C65" s="19">
+      <c r="C65" s="20">
         <v>32</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -3250,9 +3257,9 @@
       <c r="I65" s="4"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="17"/>
-      <c r="B66" s="21"/>
-      <c r="C66" s="19"/>
+      <c r="A66" s="18"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="20"/>
       <c r="D66" s="1" t="s">
         <v>152</v>
       </c>
@@ -3269,9 +3276,9 @@
       <c r="I66" s="4"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="17"/>
-      <c r="B67" s="21"/>
-      <c r="C67" s="19">
+      <c r="A67" s="18"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="20">
         <v>33</v>
       </c>
       <c r="D67" s="1" t="s">
@@ -3290,9 +3297,9 @@
       <c r="I67" s="4"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="17"/>
-      <c r="B68" s="21"/>
-      <c r="C68" s="19"/>
+      <c r="A68" s="18"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="20"/>
       <c r="D68" s="1" t="s">
         <v>156</v>
       </c>
@@ -3309,13 +3316,13 @@
       <c r="I68" s="4"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="17" t="s">
+      <c r="A69" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="B69" s="21" t="s">
+      <c r="B69" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="C69" s="19">
+      <c r="C69" s="20">
         <v>34</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -3334,9 +3341,9 @@
       <c r="I69" s="4"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="17"/>
-      <c r="B70" s="21"/>
-      <c r="C70" s="19"/>
+      <c r="A70" s="18"/>
+      <c r="B70" s="24"/>
+      <c r="C70" s="20"/>
       <c r="D70" s="1" t="s">
         <v>161</v>
       </c>
@@ -3353,13 +3360,13 @@
       <c r="I70" s="4"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="17" t="s">
+      <c r="A71" s="18" t="s">
         <v>163</v>
       </c>
-      <c r="B71" s="21" t="s">
+      <c r="B71" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="C71" s="19">
+      <c r="C71" s="20">
         <v>35</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -3378,9 +3385,9 @@
       <c r="I71" s="4"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="17"/>
-      <c r="B72" s="21"/>
-      <c r="C72" s="19"/>
+      <c r="A72" s="18"/>
+      <c r="B72" s="24"/>
+      <c r="C72" s="20"/>
       <c r="D72" s="1" t="s">
         <v>166</v>
       </c>
@@ -3397,9 +3404,9 @@
       <c r="I72" s="4"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="17"/>
-      <c r="B73" s="21"/>
-      <c r="C73" s="19">
+      <c r="A73" s="18"/>
+      <c r="B73" s="24"/>
+      <c r="C73" s="20">
         <v>36</v>
       </c>
       <c r="D73" s="1" t="s">
@@ -3418,9 +3425,9 @@
       <c r="I73" s="4"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="17"/>
-      <c r="B74" s="21"/>
-      <c r="C74" s="19"/>
+      <c r="A74" s="18"/>
+      <c r="B74" s="24"/>
+      <c r="C74" s="20"/>
       <c r="D74" s="1" t="s">
         <v>170</v>
       </c>
@@ -3437,13 +3444,13 @@
       <c r="I74" s="4"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="17" t="s">
+      <c r="A75" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="B75" s="21" t="s">
+      <c r="B75" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="C75" s="19">
+      <c r="C75" s="20">
         <v>37</v>
       </c>
       <c r="D75" s="1" t="s">
@@ -3462,9 +3469,9 @@
       <c r="I75" s="4"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="17"/>
-      <c r="B76" s="21"/>
-      <c r="C76" s="19"/>
+      <c r="A76" s="18"/>
+      <c r="B76" s="24"/>
+      <c r="C76" s="20"/>
       <c r="D76" s="1" t="s">
         <v>175</v>
       </c>
@@ -3481,9 +3488,9 @@
       <c r="I76" s="4"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="17"/>
-      <c r="B77" s="21"/>
-      <c r="C77" s="19">
+      <c r="A77" s="18"/>
+      <c r="B77" s="24"/>
+      <c r="C77" s="20">
         <v>38</v>
       </c>
       <c r="D77" s="1" t="s">
@@ -3502,9 +3509,9 @@
       <c r="I77" s="4"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="17"/>
-      <c r="B78" s="21"/>
-      <c r="C78" s="19"/>
+      <c r="A78" s="18"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="20"/>
       <c r="D78" s="1" t="s">
         <v>179</v>
       </c>
@@ -3521,13 +3528,13 @@
       <c r="I78" s="4"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="17" t="s">
+      <c r="A79" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="B79" s="21" t="s">
+      <c r="B79" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="C79" s="19">
+      <c r="C79" s="20">
         <v>39</v>
       </c>
       <c r="D79" s="1" t="s">
@@ -3546,9 +3553,9 @@
       <c r="I79" s="4"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="17"/>
-      <c r="B80" s="21"/>
-      <c r="C80" s="19"/>
+      <c r="A80" s="18"/>
+      <c r="B80" s="24"/>
+      <c r="C80" s="20"/>
       <c r="D80" s="1" t="s">
         <v>184</v>
       </c>
@@ -3565,13 +3572,13 @@
       <c r="I80" s="4"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="17" t="s">
+      <c r="A81" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="B81" s="21" t="s">
+      <c r="B81" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="C81" s="19">
+      <c r="C81" s="20">
         <v>40</v>
       </c>
       <c r="D81" s="1" t="s">
@@ -3590,9 +3597,9 @@
       <c r="I81" s="4"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="17"/>
-      <c r="B82" s="21"/>
-      <c r="C82" s="19"/>
+      <c r="A82" s="18"/>
+      <c r="B82" s="24"/>
+      <c r="C82" s="20"/>
       <c r="D82" s="1" t="s">
         <v>189</v>
       </c>
@@ -3609,13 +3616,13 @@
       <c r="I82" s="4"/>
     </row>
     <row r="83" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="17" t="s">
+      <c r="A83" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="B83" s="25" t="s">
+      <c r="B83" s="21" t="s">
         <v>216</v>
       </c>
-      <c r="C83" s="19">
+      <c r="C83" s="20">
         <v>41</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -3634,9 +3641,9 @@
       <c r="I83" s="4"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="17"/>
-      <c r="B84" s="26"/>
-      <c r="C84" s="19"/>
+      <c r="A84" s="18"/>
+      <c r="B84" s="22"/>
+      <c r="C84" s="20"/>
       <c r="D84" s="1" t="s">
         <v>194</v>
       </c>
@@ -3653,9 +3660,9 @@
       <c r="I84" s="4"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="17"/>
-      <c r="B85" s="26"/>
-      <c r="C85" s="19">
+      <c r="A85" s="18"/>
+      <c r="B85" s="22"/>
+      <c r="C85" s="20">
         <v>42</v>
       </c>
       <c r="D85" s="2" t="s">
@@ -3674,9 +3681,9 @@
       <c r="I85" s="4"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="17"/>
-      <c r="B86" s="27"/>
-      <c r="C86" s="19"/>
+      <c r="A86" s="18"/>
+      <c r="B86" s="23"/>
+      <c r="C86" s="20"/>
       <c r="D86" s="2" t="s">
         <v>220</v>
       </c>
@@ -3693,13 +3700,13 @@
       <c r="I86" s="4"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="17" t="s">
+      <c r="A87" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="B87" s="21" t="s">
+      <c r="B87" s="24" t="s">
         <v>300</v>
       </c>
-      <c r="C87" s="19">
+      <c r="C87" s="20">
         <v>43</v>
       </c>
       <c r="D87" s="2" t="s">
@@ -3718,11 +3725,11 @@
       <c r="I87" s="4"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="17"/>
-      <c r="B88" s="22" t="s">
+      <c r="A88" s="18"/>
+      <c r="B88" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C88" s="19"/>
+      <c r="C88" s="20"/>
       <c r="D88" s="2" t="s">
         <v>225</v>
       </c>
@@ -3739,11 +3746,11 @@
       <c r="I88" s="4"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" s="17"/>
-      <c r="B89" s="22" t="s">
+      <c r="A89" s="18"/>
+      <c r="B89" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C89" s="19">
+      <c r="C89" s="20">
         <v>44</v>
       </c>
       <c r="D89" s="2" t="s">
@@ -3762,11 +3769,11 @@
       <c r="I89" s="4"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90" s="17"/>
-      <c r="B90" s="22" t="s">
+      <c r="A90" s="18"/>
+      <c r="B90" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C90" s="19"/>
+      <c r="C90" s="20"/>
       <c r="D90" s="2" t="s">
         <v>229</v>
       </c>
@@ -3783,13 +3790,13 @@
       <c r="I90" s="4"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91" s="17" t="s">
+      <c r="A91" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="B91" s="21" t="s">
+      <c r="B91" s="24" t="s">
         <v>301</v>
       </c>
-      <c r="C91" s="19">
+      <c r="C91" s="20">
         <v>45</v>
       </c>
       <c r="D91" s="2" t="s">
@@ -3808,11 +3815,11 @@
       <c r="I91" s="4"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A92" s="17"/>
-      <c r="B92" s="22" t="s">
+      <c r="A92" s="18"/>
+      <c r="B92" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C92" s="19"/>
+      <c r="C92" s="20"/>
       <c r="D92" s="2" t="s">
         <v>234</v>
       </c>
@@ -3829,11 +3836,11 @@
       <c r="I92" s="4"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" s="17"/>
-      <c r="B93" s="22" t="s">
+      <c r="A93" s="18"/>
+      <c r="B93" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C93" s="19">
+      <c r="C93" s="20">
         <v>46</v>
       </c>
       <c r="D93" s="2" t="s">
@@ -3852,11 +3859,11 @@
       <c r="I93" s="4"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94" s="17"/>
-      <c r="B94" s="22" t="s">
+      <c r="A94" s="18"/>
+      <c r="B94" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C94" s="19"/>
+      <c r="C94" s="20"/>
       <c r="D94" s="2" t="s">
         <v>238</v>
       </c>
@@ -3873,13 +3880,13 @@
       <c r="I94" s="4"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95" s="17" t="s">
+      <c r="A95" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="B95" s="21" t="s">
+      <c r="B95" s="24" t="s">
         <v>302</v>
       </c>
-      <c r="C95" s="19">
+      <c r="C95" s="20">
         <v>47</v>
       </c>
       <c r="D95" s="2" t="s">
@@ -3898,11 +3905,11 @@
       <c r="I95" s="4"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A96" s="17"/>
-      <c r="B96" s="22" t="s">
+      <c r="A96" s="18"/>
+      <c r="B96" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C96" s="19"/>
+      <c r="C96" s="20"/>
       <c r="D96" s="2" t="s">
         <v>243</v>
       </c>
@@ -3919,11 +3926,11 @@
       <c r="I96" s="4"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97" s="17"/>
-      <c r="B97" s="22" t="s">
+      <c r="A97" s="18"/>
+      <c r="B97" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C97" s="19">
+      <c r="C97" s="20">
         <v>48</v>
       </c>
       <c r="D97" s="2" t="s">
@@ -3942,11 +3949,11 @@
       <c r="I97" s="4"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98" s="17"/>
-      <c r="B98" s="22" t="s">
+      <c r="A98" s="18"/>
+      <c r="B98" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C98" s="19"/>
+      <c r="C98" s="20"/>
       <c r="D98" s="2" t="s">
         <v>247</v>
       </c>
@@ -3963,13 +3970,13 @@
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" s="17" t="s">
+      <c r="A99" s="18" t="s">
         <v>249</v>
       </c>
-      <c r="B99" s="21" t="s">
+      <c r="B99" s="24" t="s">
         <v>303</v>
       </c>
-      <c r="C99" s="19">
+      <c r="C99" s="20">
         <v>49</v>
       </c>
       <c r="D99" s="2" t="s">
@@ -3988,11 +3995,11 @@
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" s="17"/>
-      <c r="B100" s="22" t="s">
+      <c r="A100" s="18"/>
+      <c r="B100" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C100" s="19"/>
+      <c r="C100" s="20"/>
       <c r="D100" s="2" t="s">
         <v>252</v>
       </c>
@@ -4009,11 +4016,11 @@
       <c r="I100" s="4"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101" s="17"/>
-      <c r="B101" s="22" t="s">
+      <c r="A101" s="18"/>
+      <c r="B101" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C101" s="19">
+      <c r="C101" s="20">
         <v>50</v>
       </c>
       <c r="D101" s="2" t="s">
@@ -4032,11 +4039,11 @@
       <c r="I101" s="4"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A102" s="17"/>
-      <c r="B102" s="22" t="s">
+      <c r="A102" s="18"/>
+      <c r="B102" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C102" s="19"/>
+      <c r="C102" s="20"/>
       <c r="D102" s="2" t="s">
         <v>256</v>
       </c>
@@ -4053,13 +4060,13 @@
       <c r="I102" s="4"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A103" s="17" t="s">
+      <c r="A103" s="18" t="s">
         <v>258</v>
       </c>
-      <c r="B103" s="21" t="s">
+      <c r="B103" s="24" t="s">
         <v>304</v>
       </c>
-      <c r="C103" s="19">
+      <c r="C103" s="20">
         <v>51</v>
       </c>
       <c r="D103" s="2" t="s">
@@ -4078,11 +4085,11 @@
       <c r="I103" s="4"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" s="17"/>
-      <c r="B104" s="22" t="s">
+      <c r="A104" s="18"/>
+      <c r="B104" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C104" s="19"/>
+      <c r="C104" s="20"/>
       <c r="D104" s="2" t="s">
         <v>60</v>
       </c>
@@ -4099,13 +4106,13 @@
       <c r="I104" s="4"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A105" s="17" t="s">
+      <c r="A105" s="18" t="s">
         <v>261</v>
       </c>
-      <c r="B105" s="22" t="s">
+      <c r="B105" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="C105" s="19">
+      <c r="C105" s="20">
         <v>52</v>
       </c>
       <c r="D105" s="2" t="s">
@@ -4124,11 +4131,11 @@
       <c r="I105" s="4"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A106" s="17"/>
-      <c r="B106" s="22" t="s">
+      <c r="A106" s="18"/>
+      <c r="B106" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C106" s="19"/>
+      <c r="C106" s="20"/>
       <c r="D106" s="2" t="s">
         <v>24</v>
       </c>
@@ -4145,11 +4152,11 @@
       <c r="I106" s="4"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A107" s="17"/>
-      <c r="B107" s="22" t="s">
+      <c r="A107" s="18"/>
+      <c r="B107" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C107" s="19">
+      <c r="C107" s="20">
         <v>53</v>
       </c>
       <c r="D107" s="2" t="s">
@@ -4168,11 +4175,11 @@
       <c r="I107" s="4"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A108" s="17"/>
-      <c r="B108" s="22" t="s">
+      <c r="A108" s="18"/>
+      <c r="B108" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C108" s="19"/>
+      <c r="C108" s="20"/>
       <c r="D108" s="2" t="s">
         <v>136</v>
       </c>
@@ -4189,13 +4196,13 @@
       <c r="I108" s="4"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" s="17" t="s">
+      <c r="A109" s="18" t="s">
         <v>265</v>
       </c>
-      <c r="B109" s="21" t="s">
+      <c r="B109" s="24" t="s">
         <v>305</v>
       </c>
-      <c r="C109" s="19">
+      <c r="C109" s="20">
         <v>54</v>
       </c>
       <c r="D109" s="2" t="s">
@@ -4214,11 +4221,11 @@
       <c r="I109" s="4"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A110" s="17"/>
-      <c r="B110" s="22" t="s">
+      <c r="A110" s="18"/>
+      <c r="B110" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C110" s="19"/>
+      <c r="C110" s="20"/>
       <c r="D110" s="2" t="s">
         <v>268</v>
       </c>
@@ -4235,13 +4242,13 @@
       <c r="I110" s="4"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A111" s="17" t="s">
+      <c r="A111" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="B111" s="21" t="s">
+      <c r="B111" s="24" t="s">
         <v>306</v>
       </c>
-      <c r="C111" s="19">
+      <c r="C111" s="20">
         <v>55</v>
       </c>
       <c r="D111" s="2" t="s">
@@ -4260,11 +4267,11 @@
       <c r="I111" s="4"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A112" s="17"/>
-      <c r="B112" s="22" t="s">
+      <c r="A112" s="18"/>
+      <c r="B112" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C112" s="19"/>
+      <c r="C112" s="20"/>
       <c r="D112" s="2" t="s">
         <v>273</v>
       </c>
@@ -4281,13 +4288,13 @@
       <c r="I112" s="4"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A113" s="17" t="s">
+      <c r="A113" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="B113" s="22" t="s">
+      <c r="B113" s="19" t="s">
         <v>276</v>
       </c>
-      <c r="C113" s="19">
+      <c r="C113" s="20">
         <v>56</v>
       </c>
       <c r="D113" s="2" t="s">
@@ -4306,11 +4313,11 @@
       <c r="I113" s="4"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A114" s="17"/>
-      <c r="B114" s="22" t="s">
+      <c r="A114" s="18"/>
+      <c r="B114" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C114" s="19"/>
+      <c r="C114" s="20"/>
       <c r="D114" s="2" t="s">
         <v>279</v>
       </c>
@@ -4327,11 +4334,11 @@
       <c r="I114" s="4"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A115" s="17"/>
-      <c r="B115" s="22" t="s">
+      <c r="A115" s="18"/>
+      <c r="B115" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C115" s="19">
+      <c r="C115" s="20">
         <v>57</v>
       </c>
       <c r="D115" s="2" t="s">
@@ -4350,11 +4357,11 @@
       <c r="I115" s="4"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A116" s="17"/>
-      <c r="B116" s="22" t="s">
+      <c r="A116" s="18"/>
+      <c r="B116" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C116" s="19"/>
+      <c r="C116" s="20"/>
       <c r="D116" s="2" t="s">
         <v>283</v>
       </c>
@@ -4371,13 +4378,13 @@
       <c r="I116" s="4"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A117" s="17" t="s">
+      <c r="A117" s="18" t="s">
         <v>285</v>
       </c>
-      <c r="B117" s="22" t="s">
+      <c r="B117" s="19" t="s">
         <v>286</v>
       </c>
-      <c r="C117" s="19">
+      <c r="C117" s="20">
         <v>58</v>
       </c>
       <c r="D117" s="2" t="s">
@@ -4396,11 +4403,11 @@
       <c r="I117" s="4"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A118" s="17"/>
-      <c r="B118" s="22" t="s">
+      <c r="A118" s="18"/>
+      <c r="B118" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C118" s="19"/>
+      <c r="C118" s="20"/>
       <c r="D118" s="2" t="s">
         <v>289</v>
       </c>
@@ -4417,11 +4424,11 @@
       <c r="I118" s="4"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A119" s="17"/>
-      <c r="B119" s="22" t="s">
+      <c r="A119" s="18"/>
+      <c r="B119" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C119" s="19">
+      <c r="C119" s="20">
         <v>59</v>
       </c>
       <c r="D119" s="2" t="s">
@@ -4440,11 +4447,11 @@
       <c r="I119" s="4"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A120" s="17"/>
-      <c r="B120" s="22" t="s">
+      <c r="A120" s="18"/>
+      <c r="B120" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="C120" s="19"/>
+      <c r="C120" s="20"/>
       <c r="D120" s="2" t="s">
         <v>291</v>
       </c>
@@ -4461,13 +4468,13 @@
       <c r="I120" s="4"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" s="17" t="s">
+      <c r="A121" s="18" t="s">
         <v>293</v>
       </c>
-      <c r="B121" s="22" t="s">
+      <c r="B121" s="19" t="s">
         <v>294</v>
       </c>
-      <c r="C121" s="19">
+      <c r="C121" s="20">
         <v>60</v>
       </c>
       <c r="D121" s="2" t="s">
@@ -4486,9 +4493,9 @@
       <c r="I121" s="4"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A122" s="17"/>
-      <c r="B122" s="22"/>
-      <c r="C122" s="19"/>
+      <c r="A122" s="18"/>
+      <c r="B122" s="19"/>
+      <c r="C122" s="20"/>
       <c r="D122" s="2" t="s">
         <v>297</v>
       </c>
@@ -4505,9 +4512,9 @@
       <c r="I122" s="4"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A123" s="17"/>
-      <c r="B123" s="22"/>
-      <c r="C123" s="19">
+      <c r="A123" s="18"/>
+      <c r="B123" s="19"/>
+      <c r="C123" s="20">
         <v>61</v>
       </c>
       <c r="D123" s="2" t="s">
@@ -4526,9 +4533,9 @@
       <c r="I123" s="4"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A124" s="17"/>
-      <c r="B124" s="22"/>
-      <c r="C124" s="19"/>
+      <c r="A124" s="18"/>
+      <c r="B124" s="19"/>
+      <c r="C124" s="20"/>
       <c r="D124" s="2" t="s">
         <v>309</v>
       </c>
@@ -4545,9 +4552,9 @@
       <c r="I124" s="4"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A125" s="17"/>
-      <c r="B125" s="22"/>
-      <c r="C125" s="19">
+      <c r="A125" s="18"/>
+      <c r="B125" s="19"/>
+      <c r="C125" s="20">
         <v>62</v>
       </c>
       <c r="D125" s="2" t="s">
@@ -4566,9 +4573,9 @@
       <c r="I125" s="4"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A126" s="17"/>
-      <c r="B126" s="22"/>
-      <c r="C126" s="19"/>
+      <c r="A126" s="18"/>
+      <c r="B126" s="19"/>
+      <c r="C126" s="20"/>
       <c r="D126" s="2" t="s">
         <v>313</v>
       </c>
@@ -4586,6 +4593,123 @@
     </row>
   </sheetData>
   <mergeCells count="141">
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A41:A44"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A75:A78"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="A71:A74"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="C83:C84"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="B41:B44"/>
+    <mergeCell ref="A83:A86"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="A91:A94"/>
+    <mergeCell ref="A95:A98"/>
+    <mergeCell ref="A99:A102"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="B71:B74"/>
+    <mergeCell ref="B75:B78"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A117:A120"/>
+    <mergeCell ref="B87:B90"/>
+    <mergeCell ref="B91:B94"/>
+    <mergeCell ref="B95:B98"/>
+    <mergeCell ref="B99:B102"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="B109:B110"/>
+    <mergeCell ref="B111:B112"/>
+    <mergeCell ref="B113:B116"/>
+    <mergeCell ref="B117:B120"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="A105:A108"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A113:A116"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="C101:C102"/>
+    <mergeCell ref="C103:C104"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="C93:C94"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:G2"/>
@@ -4610,123 +4734,6 @@
     <mergeCell ref="C111:C112"/>
     <mergeCell ref="C113:C114"/>
     <mergeCell ref="C95:C96"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="C103:C104"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="A117:A120"/>
-    <mergeCell ref="B87:B90"/>
-    <mergeCell ref="B91:B94"/>
-    <mergeCell ref="B95:B98"/>
-    <mergeCell ref="B99:B102"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="B109:B110"/>
-    <mergeCell ref="B111:B112"/>
-    <mergeCell ref="B113:B116"/>
-    <mergeCell ref="B117:B120"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="A105:A108"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A113:A116"/>
-    <mergeCell ref="A83:A86"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="A91:A94"/>
-    <mergeCell ref="A95:A98"/>
-    <mergeCell ref="A99:A102"/>
-    <mergeCell ref="B47:B50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B71:B74"/>
-    <mergeCell ref="B75:B78"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="B31:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="C83:C84"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A18"/>
-    <mergeCell ref="A19:A22"/>
-    <mergeCell ref="A75:A78"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="A71:A74"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="A41:A44"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A51:A52"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G126" xr:uid="{BD7D4049-E182-46D9-ABFE-ED680993C7C2}">
@@ -4794,9 +4801,11 @@
     <hyperlink ref="F60" r:id="rId58" xr:uid="{9CECBBD6-2F14-4F88-B6F4-C08AF3014E4F}"/>
     <hyperlink ref="F61" r:id="rId59" xr:uid="{F9AF7E56-A77D-4520-87E8-16AD5AF5E883}"/>
     <hyperlink ref="F62" r:id="rId60" xr:uid="{CD8C3D13-0D28-42DD-AC01-181A7BF0563D}"/>
+    <hyperlink ref="F63" r:id="rId61" xr:uid="{A70F3F27-3F11-4F9A-BC23-AE33E52090AB}"/>
+    <hyperlink ref="F64" r:id="rId62" xr:uid="{5CDF4550-20CC-477E-9481-AC77674048F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId61"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId63"/>
 </worksheet>
 </file>
 

</xml_diff>